<commit_message>
0.71 - vercel test
</commit_message>
<xml_diff>
--- a/Docs/ΕΥΚΑΡΔΙΑ Πεδία Βάσης Δεδομένων.xlsx
+++ b/Docs/ΕΥΚΑΡΔΙΑ Πεδία Βάσης Δεδομένων.xlsx
@@ -8,17 +8,19 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Development\Eukardia\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{868DC5DF-E5D7-47D9-8A18-C5F86A629959}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2547805-38B5-4B4C-B499-02B7F2005D54}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11625" tabRatio="481" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11625" tabRatio="481" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Πεδία" sheetId="1" r:id="rId1"/>
+    <sheet name="dim" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm.Print_Area" localSheetId="0">Πίνακας1[[#All],[Περιγραφή πεδίου]:[Επιτρεπόμενες τιμές ή εύρος τιμών]]</definedName>
+    <definedName name="types">dim!$K$1:$L$9</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -28,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="353" uniqueCount="158">
   <si>
     <t>Όνομα πεδίου</t>
   </si>
@@ -348,9 +350,6 @@
     <t>Έτος διάγνωσης καρκίνου</t>
   </si>
   <si>
-    <t>deathCVD</t>
-  </si>
-  <si>
     <t>Δείκτης Μάζας Σώματος (BMI)</t>
   </si>
   <si>
@@ -387,9 +386,6 @@
     <t>Έτος θανάτου</t>
   </si>
   <si>
-    <t>yrCVDdeath</t>
-  </si>
-  <si>
     <t>Ναι/Όχι</t>
   </si>
   <si>
@@ -397,13 +393,124 @@
   </si>
   <si>
     <t>yrcancer</t>
+  </si>
+  <si>
+    <t>deathcvd</t>
+  </si>
+  <si>
+    <t>yrcvddeath</t>
+  </si>
+  <si>
+    <t>int(11)</t>
+  </si>
+  <si>
+    <t>NO</t>
+  </si>
+  <si>
+    <t>PRI</t>
+  </si>
+  <si>
+    <t>auto_increment</t>
+  </si>
+  <si>
+    <t>tinyint(1)</t>
+  </si>
+  <si>
+    <t>patientId</t>
+  </si>
+  <si>
+    <t>varchar(255)</t>
+  </si>
+  <si>
+    <t>MUL</t>
+  </si>
+  <si>
+    <t>tinyint(4)</t>
+  </si>
+  <si>
+    <t>YES</t>
+  </si>
+  <si>
+    <t>drugbp</t>
+  </si>
+  <si>
+    <t>sbp</t>
+  </si>
+  <si>
+    <t>float</t>
+  </si>
+  <si>
+    <t>dbp</t>
+  </si>
+  <si>
+    <t>diebetes</t>
+  </si>
+  <si>
+    <t>druglipids</t>
+  </si>
+  <si>
+    <t>artialfibrillation</t>
+  </si>
+  <si>
+    <t>cvd</t>
+  </si>
+  <si>
+    <t>yrcvd</t>
+  </si>
+  <si>
+    <t>smallint(6)</t>
+  </si>
+  <si>
+    <t>comments</t>
+  </si>
+  <si>
+    <t>mediumtext</t>
+  </si>
+  <si>
+    <t>datetime</t>
+  </si>
+  <si>
+    <t>Πεδίο</t>
+  </si>
+  <si>
+    <t>Τύπος (κατανοητός)</t>
+  </si>
+  <si>
+    <t>Τύπος SQL</t>
+  </si>
+  <si>
+    <t>Key</t>
+  </si>
+  <si>
+    <t>Default value</t>
+  </si>
+  <si>
+    <t>Extra</t>
+  </si>
+  <si>
+    <t>Μεγάλο κείμενο</t>
+  </si>
+  <si>
+    <t>Ημερομηνία και Ώρα</t>
+  </si>
+  <si>
+    <t>Δεκαδικός αριθμός</t>
+  </si>
+  <si>
+    <t>Ακέραιος μέχρι 65535</t>
+  </si>
+  <si>
+    <t>Ακέραιος μέχρι 2147483647</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ακέραιος ή λίστα μέχρι 127 </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -452,8 +559,16 @@
       <family val="2"/>
       <scheme val="major"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -466,8 +581,14 @@
         <bgColor theme="8"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor theme="9"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="3">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -493,11 +614,20 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="9"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -515,11 +645,43 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Κανονικό" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="19">
+  <dxfs count="27">
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <font>
         <strike val="0"/>
@@ -797,34 +959,52 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Πίνακας1" displayName="Πίνακας1" ref="A1:G37" totalsRowShown="0" headerRowDxfId="18" dataDxfId="17">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Πίνακας1" displayName="Πίνακας1" ref="A1:G37" totalsRowShown="0" headerRowDxfId="26" dataDxfId="25">
   <autoFilter ref="A1:G37" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Περιγραφή πεδίου" dataDxfId="16"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Υποχρεωτική συμπλήρωση" dataDxfId="15"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="Όνομα πεδίου βάσης" dataDxfId="14"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Τύπος" dataDxfId="13"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Μονάδες μέτρησης" dataDxfId="12"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Επιτρεπόμενες τιμές ή εύρος τιμών" dataDxfId="11"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Περιγραφή" dataDxfId="10"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Περιγραφή πεδίου" dataDxfId="24"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Υποχρεωτική συμπλήρωση" dataDxfId="23"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="Όνομα πεδίου βάσης" dataDxfId="22"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Τύπος" dataDxfId="21"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Μονάδες μέτρησης" dataDxfId="20"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Επιτρεπόμενες τιμές ή εύρος τιμών" dataDxfId="19"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Περιγραφή" dataDxfId="18"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight13" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Πίνακας2" displayName="Πίνακας2" ref="A42:G46" totalsRowShown="0" headerRowDxfId="9" dataDxfId="8" tableBorderDxfId="7">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Πίνακας2" displayName="Πίνακας2" ref="A42:G46" totalsRowShown="0" headerRowDxfId="17" dataDxfId="16" tableBorderDxfId="15">
   <autoFilter ref="A42:G46" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="Όνομα πεδίου" dataDxfId="6"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0100-000004000000}" name="Υποχρεωτικό" dataDxfId="5"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0100-000007000000}" name="Πεδίο βάσης" dataDxfId="4"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="Τύπος" dataDxfId="3"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="Μονάδες μέτρησης" dataDxfId="2"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0100-000005000000}" name="Επιτρεπόμενες τιμές" dataDxfId="1"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0100-000006000000}" name="Περιγραφή" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="Όνομα πεδίου" dataDxfId="14"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0100-000004000000}" name="Υποχρεωτικό" dataDxfId="13"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0100-000007000000}" name="Πεδίο βάσης" dataDxfId="12"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="Τύπος" dataDxfId="11"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="Μονάδες μέτρησης" dataDxfId="10"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0100-000005000000}" name="Επιτρεπόμενες τιμές" dataDxfId="9"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0100-000006000000}" name="Περιγραφή" dataDxfId="8"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight12" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{124B803E-62B7-4DF6-97EB-31E33393CFE8}" name="Πίνακας3" displayName="Πίνακας3" ref="A1:G42" totalsRowShown="0" dataDxfId="1">
+  <autoFilter ref="A1:G42" xr:uid="{89C5C1E3-CE08-4CF4-BF51-207D1F88BF61}"/>
+  <tableColumns count="7">
+    <tableColumn id="1" xr3:uid="{310BA3A6-8BAB-4AFE-9044-3DBC1F268DB3}" name="Πεδίο" dataDxfId="7"/>
+    <tableColumn id="2" xr3:uid="{3986543B-C60B-42C6-BDEF-7981CFB32FA8}" name="Τύπος (κατανοητός)" dataDxfId="0">
+      <calculatedColumnFormula>VLOOKUP(Πίνακας3[[#This Row],[Τύπος SQL]],types,2,FALSE)</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="3" xr3:uid="{BD85B841-8B4D-4BCC-B5C9-A161325437D0}" name="Τύπος SQL" dataDxfId="6"/>
+    <tableColumn id="4" xr3:uid="{72048646-56D9-4F1A-9344-EFC38B058077}" name="Υποχρεωτικό" dataDxfId="5"/>
+    <tableColumn id="5" xr3:uid="{EF472430-A112-45C0-A202-A1F958E3AB86}" name="Key" dataDxfId="4"/>
+    <tableColumn id="6" xr3:uid="{7A28CF5F-9508-41CD-A516-6F0B3FB0681E}" name="Default value" dataDxfId="3"/>
+    <tableColumn id="7" xr3:uid="{A4C62788-3491-4A41-9F8A-B8B83DEFB0B7}" name="Extra" dataDxfId="2"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight14" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
@@ -1096,8 +1276,8 @@
   </sheetPr>
   <dimension ref="A1:G46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C37" sqref="C37"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1143,7 +1323,7 @@
         <v>52</v>
       </c>
       <c r="D2" s="10" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="E2" s="10"/>
       <c r="F2" s="10"/>
@@ -1207,7 +1387,7 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C6" s="3" t="s">
         <v>92</v>
@@ -1286,7 +1466,7 @@
         <v>83</v>
       </c>
       <c r="D11" s="10" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="E11" s="3" t="s">
         <v>30</v>
@@ -1312,7 +1492,7 @@
         <v>104</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="13" spans="1:7" ht="45" x14ac:dyDescent="0.25">
@@ -1329,27 +1509,27 @@
         <v>30</v>
       </c>
       <c r="F13" s="5" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="14" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="C14" s="3" t="s">
         <v>109</v>
-      </c>
-      <c r="C14" s="3" t="s">
-        <v>110</v>
       </c>
       <c r="D14" s="3" t="s">
         <v>6</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
@@ -1378,7 +1558,7 @@
         <v>90</v>
       </c>
       <c r="D16" s="10" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="E16" s="4"/>
       <c r="F16" s="3" t="s">
@@ -1447,7 +1627,7 @@
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B21" s="4"/>
       <c r="C21" s="3" t="s">
@@ -1568,14 +1748,14 @@
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B29" s="4"/>
       <c r="C29" s="3" t="s">
         <v>85</v>
       </c>
-      <c r="D29" s="3" t="s">
-        <v>6</v>
+      <c r="D29" s="10" t="s">
+        <v>118</v>
       </c>
       <c r="E29" s="4" t="s">
         <v>30</v>
@@ -1586,14 +1766,14 @@
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" s="3" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B30" s="4"/>
       <c r="C30" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="D30" s="3" t="s">
-        <v>6</v>
+      <c r="D30" s="10" t="s">
+        <v>118</v>
       </c>
       <c r="E30" s="4" t="s">
         <v>30</v>
@@ -1604,14 +1784,14 @@
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" s="3" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B31" s="4"/>
       <c r="C31" s="3" t="s">
         <v>95</v>
       </c>
-      <c r="D31" s="3" t="s">
-        <v>6</v>
+      <c r="D31" s="10" t="s">
+        <v>118</v>
       </c>
       <c r="E31" s="4" t="s">
         <v>30</v>
@@ -1637,14 +1817,14 @@
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" s="3" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B33" s="4"/>
       <c r="C33" s="3" t="s">
-        <v>106</v>
-      </c>
-      <c r="D33" s="3" t="s">
-        <v>6</v>
+        <v>121</v>
+      </c>
+      <c r="D33" s="10" t="s">
+        <v>118</v>
       </c>
       <c r="F33" s="3" t="s">
         <v>91</v>
@@ -1652,11 +1832,11 @@
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" s="3" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B34" s="4"/>
       <c r="C34" s="3" t="s">
-        <v>119</v>
+        <v>122</v>
       </c>
       <c r="D34" s="3" t="s">
         <v>27</v>
@@ -1667,14 +1847,14 @@
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" s="3" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B35" s="4"/>
       <c r="C35" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="D35" s="3" t="s">
-        <v>6</v>
+      <c r="D35" s="10" t="s">
+        <v>118</v>
       </c>
       <c r="E35" s="4" t="s">
         <v>30</v>
@@ -1691,8 +1871,8 @@
       <c r="C36" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="D36" s="3" t="s">
-        <v>6</v>
+      <c r="D36" s="10" t="s">
+        <v>118</v>
       </c>
       <c r="E36" s="4" t="s">
         <v>30</v>
@@ -1706,7 +1886,7 @@
         <v>105</v>
       </c>
       <c r="C37" s="3" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="D37" s="3" t="s">
         <v>27</v>
@@ -1841,4 +2021,855 @@
     <tablePart r:id="rId3"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{13E70851-83B8-43A0-B14E-A8B2D42B9ED9}">
+  <dimension ref="A1:L42"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="25.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="28.140625" customWidth="1"/>
+    <col min="3" max="3" width="15.28515625" customWidth="1"/>
+    <col min="4" max="4" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="9.28515625" customWidth="1"/>
+    <col min="7" max="7" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="33.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>146</v>
+      </c>
+      <c r="B1" t="s">
+        <v>147</v>
+      </c>
+      <c r="C1" t="s">
+        <v>148</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>149</v>
+      </c>
+      <c r="F1" t="s">
+        <v>150</v>
+      </c>
+      <c r="G1" t="s">
+        <v>151</v>
+      </c>
+      <c r="K1" s="12" t="s">
+        <v>148</v>
+      </c>
+      <c r="L1" s="12" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2" s="11" t="s">
+        <v>72</v>
+      </c>
+      <c r="B2" s="11" t="str">
+        <f>VLOOKUP(Πίνακας3[[#This Row],[Τύπος SQL]],types,2,FALSE)</f>
+        <v>Ακέραιος μέχρι 2147483647</v>
+      </c>
+      <c r="C2" s="11" t="s">
+        <v>123</v>
+      </c>
+      <c r="D2" s="11" t="s">
+        <v>124</v>
+      </c>
+      <c r="E2" s="11" t="s">
+        <v>125</v>
+      </c>
+      <c r="F2" s="11"/>
+      <c r="G2" s="11" t="s">
+        <v>126</v>
+      </c>
+      <c r="K2" s="13" t="s">
+        <v>123</v>
+      </c>
+      <c r="L2" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A3" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="B3" s="11" t="str">
+        <f>VLOOKUP(Πίνακας3[[#This Row],[Τύπος SQL]],types,2,FALSE)</f>
+        <v>Ναι/Όχι</v>
+      </c>
+      <c r="C3" s="11" t="s">
+        <v>127</v>
+      </c>
+      <c r="D3" s="11" t="s">
+        <v>124</v>
+      </c>
+      <c r="E3" s="11"/>
+      <c r="F3" s="11">
+        <v>0</v>
+      </c>
+      <c r="G3" s="11"/>
+      <c r="K3" s="13" t="s">
+        <v>127</v>
+      </c>
+      <c r="L3" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A4" s="11" t="s">
+        <v>128</v>
+      </c>
+      <c r="B4" s="11" t="str">
+        <f>VLOOKUP(Πίνακας3[[#This Row],[Τύπος SQL]],types,2,FALSE)</f>
+        <v>Σύντομο κείμενο</v>
+      </c>
+      <c r="C4" s="11" t="s">
+        <v>129</v>
+      </c>
+      <c r="D4" s="11" t="s">
+        <v>124</v>
+      </c>
+      <c r="E4" s="11" t="s">
+        <v>130</v>
+      </c>
+      <c r="F4" s="11"/>
+      <c r="G4" s="11"/>
+      <c r="K4" s="13" t="s">
+        <v>129</v>
+      </c>
+      <c r="L4" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A5" s="11" t="s">
+        <v>54</v>
+      </c>
+      <c r="B5" s="11" t="str">
+        <f>VLOOKUP(Πίνακας3[[#This Row],[Τύπος SQL]],types,2,FALSE)</f>
+        <v xml:space="preserve">Ακέραιος ή λίστα μέχρι 127 </v>
+      </c>
+      <c r="C5" s="11" t="s">
+        <v>131</v>
+      </c>
+      <c r="D5" s="11" t="s">
+        <v>132</v>
+      </c>
+      <c r="E5" s="11"/>
+      <c r="F5" s="11"/>
+      <c r="G5" s="11"/>
+      <c r="K5" s="13" t="s">
+        <v>131</v>
+      </c>
+      <c r="L5" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A6" s="11" t="s">
+        <v>55</v>
+      </c>
+      <c r="B6" s="11" t="str">
+        <f>VLOOKUP(Πίνακας3[[#This Row],[Τύπος SQL]],types,2,FALSE)</f>
+        <v xml:space="preserve">Ακέραιος ή λίστα μέχρι 127 </v>
+      </c>
+      <c r="C6" s="11" t="s">
+        <v>131</v>
+      </c>
+      <c r="D6" s="11" t="s">
+        <v>132</v>
+      </c>
+      <c r="E6" s="11"/>
+      <c r="F6" s="11"/>
+      <c r="G6" s="11"/>
+      <c r="K6" s="13" t="s">
+        <v>135</v>
+      </c>
+      <c r="L6" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A7" s="11" t="s">
+        <v>133</v>
+      </c>
+      <c r="B7" s="11" t="str">
+        <f>VLOOKUP(Πίνακας3[[#This Row],[Τύπος SQL]],types,2,FALSE)</f>
+        <v>Ναι/Όχι</v>
+      </c>
+      <c r="C7" s="11" t="s">
+        <v>127</v>
+      </c>
+      <c r="D7" s="11" t="s">
+        <v>132</v>
+      </c>
+      <c r="E7" s="11"/>
+      <c r="F7" s="11"/>
+      <c r="G7" s="11"/>
+      <c r="K7" s="13" t="s">
+        <v>142</v>
+      </c>
+      <c r="L7" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A8" s="11" t="s">
+        <v>134</v>
+      </c>
+      <c r="B8" s="11" t="str">
+        <f>VLOOKUP(Πίνακας3[[#This Row],[Τύπος SQL]],types,2,FALSE)</f>
+        <v>Δεκαδικός αριθμός</v>
+      </c>
+      <c r="C8" s="11" t="s">
+        <v>135</v>
+      </c>
+      <c r="D8" s="11" t="s">
+        <v>132</v>
+      </c>
+      <c r="E8" s="11"/>
+      <c r="F8" s="11"/>
+      <c r="G8" s="11"/>
+      <c r="K8" s="13" t="s">
+        <v>144</v>
+      </c>
+      <c r="L8" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A9" s="11" t="s">
+        <v>136</v>
+      </c>
+      <c r="B9" s="11" t="str">
+        <f>VLOOKUP(Πίνακας3[[#This Row],[Τύπος SQL]],types,2,FALSE)</f>
+        <v>Δεκαδικός αριθμός</v>
+      </c>
+      <c r="C9" s="11" t="s">
+        <v>135</v>
+      </c>
+      <c r="D9" s="11" t="s">
+        <v>132</v>
+      </c>
+      <c r="E9" s="11"/>
+      <c r="F9" s="11"/>
+      <c r="G9" s="11"/>
+      <c r="K9" s="13" t="s">
+        <v>145</v>
+      </c>
+      <c r="L9" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A10" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="B10" s="11" t="str">
+        <f>VLOOKUP(Πίνακας3[[#This Row],[Τύπος SQL]],types,2,FALSE)</f>
+        <v>Δεκαδικός αριθμός</v>
+      </c>
+      <c r="C10" s="11" t="s">
+        <v>135</v>
+      </c>
+      <c r="D10" s="11" t="s">
+        <v>132</v>
+      </c>
+      <c r="E10" s="11"/>
+      <c r="F10" s="11"/>
+      <c r="G10" s="11"/>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A11" s="11" t="s">
+        <v>68</v>
+      </c>
+      <c r="B11" s="11" t="str">
+        <f>VLOOKUP(Πίνακας3[[#This Row],[Τύπος SQL]],types,2,FALSE)</f>
+        <v>Δεκαδικός αριθμός</v>
+      </c>
+      <c r="C11" s="11" t="s">
+        <v>135</v>
+      </c>
+      <c r="D11" s="11" t="s">
+        <v>132</v>
+      </c>
+      <c r="E11" s="11"/>
+      <c r="F11" s="11"/>
+      <c r="G11" s="11"/>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A12" s="11" t="s">
+        <v>137</v>
+      </c>
+      <c r="B12" s="11" t="str">
+        <f>VLOOKUP(Πίνακας3[[#This Row],[Τύπος SQL]],types,2,FALSE)</f>
+        <v>Ναι/Όχι</v>
+      </c>
+      <c r="C12" s="11" t="s">
+        <v>127</v>
+      </c>
+      <c r="D12" s="11" t="s">
+        <v>132</v>
+      </c>
+      <c r="E12" s="11"/>
+      <c r="F12" s="11"/>
+      <c r="G12" s="11"/>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A13" s="11" t="s">
+        <v>58</v>
+      </c>
+      <c r="B13" s="11" t="str">
+        <f>VLOOKUP(Πίνακας3[[#This Row],[Τύπος SQL]],types,2,FALSE)</f>
+        <v xml:space="preserve">Ακέραιος ή λίστα μέχρι 127 </v>
+      </c>
+      <c r="C13" s="11" t="s">
+        <v>131</v>
+      </c>
+      <c r="D13" s="11" t="s">
+        <v>132</v>
+      </c>
+      <c r="E13" s="11"/>
+      <c r="F13" s="11"/>
+      <c r="G13" s="11"/>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A14" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="B14" s="11" t="str">
+        <f>VLOOKUP(Πίνακας3[[#This Row],[Τύπος SQL]],types,2,FALSE)</f>
+        <v xml:space="preserve">Ακέραιος ή λίστα μέχρι 127 </v>
+      </c>
+      <c r="C14" s="11" t="s">
+        <v>131</v>
+      </c>
+      <c r="D14" s="11" t="s">
+        <v>132</v>
+      </c>
+      <c r="E14" s="11"/>
+      <c r="F14" s="11"/>
+      <c r="G14" s="11"/>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A15" s="11" t="s">
+        <v>109</v>
+      </c>
+      <c r="B15" s="11" t="str">
+        <f>VLOOKUP(Πίνακας3[[#This Row],[Τύπος SQL]],types,2,FALSE)</f>
+        <v xml:space="preserve">Ακέραιος ή λίστα μέχρι 127 </v>
+      </c>
+      <c r="C15" s="11" t="s">
+        <v>131</v>
+      </c>
+      <c r="D15" s="11" t="s">
+        <v>132</v>
+      </c>
+      <c r="E15" s="11"/>
+      <c r="F15" s="11"/>
+      <c r="G15" s="11"/>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A16" s="11" t="s">
+        <v>60</v>
+      </c>
+      <c r="B16" s="11" t="str">
+        <f>VLOOKUP(Πίνακας3[[#This Row],[Τύπος SQL]],types,2,FALSE)</f>
+        <v xml:space="preserve">Ακέραιος ή λίστα μέχρι 127 </v>
+      </c>
+      <c r="C16" s="11" t="s">
+        <v>131</v>
+      </c>
+      <c r="D16" s="11" t="s">
+        <v>132</v>
+      </c>
+      <c r="E16" s="11"/>
+      <c r="F16" s="11"/>
+      <c r="G16" s="11"/>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" s="11" t="s">
+        <v>138</v>
+      </c>
+      <c r="B17" s="11" t="str">
+        <f>VLOOKUP(Πίνακας3[[#This Row],[Τύπος SQL]],types,2,FALSE)</f>
+        <v>Ναι/Όχι</v>
+      </c>
+      <c r="C17" s="11" t="s">
+        <v>127</v>
+      </c>
+      <c r="D17" s="11" t="s">
+        <v>132</v>
+      </c>
+      <c r="E17" s="11"/>
+      <c r="F17" s="11"/>
+      <c r="G17" s="11"/>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" s="11" t="s">
+        <v>84</v>
+      </c>
+      <c r="B18" s="11" t="str">
+        <f>VLOOKUP(Πίνακας3[[#This Row],[Τύπος SQL]],types,2,FALSE)</f>
+        <v>Δεκαδικός αριθμός</v>
+      </c>
+      <c r="C18" s="11" t="s">
+        <v>135</v>
+      </c>
+      <c r="D18" s="11" t="s">
+        <v>132</v>
+      </c>
+      <c r="E18" s="11"/>
+      <c r="F18" s="11"/>
+      <c r="G18" s="11"/>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19" s="11" t="s">
+        <v>61</v>
+      </c>
+      <c r="B19" s="11" t="str">
+        <f>VLOOKUP(Πίνακας3[[#This Row],[Τύπος SQL]],types,2,FALSE)</f>
+        <v>Δεκαδικός αριθμός</v>
+      </c>
+      <c r="C19" s="11" t="s">
+        <v>135</v>
+      </c>
+      <c r="D19" s="11" t="s">
+        <v>132</v>
+      </c>
+      <c r="E19" s="11"/>
+      <c r="F19" s="11"/>
+      <c r="G19" s="11"/>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20" s="11" t="s">
+        <v>66</v>
+      </c>
+      <c r="B20" s="11" t="str">
+        <f>VLOOKUP(Πίνακας3[[#This Row],[Τύπος SQL]],types,2,FALSE)</f>
+        <v>Δεκαδικός αριθμός</v>
+      </c>
+      <c r="C20" s="11" t="s">
+        <v>135</v>
+      </c>
+      <c r="D20" s="11" t="s">
+        <v>132</v>
+      </c>
+      <c r="E20" s="11"/>
+      <c r="F20" s="11"/>
+      <c r="G20" s="11"/>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21" s="11" t="s">
+        <v>67</v>
+      </c>
+      <c r="B21" s="11" t="str">
+        <f>VLOOKUP(Πίνακας3[[#This Row],[Τύπος SQL]],types,2,FALSE)</f>
+        <v>Δεκαδικός αριθμός</v>
+      </c>
+      <c r="C21" s="11" t="s">
+        <v>135</v>
+      </c>
+      <c r="D21" s="11" t="s">
+        <v>132</v>
+      </c>
+      <c r="E21" s="11"/>
+      <c r="F21" s="11"/>
+      <c r="G21" s="11"/>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A22" s="11" t="s">
+        <v>62</v>
+      </c>
+      <c r="B22" s="11" t="str">
+        <f>VLOOKUP(Πίνακας3[[#This Row],[Τύπος SQL]],types,2,FALSE)</f>
+        <v>Δεκαδικός αριθμός</v>
+      </c>
+      <c r="C22" s="11" t="s">
+        <v>135</v>
+      </c>
+      <c r="D22" s="11" t="s">
+        <v>132</v>
+      </c>
+      <c r="E22" s="11"/>
+      <c r="F22" s="11"/>
+      <c r="G22" s="11"/>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A23" s="11" t="s">
+        <v>63</v>
+      </c>
+      <c r="B23" s="11" t="str">
+        <f>VLOOKUP(Πίνακας3[[#This Row],[Τύπος SQL]],types,2,FALSE)</f>
+        <v>Δεκαδικός αριθμός</v>
+      </c>
+      <c r="C23" s="11" t="s">
+        <v>135</v>
+      </c>
+      <c r="D23" s="11" t="s">
+        <v>132</v>
+      </c>
+      <c r="E23" s="11"/>
+      <c r="F23" s="11"/>
+      <c r="G23" s="11"/>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24" s="11" t="s">
+        <v>77</v>
+      </c>
+      <c r="B24" s="11" t="str">
+        <f>VLOOKUP(Πίνακας3[[#This Row],[Τύπος SQL]],types,2,FALSE)</f>
+        <v>Δεκαδικός αριθμός</v>
+      </c>
+      <c r="C24" s="11" t="s">
+        <v>135</v>
+      </c>
+      <c r="D24" s="11" t="s">
+        <v>132</v>
+      </c>
+      <c r="E24" s="11"/>
+      <c r="F24" s="11"/>
+      <c r="G24" s="11"/>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A25" s="11" t="s">
+        <v>94</v>
+      </c>
+      <c r="B25" s="11" t="str">
+        <f>VLOOKUP(Πίνακας3[[#This Row],[Τύπος SQL]],types,2,FALSE)</f>
+        <v>Δεκαδικός αριθμός</v>
+      </c>
+      <c r="C25" s="11" t="s">
+        <v>135</v>
+      </c>
+      <c r="D25" s="11" t="s">
+        <v>132</v>
+      </c>
+      <c r="E25" s="11"/>
+      <c r="F25" s="11"/>
+      <c r="G25" s="11"/>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A26" s="11" t="s">
+        <v>64</v>
+      </c>
+      <c r="B26" s="11" t="str">
+        <f>VLOOKUP(Πίνακας3[[#This Row],[Τύπος SQL]],types,2,FALSE)</f>
+        <v>Δεκαδικός αριθμός</v>
+      </c>
+      <c r="C26" s="11" t="s">
+        <v>135</v>
+      </c>
+      <c r="D26" s="11" t="s">
+        <v>132</v>
+      </c>
+      <c r="E26" s="11"/>
+      <c r="F26" s="11"/>
+      <c r="G26" s="11"/>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A27" s="11" t="s">
+        <v>82</v>
+      </c>
+      <c r="B27" s="11" t="str">
+        <f>VLOOKUP(Πίνακας3[[#This Row],[Τύπος SQL]],types,2,FALSE)</f>
+        <v>Δεκαδικός αριθμός</v>
+      </c>
+      <c r="C27" s="11" t="s">
+        <v>135</v>
+      </c>
+      <c r="D27" s="11" t="s">
+        <v>132</v>
+      </c>
+      <c r="E27" s="11"/>
+      <c r="F27" s="11"/>
+      <c r="G27" s="11"/>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A28" s="11" t="s">
+        <v>65</v>
+      </c>
+      <c r="B28" s="11" t="str">
+        <f>VLOOKUP(Πίνακας3[[#This Row],[Τύπος SQL]],types,2,FALSE)</f>
+        <v>Δεκαδικός αριθμός</v>
+      </c>
+      <c r="C28" s="11" t="s">
+        <v>135</v>
+      </c>
+      <c r="D28" s="11" t="s">
+        <v>132</v>
+      </c>
+      <c r="E28" s="11"/>
+      <c r="F28" s="11"/>
+      <c r="G28" s="11"/>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A29" s="11" t="s">
+        <v>71</v>
+      </c>
+      <c r="B29" s="11" t="str">
+        <f>VLOOKUP(Πίνακας3[[#This Row],[Τύπος SQL]],types,2,FALSE)</f>
+        <v>Δεκαδικός αριθμός</v>
+      </c>
+      <c r="C29" s="11" t="s">
+        <v>135</v>
+      </c>
+      <c r="D29" s="11" t="s">
+        <v>132</v>
+      </c>
+      <c r="E29" s="11"/>
+      <c r="F29" s="11"/>
+      <c r="G29" s="11"/>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A30" s="11" t="s">
+        <v>139</v>
+      </c>
+      <c r="B30" s="11" t="str">
+        <f>VLOOKUP(Πίνακας3[[#This Row],[Τύπος SQL]],types,2,FALSE)</f>
+        <v>Ναι/Όχι</v>
+      </c>
+      <c r="C30" s="11" t="s">
+        <v>127</v>
+      </c>
+      <c r="D30" s="11" t="s">
+        <v>132</v>
+      </c>
+      <c r="E30" s="11"/>
+      <c r="F30" s="11"/>
+      <c r="G30" s="11"/>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A31" s="11" t="s">
+        <v>69</v>
+      </c>
+      <c r="B31" s="11" t="str">
+        <f>VLOOKUP(Πίνακας3[[#This Row],[Τύπος SQL]],types,2,FALSE)</f>
+        <v>Ναι/Όχι</v>
+      </c>
+      <c r="C31" s="11" t="s">
+        <v>127</v>
+      </c>
+      <c r="D31" s="11" t="s">
+        <v>132</v>
+      </c>
+      <c r="E31" s="11"/>
+      <c r="F31" s="11"/>
+      <c r="G31" s="11"/>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A32" s="11" t="s">
+        <v>140</v>
+      </c>
+      <c r="B32" s="11" t="str">
+        <f>VLOOKUP(Πίνακας3[[#This Row],[Τύπος SQL]],types,2,FALSE)</f>
+        <v>Ναι/Όχι</v>
+      </c>
+      <c r="C32" s="11" t="s">
+        <v>127</v>
+      </c>
+      <c r="D32" s="11" t="s">
+        <v>132</v>
+      </c>
+      <c r="E32" s="11"/>
+      <c r="F32" s="11"/>
+      <c r="G32" s="11"/>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A33" s="11" t="s">
+        <v>141</v>
+      </c>
+      <c r="B33" s="11" t="str">
+        <f>VLOOKUP(Πίνακας3[[#This Row],[Τύπος SQL]],types,2,FALSE)</f>
+        <v>Ακέραιος μέχρι 65535</v>
+      </c>
+      <c r="C33" s="11" t="s">
+        <v>142</v>
+      </c>
+      <c r="D33" s="11" t="s">
+        <v>132</v>
+      </c>
+      <c r="E33" s="11"/>
+      <c r="F33" s="11"/>
+      <c r="G33" s="11"/>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A34" s="11" t="s">
+        <v>121</v>
+      </c>
+      <c r="B34" s="11" t="str">
+        <f>VLOOKUP(Πίνακας3[[#This Row],[Τύπος SQL]],types,2,FALSE)</f>
+        <v>Ναι/Όχι</v>
+      </c>
+      <c r="C34" s="11" t="s">
+        <v>127</v>
+      </c>
+      <c r="D34" s="11" t="s">
+        <v>132</v>
+      </c>
+      <c r="E34" s="11"/>
+      <c r="F34" s="11"/>
+      <c r="G34" s="11"/>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A35" s="11" t="s">
+        <v>122</v>
+      </c>
+      <c r="B35" s="11" t="str">
+        <f>VLOOKUP(Πίνακας3[[#This Row],[Τύπος SQL]],types,2,FALSE)</f>
+        <v>Ακέραιος μέχρι 65535</v>
+      </c>
+      <c r="C35" s="11" t="s">
+        <v>142</v>
+      </c>
+      <c r="D35" s="11" t="s">
+        <v>132</v>
+      </c>
+      <c r="E35" s="11"/>
+      <c r="F35" s="11"/>
+      <c r="G35" s="11"/>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A36" s="11" t="s">
+        <v>57</v>
+      </c>
+      <c r="B36" s="11" t="str">
+        <f>VLOOKUP(Πίνακας3[[#This Row],[Τύπος SQL]],types,2,FALSE)</f>
+        <v>Ναι/Όχι</v>
+      </c>
+      <c r="C36" s="11" t="s">
+        <v>127</v>
+      </c>
+      <c r="D36" s="11" t="s">
+        <v>132</v>
+      </c>
+      <c r="E36" s="11"/>
+      <c r="F36" s="11"/>
+      <c r="G36" s="11"/>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A37" s="11" t="s">
+        <v>70</v>
+      </c>
+      <c r="B37" s="11" t="str">
+        <f>VLOOKUP(Πίνακας3[[#This Row],[Τύπος SQL]],types,2,FALSE)</f>
+        <v>Ναι/Όχι</v>
+      </c>
+      <c r="C37" s="11" t="s">
+        <v>127</v>
+      </c>
+      <c r="D37" s="11" t="s">
+        <v>132</v>
+      </c>
+      <c r="E37" s="11"/>
+      <c r="F37" s="11"/>
+      <c r="G37" s="11"/>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A38" s="11" t="s">
+        <v>120</v>
+      </c>
+      <c r="B38" s="11" t="str">
+        <f>VLOOKUP(Πίνακας3[[#This Row],[Τύπος SQL]],types,2,FALSE)</f>
+        <v>Ακέραιος μέχρι 65535</v>
+      </c>
+      <c r="C38" s="11" t="s">
+        <v>142</v>
+      </c>
+      <c r="D38" s="11" t="s">
+        <v>132</v>
+      </c>
+      <c r="E38" s="11"/>
+      <c r="F38" s="11"/>
+      <c r="G38" s="11"/>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A39" s="11" t="s">
+        <v>143</v>
+      </c>
+      <c r="B39" s="11" t="str">
+        <f>VLOOKUP(Πίνακας3[[#This Row],[Τύπος SQL]],types,2,FALSE)</f>
+        <v>Μεγάλο κείμενο</v>
+      </c>
+      <c r="C39" s="11" t="s">
+        <v>144</v>
+      </c>
+      <c r="D39" s="11" t="s">
+        <v>132</v>
+      </c>
+      <c r="E39" s="11"/>
+      <c r="F39" s="11"/>
+      <c r="G39" s="11"/>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A40" s="11" t="s">
+        <v>74</v>
+      </c>
+      <c r="B40" s="11" t="str">
+        <f>VLOOKUP(Πίνακας3[[#This Row],[Τύπος SQL]],types,2,FALSE)</f>
+        <v>Ημερομηνία και Ώρα</v>
+      </c>
+      <c r="C40" s="11" t="s">
+        <v>145</v>
+      </c>
+      <c r="D40" s="11" t="s">
+        <v>124</v>
+      </c>
+      <c r="E40" s="11"/>
+      <c r="F40" s="11"/>
+      <c r="G40" s="11"/>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A41" s="11" t="s">
+        <v>75</v>
+      </c>
+      <c r="B41" s="11" t="str">
+        <f>VLOOKUP(Πίνακας3[[#This Row],[Τύπος SQL]],types,2,FALSE)</f>
+        <v>Ημερομηνία και Ώρα</v>
+      </c>
+      <c r="C41" s="11" t="s">
+        <v>145</v>
+      </c>
+      <c r="D41" s="11" t="s">
+        <v>124</v>
+      </c>
+      <c r="E41" s="11"/>
+      <c r="F41" s="11"/>
+      <c r="G41" s="11"/>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A42" s="11" t="s">
+        <v>73</v>
+      </c>
+      <c r="B42" s="11" t="str">
+        <f>VLOOKUP(Πίνακας3[[#This Row],[Τύπος SQL]],types,2,FALSE)</f>
+        <v>Σύντομο κείμενο</v>
+      </c>
+      <c r="C42" s="11" t="s">
+        <v>129</v>
+      </c>
+      <c r="D42" s="11" t="s">
+        <v>132</v>
+      </c>
+      <c r="E42" s="11" t="s">
+        <v>130</v>
+      </c>
+      <c r="F42" s="11"/>
+      <c r="G42" s="11"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
0.72 - new fields prod
</commit_message>
<xml_diff>
--- a/Docs/ΕΥΚΑΡΔΙΑ Πεδία Βάσης Δεδομένων.xlsx
+++ b/Docs/ΕΥΚΑΡΔΙΑ Πεδία Βάσης Δεδομένων.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Development\Eukardia\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2547805-38B5-4B4C-B499-02B7F2005D54}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01169EB7-9E24-4101-AA28-0ABA12F11CB5}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11625" tabRatio="481" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2025,7 +2025,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{13E70851-83B8-43A0-B14E-A8B2D42B9ED9}">
-  <dimension ref="A1:L42"/>
+  <dimension ref="A1:T42"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -2040,7 +2040,7 @@
     <col min="12" max="12" width="33.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>146</v>
       </c>
@@ -2068,8 +2068,14 @@
       <c r="L1" s="12" t="s">
         <v>147</v>
       </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="O1" s="11"/>
+      <c r="P1" s="11"/>
+      <c r="Q1" s="11"/>
+      <c r="R1" s="11"/>
+      <c r="S1" s="11"/>
+      <c r="T1" s="11"/>
+    </row>
+    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A2" s="11" t="s">
         <v>72</v>
       </c>
@@ -2090,14 +2096,21 @@
       <c r="G2" s="11" t="s">
         <v>126</v>
       </c>
+      <c r="I2" s="11"/>
       <c r="K2" s="13" t="s">
         <v>123</v>
       </c>
       <c r="L2" t="s">
         <v>156</v>
       </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="O2" s="11"/>
+      <c r="P2" s="11"/>
+      <c r="Q2" s="11"/>
+      <c r="R2" s="11"/>
+      <c r="S2" s="11"/>
+      <c r="T2" s="11"/>
+    </row>
+    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A3" s="11" t="s">
         <v>52</v>
       </c>
@@ -2116,14 +2129,21 @@
         <v>0</v>
       </c>
       <c r="G3" s="11"/>
+      <c r="I3" s="11"/>
       <c r="K3" s="13" t="s">
         <v>127</v>
       </c>
       <c r="L3" t="s">
         <v>118</v>
       </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="O3" s="11"/>
+      <c r="P3" s="11"/>
+      <c r="Q3" s="11"/>
+      <c r="R3" s="11"/>
+      <c r="S3" s="11"/>
+      <c r="T3" s="11"/>
+    </row>
+    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A4" s="11" t="s">
         <v>128</v>
       </c>
@@ -2142,14 +2162,21 @@
       </c>
       <c r="F4" s="11"/>
       <c r="G4" s="11"/>
+      <c r="I4" s="11"/>
       <c r="K4" s="13" t="s">
         <v>129</v>
       </c>
       <c r="L4" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="O4" s="11"/>
+      <c r="P4" s="11"/>
+      <c r="Q4" s="11"/>
+      <c r="R4" s="11"/>
+      <c r="S4" s="11"/>
+      <c r="T4" s="11"/>
+    </row>
+    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A5" s="11" t="s">
         <v>54</v>
       </c>
@@ -2166,14 +2193,21 @@
       <c r="E5" s="11"/>
       <c r="F5" s="11"/>
       <c r="G5" s="11"/>
+      <c r="I5" s="11"/>
       <c r="K5" s="13" t="s">
         <v>131</v>
       </c>
       <c r="L5" t="s">
         <v>157</v>
       </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="O5" s="11"/>
+      <c r="P5" s="11"/>
+      <c r="Q5" s="11"/>
+      <c r="R5" s="11"/>
+      <c r="S5" s="11"/>
+      <c r="T5" s="11"/>
+    </row>
+    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A6" s="11" t="s">
         <v>55</v>
       </c>
@@ -2190,14 +2224,21 @@
       <c r="E6" s="11"/>
       <c r="F6" s="11"/>
       <c r="G6" s="11"/>
+      <c r="I6" s="11"/>
       <c r="K6" s="13" t="s">
         <v>135</v>
       </c>
       <c r="L6" t="s">
         <v>154</v>
       </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="O6" s="11"/>
+      <c r="P6" s="11"/>
+      <c r="Q6" s="11"/>
+      <c r="R6" s="11"/>
+      <c r="S6" s="11"/>
+      <c r="T6" s="11"/>
+    </row>
+    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A7" s="11" t="s">
         <v>133</v>
       </c>
@@ -2214,14 +2255,21 @@
       <c r="E7" s="11"/>
       <c r="F7" s="11"/>
       <c r="G7" s="11"/>
+      <c r="I7" s="11"/>
       <c r="K7" s="13" t="s">
         <v>142</v>
       </c>
       <c r="L7" t="s">
         <v>155</v>
       </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="O7" s="11"/>
+      <c r="P7" s="11"/>
+      <c r="Q7" s="11"/>
+      <c r="R7" s="11"/>
+      <c r="S7" s="11"/>
+      <c r="T7" s="11"/>
+    </row>
+    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A8" s="11" t="s">
         <v>134</v>
       </c>
@@ -2238,14 +2286,21 @@
       <c r="E8" s="11"/>
       <c r="F8" s="11"/>
       <c r="G8" s="11"/>
+      <c r="I8" s="11"/>
       <c r="K8" s="13" t="s">
         <v>144</v>
       </c>
       <c r="L8" t="s">
         <v>152</v>
       </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="O8" s="11"/>
+      <c r="P8" s="11"/>
+      <c r="Q8" s="11"/>
+      <c r="R8" s="11"/>
+      <c r="S8" s="11"/>
+      <c r="T8" s="11"/>
+    </row>
+    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A9" s="11" t="s">
         <v>136</v>
       </c>
@@ -2262,14 +2317,21 @@
       <c r="E9" s="11"/>
       <c r="F9" s="11"/>
       <c r="G9" s="11"/>
+      <c r="I9" s="11"/>
       <c r="K9" s="13" t="s">
         <v>145</v>
       </c>
       <c r="L9" t="s">
         <v>153</v>
       </c>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="O9" s="11"/>
+      <c r="P9" s="11"/>
+      <c r="Q9" s="11"/>
+      <c r="R9" s="11"/>
+      <c r="S9" s="11"/>
+      <c r="T9" s="11"/>
+    </row>
+    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A10" s="11" t="s">
         <v>56</v>
       </c>
@@ -2286,8 +2348,15 @@
       <c r="E10" s="11"/>
       <c r="F10" s="11"/>
       <c r="G10" s="11"/>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="I10" s="11"/>
+      <c r="O10" s="11"/>
+      <c r="P10" s="11"/>
+      <c r="Q10" s="11"/>
+      <c r="R10" s="11"/>
+      <c r="S10" s="11"/>
+      <c r="T10" s="11"/>
+    </row>
+    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A11" s="11" t="s">
         <v>68</v>
       </c>
@@ -2304,8 +2373,15 @@
       <c r="E11" s="11"/>
       <c r="F11" s="11"/>
       <c r="G11" s="11"/>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="I11" s="11"/>
+      <c r="O11" s="11"/>
+      <c r="P11" s="11"/>
+      <c r="Q11" s="11"/>
+      <c r="R11" s="11"/>
+      <c r="S11" s="11"/>
+      <c r="T11" s="11"/>
+    </row>
+    <row r="12" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A12" s="11" t="s">
         <v>137</v>
       </c>
@@ -2322,8 +2398,15 @@
       <c r="E12" s="11"/>
       <c r="F12" s="11"/>
       <c r="G12" s="11"/>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="I12" s="11"/>
+      <c r="O12" s="11"/>
+      <c r="P12" s="11"/>
+      <c r="Q12" s="11"/>
+      <c r="R12" s="11"/>
+      <c r="S12" s="11"/>
+      <c r="T12" s="11"/>
+    </row>
+    <row r="13" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A13" s="11" t="s">
         <v>58</v>
       </c>
@@ -2340,8 +2423,15 @@
       <c r="E13" s="11"/>
       <c r="F13" s="11"/>
       <c r="G13" s="11"/>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="I13" s="11"/>
+      <c r="O13" s="11"/>
+      <c r="P13" s="11"/>
+      <c r="Q13" s="11"/>
+      <c r="R13" s="11"/>
+      <c r="S13" s="11"/>
+      <c r="T13" s="11"/>
+    </row>
+    <row r="14" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A14" s="11" t="s">
         <v>59</v>
       </c>
@@ -2358,8 +2448,15 @@
       <c r="E14" s="11"/>
       <c r="F14" s="11"/>
       <c r="G14" s="11"/>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="I14" s="11"/>
+      <c r="O14" s="11"/>
+      <c r="P14" s="11"/>
+      <c r="Q14" s="11"/>
+      <c r="R14" s="11"/>
+      <c r="S14" s="11"/>
+      <c r="T14" s="11"/>
+    </row>
+    <row r="15" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A15" s="11" t="s">
         <v>109</v>
       </c>
@@ -2376,8 +2473,15 @@
       <c r="E15" s="11"/>
       <c r="F15" s="11"/>
       <c r="G15" s="11"/>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="I15" s="11"/>
+      <c r="O15" s="11"/>
+      <c r="P15" s="11"/>
+      <c r="Q15" s="11"/>
+      <c r="R15" s="11"/>
+      <c r="S15" s="11"/>
+      <c r="T15" s="11"/>
+    </row>
+    <row r="16" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A16" s="11" t="s">
         <v>60</v>
       </c>
@@ -2394,8 +2498,15 @@
       <c r="E16" s="11"/>
       <c r="F16" s="11"/>
       <c r="G16" s="11"/>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I16" s="11"/>
+      <c r="O16" s="11"/>
+      <c r="P16" s="11"/>
+      <c r="Q16" s="11"/>
+      <c r="R16" s="11"/>
+      <c r="S16" s="11"/>
+      <c r="T16" s="11"/>
+    </row>
+    <row r="17" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A17" s="11" t="s">
         <v>138</v>
       </c>
@@ -2412,8 +2523,15 @@
       <c r="E17" s="11"/>
       <c r="F17" s="11"/>
       <c r="G17" s="11"/>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I17" s="11"/>
+      <c r="O17" s="11"/>
+      <c r="P17" s="11"/>
+      <c r="Q17" s="11"/>
+      <c r="R17" s="11"/>
+      <c r="S17" s="11"/>
+      <c r="T17" s="11"/>
+    </row>
+    <row r="18" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A18" s="11" t="s">
         <v>84</v>
       </c>
@@ -2430,8 +2548,15 @@
       <c r="E18" s="11"/>
       <c r="F18" s="11"/>
       <c r="G18" s="11"/>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I18" s="11"/>
+      <c r="O18" s="11"/>
+      <c r="P18" s="11"/>
+      <c r="Q18" s="11"/>
+      <c r="R18" s="11"/>
+      <c r="S18" s="11"/>
+      <c r="T18" s="11"/>
+    </row>
+    <row r="19" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A19" s="11" t="s">
         <v>61</v>
       </c>
@@ -2448,8 +2573,15 @@
       <c r="E19" s="11"/>
       <c r="F19" s="11"/>
       <c r="G19" s="11"/>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I19" s="11"/>
+      <c r="O19" s="11"/>
+      <c r="P19" s="11"/>
+      <c r="Q19" s="11"/>
+      <c r="R19" s="11"/>
+      <c r="S19" s="11"/>
+      <c r="T19" s="11"/>
+    </row>
+    <row r="20" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A20" s="11" t="s">
         <v>66</v>
       </c>
@@ -2466,8 +2598,15 @@
       <c r="E20" s="11"/>
       <c r="F20" s="11"/>
       <c r="G20" s="11"/>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I20" s="11"/>
+      <c r="O20" s="11"/>
+      <c r="P20" s="11"/>
+      <c r="Q20" s="11"/>
+      <c r="R20" s="11"/>
+      <c r="S20" s="11"/>
+      <c r="T20" s="11"/>
+    </row>
+    <row r="21" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A21" s="11" t="s">
         <v>67</v>
       </c>
@@ -2484,8 +2623,15 @@
       <c r="E21" s="11"/>
       <c r="F21" s="11"/>
       <c r="G21" s="11"/>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I21" s="11"/>
+      <c r="O21" s="11"/>
+      <c r="P21" s="11"/>
+      <c r="Q21" s="11"/>
+      <c r="R21" s="11"/>
+      <c r="S21" s="11"/>
+      <c r="T21" s="11"/>
+    </row>
+    <row r="22" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A22" s="11" t="s">
         <v>62</v>
       </c>
@@ -2502,8 +2648,15 @@
       <c r="E22" s="11"/>
       <c r="F22" s="11"/>
       <c r="G22" s="11"/>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I22" s="11"/>
+      <c r="O22" s="11"/>
+      <c r="P22" s="11"/>
+      <c r="Q22" s="11"/>
+      <c r="R22" s="11"/>
+      <c r="S22" s="11"/>
+      <c r="T22" s="11"/>
+    </row>
+    <row r="23" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A23" s="11" t="s">
         <v>63</v>
       </c>
@@ -2520,8 +2673,15 @@
       <c r="E23" s="11"/>
       <c r="F23" s="11"/>
       <c r="G23" s="11"/>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I23" s="11"/>
+      <c r="O23" s="11"/>
+      <c r="P23" s="11"/>
+      <c r="Q23" s="11"/>
+      <c r="R23" s="11"/>
+      <c r="S23" s="11"/>
+      <c r="T23" s="11"/>
+    </row>
+    <row r="24" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A24" s="11" t="s">
         <v>77</v>
       </c>
@@ -2538,8 +2698,15 @@
       <c r="E24" s="11"/>
       <c r="F24" s="11"/>
       <c r="G24" s="11"/>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I24" s="11"/>
+      <c r="O24" s="11"/>
+      <c r="P24" s="11"/>
+      <c r="Q24" s="11"/>
+      <c r="R24" s="11"/>
+      <c r="S24" s="11"/>
+      <c r="T24" s="11"/>
+    </row>
+    <row r="25" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A25" s="11" t="s">
         <v>94</v>
       </c>
@@ -2556,8 +2723,15 @@
       <c r="E25" s="11"/>
       <c r="F25" s="11"/>
       <c r="G25" s="11"/>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I25" s="11"/>
+      <c r="O25" s="11"/>
+      <c r="P25" s="11"/>
+      <c r="Q25" s="11"/>
+      <c r="R25" s="11"/>
+      <c r="S25" s="11"/>
+      <c r="T25" s="11"/>
+    </row>
+    <row r="26" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A26" s="11" t="s">
         <v>64</v>
       </c>
@@ -2574,8 +2748,15 @@
       <c r="E26" s="11"/>
       <c r="F26" s="11"/>
       <c r="G26" s="11"/>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I26" s="11"/>
+      <c r="O26" s="11"/>
+      <c r="P26" s="11"/>
+      <c r="Q26" s="11"/>
+      <c r="R26" s="11"/>
+      <c r="S26" s="11"/>
+      <c r="T26" s="11"/>
+    </row>
+    <row r="27" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A27" s="11" t="s">
         <v>82</v>
       </c>
@@ -2592,8 +2773,15 @@
       <c r="E27" s="11"/>
       <c r="F27" s="11"/>
       <c r="G27" s="11"/>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I27" s="11"/>
+      <c r="O27" s="11"/>
+      <c r="P27" s="11"/>
+      <c r="Q27" s="11"/>
+      <c r="R27" s="11"/>
+      <c r="S27" s="11"/>
+      <c r="T27" s="11"/>
+    </row>
+    <row r="28" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A28" s="11" t="s">
         <v>65</v>
       </c>
@@ -2610,8 +2798,15 @@
       <c r="E28" s="11"/>
       <c r="F28" s="11"/>
       <c r="G28" s="11"/>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I28" s="11"/>
+      <c r="O28" s="11"/>
+      <c r="P28" s="11"/>
+      <c r="Q28" s="11"/>
+      <c r="R28" s="11"/>
+      <c r="S28" s="11"/>
+      <c r="T28" s="11"/>
+    </row>
+    <row r="29" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A29" s="11" t="s">
         <v>71</v>
       </c>
@@ -2628,8 +2823,15 @@
       <c r="E29" s="11"/>
       <c r="F29" s="11"/>
       <c r="G29" s="11"/>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I29" s="11"/>
+      <c r="O29" s="11"/>
+      <c r="P29" s="11"/>
+      <c r="Q29" s="11"/>
+      <c r="R29" s="11"/>
+      <c r="S29" s="11"/>
+      <c r="T29" s="11"/>
+    </row>
+    <row r="30" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A30" s="11" t="s">
         <v>139</v>
       </c>
@@ -2646,8 +2848,15 @@
       <c r="E30" s="11"/>
       <c r="F30" s="11"/>
       <c r="G30" s="11"/>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I30" s="11"/>
+      <c r="O30" s="11"/>
+      <c r="P30" s="11"/>
+      <c r="Q30" s="11"/>
+      <c r="R30" s="11"/>
+      <c r="S30" s="11"/>
+      <c r="T30" s="11"/>
+    </row>
+    <row r="31" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A31" s="11" t="s">
         <v>69</v>
       </c>
@@ -2664,8 +2873,15 @@
       <c r="E31" s="11"/>
       <c r="F31" s="11"/>
       <c r="G31" s="11"/>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I31" s="11"/>
+      <c r="O31" s="11"/>
+      <c r="P31" s="11"/>
+      <c r="Q31" s="11"/>
+      <c r="R31" s="11"/>
+      <c r="S31" s="11"/>
+      <c r="T31" s="11"/>
+    </row>
+    <row r="32" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A32" s="11" t="s">
         <v>140</v>
       </c>
@@ -2682,8 +2898,15 @@
       <c r="E32" s="11"/>
       <c r="F32" s="11"/>
       <c r="G32" s="11"/>
-    </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I32" s="11"/>
+      <c r="O32" s="11"/>
+      <c r="P32" s="11"/>
+      <c r="Q32" s="11"/>
+      <c r="R32" s="11"/>
+      <c r="S32" s="11"/>
+      <c r="T32" s="11"/>
+    </row>
+    <row r="33" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A33" s="11" t="s">
         <v>141</v>
       </c>
@@ -2700,8 +2923,15 @@
       <c r="E33" s="11"/>
       <c r="F33" s="11"/>
       <c r="G33" s="11"/>
-    </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I33" s="11"/>
+      <c r="O33" s="11"/>
+      <c r="P33" s="11"/>
+      <c r="Q33" s="11"/>
+      <c r="R33" s="11"/>
+      <c r="S33" s="11"/>
+      <c r="T33" s="11"/>
+    </row>
+    <row r="34" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A34" s="11" t="s">
         <v>121</v>
       </c>
@@ -2718,8 +2948,15 @@
       <c r="E34" s="11"/>
       <c r="F34" s="11"/>
       <c r="G34" s="11"/>
-    </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I34" s="11"/>
+      <c r="O34" s="11"/>
+      <c r="P34" s="11"/>
+      <c r="Q34" s="11"/>
+      <c r="R34" s="11"/>
+      <c r="S34" s="11"/>
+      <c r="T34" s="11"/>
+    </row>
+    <row r="35" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A35" s="11" t="s">
         <v>122</v>
       </c>
@@ -2736,8 +2973,15 @@
       <c r="E35" s="11"/>
       <c r="F35" s="11"/>
       <c r="G35" s="11"/>
-    </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I35" s="11"/>
+      <c r="O35" s="11"/>
+      <c r="P35" s="11"/>
+      <c r="Q35" s="11"/>
+      <c r="R35" s="11"/>
+      <c r="S35" s="11"/>
+      <c r="T35" s="11"/>
+    </row>
+    <row r="36" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A36" s="11" t="s">
         <v>57</v>
       </c>
@@ -2754,8 +2998,15 @@
       <c r="E36" s="11"/>
       <c r="F36" s="11"/>
       <c r="G36" s="11"/>
-    </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I36" s="11"/>
+      <c r="O36" s="11"/>
+      <c r="P36" s="11"/>
+      <c r="Q36" s="11"/>
+      <c r="R36" s="11"/>
+      <c r="S36" s="11"/>
+      <c r="T36" s="11"/>
+    </row>
+    <row r="37" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A37" s="11" t="s">
         <v>70</v>
       </c>
@@ -2772,8 +3023,15 @@
       <c r="E37" s="11"/>
       <c r="F37" s="11"/>
       <c r="G37" s="11"/>
-    </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I37" s="11"/>
+      <c r="O37" s="11"/>
+      <c r="P37" s="11"/>
+      <c r="Q37" s="11"/>
+      <c r="R37" s="11"/>
+      <c r="S37" s="11"/>
+      <c r="T37" s="11"/>
+    </row>
+    <row r="38" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A38" s="11" t="s">
         <v>120</v>
       </c>
@@ -2790,8 +3048,15 @@
       <c r="E38" s="11"/>
       <c r="F38" s="11"/>
       <c r="G38" s="11"/>
-    </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I38" s="11"/>
+      <c r="O38" s="11"/>
+      <c r="P38" s="11"/>
+      <c r="Q38" s="11"/>
+      <c r="R38" s="11"/>
+      <c r="S38" s="11"/>
+      <c r="T38" s="11"/>
+    </row>
+    <row r="39" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A39" s="11" t="s">
         <v>143</v>
       </c>
@@ -2808,8 +3073,15 @@
       <c r="E39" s="11"/>
       <c r="F39" s="11"/>
       <c r="G39" s="11"/>
-    </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I39" s="11"/>
+      <c r="O39" s="11"/>
+      <c r="P39" s="11"/>
+      <c r="Q39" s="11"/>
+      <c r="R39" s="11"/>
+      <c r="S39" s="11"/>
+      <c r="T39" s="11"/>
+    </row>
+    <row r="40" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A40" s="11" t="s">
         <v>74</v>
       </c>
@@ -2826,8 +3098,15 @@
       <c r="E40" s="11"/>
       <c r="F40" s="11"/>
       <c r="G40" s="11"/>
-    </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I40" s="11"/>
+      <c r="O40" s="11"/>
+      <c r="P40" s="11"/>
+      <c r="Q40" s="11"/>
+      <c r="R40" s="11"/>
+      <c r="S40" s="11"/>
+      <c r="T40" s="11"/>
+    </row>
+    <row r="41" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A41" s="11" t="s">
         <v>75</v>
       </c>
@@ -2844,8 +3123,15 @@
       <c r="E41" s="11"/>
       <c r="F41" s="11"/>
       <c r="G41" s="11"/>
-    </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I41" s="11"/>
+      <c r="O41" s="11"/>
+      <c r="P41" s="11"/>
+      <c r="Q41" s="11"/>
+      <c r="R41" s="11"/>
+      <c r="S41" s="11"/>
+      <c r="T41" s="11"/>
+    </row>
+    <row r="42" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A42" s="11" t="s">
         <v>73</v>
       </c>
@@ -2864,6 +3150,13 @@
       </c>
       <c r="F42" s="11"/>
       <c r="G42" s="11"/>
+      <c r="I42" s="11"/>
+      <c r="O42" s="11"/>
+      <c r="P42" s="11"/>
+      <c r="Q42" s="11"/>
+      <c r="R42" s="11"/>
+      <c r="S42" s="11"/>
+      <c r="T42" s="11"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
0.8 - duplicate warning
</commit_message>
<xml_diff>
--- a/Docs/ΕΥΚΑΡΔΙΑ Πεδία Βάσης Δεδομένων.xlsx
+++ b/Docs/ΕΥΚΑΡΔΙΑ Πεδία Βάσης Δεδομένων.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Development\Eukardia\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01169EB7-9E24-4101-AA28-0ABA12F11CB5}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4207EED7-8749-4426-82D8-7DC791F4DFE9}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11625" tabRatio="481" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="353" uniqueCount="158">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="354" uniqueCount="159">
   <si>
     <t>Όνομα πεδίου</t>
   </si>
@@ -504,6 +504,9 @@
   </si>
   <si>
     <t xml:space="preserve">Ακέραιος ή λίστα μέχρι 127 </t>
+  </si>
+  <si>
+    <t>SQL view</t>
   </si>
 </sst>
 </file>
@@ -656,7 +659,7 @@
   <cellStyles count="1">
     <cellStyle name="Κανονικό" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="27">
+  <dxfs count="28">
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -674,6 +677,10 @@
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -959,50 +966,53 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Πίνακας1" displayName="Πίνακας1" ref="A1:G37" totalsRowShown="0" headerRowDxfId="26" dataDxfId="25">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Πίνακας1" displayName="Πίνακας1" ref="A1:G37" totalsRowShown="0" headerRowDxfId="27" dataDxfId="26">
   <autoFilter ref="A1:G37" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Περιγραφή πεδίου" dataDxfId="24"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Υποχρεωτική συμπλήρωση" dataDxfId="23"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="Όνομα πεδίου βάσης" dataDxfId="22"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Τύπος" dataDxfId="21"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Μονάδες μέτρησης" dataDxfId="20"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Επιτρεπόμενες τιμές ή εύρος τιμών" dataDxfId="19"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Περιγραφή" dataDxfId="18"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Περιγραφή πεδίου" dataDxfId="25"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Υποχρεωτική συμπλήρωση" dataDxfId="24"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="Όνομα πεδίου βάσης" dataDxfId="23"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Τύπος" dataDxfId="22"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Μονάδες μέτρησης" dataDxfId="21"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Επιτρεπόμενες τιμές ή εύρος τιμών" dataDxfId="20"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Περιγραφή" dataDxfId="19"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight13" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Πίνακας2" displayName="Πίνακας2" ref="A42:G46" totalsRowShown="0" headerRowDxfId="17" dataDxfId="16" tableBorderDxfId="15">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Πίνακας2" displayName="Πίνακας2" ref="A42:G46" totalsRowShown="0" headerRowDxfId="18" dataDxfId="17" tableBorderDxfId="16">
   <autoFilter ref="A42:G46" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="Όνομα πεδίου" dataDxfId="14"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0100-000004000000}" name="Υποχρεωτικό" dataDxfId="13"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0100-000007000000}" name="Πεδίο βάσης" dataDxfId="12"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="Τύπος" dataDxfId="11"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="Μονάδες μέτρησης" dataDxfId="10"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0100-000005000000}" name="Επιτρεπόμενες τιμές" dataDxfId="9"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0100-000006000000}" name="Περιγραφή" dataDxfId="8"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="Όνομα πεδίου" dataDxfId="15"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0100-000004000000}" name="Υποχρεωτικό" dataDxfId="14"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0100-000007000000}" name="Πεδίο βάσης" dataDxfId="13"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="Τύπος" dataDxfId="12"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="Μονάδες μέτρησης" dataDxfId="11"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0100-000005000000}" name="Επιτρεπόμενες τιμές" dataDxfId="10"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0100-000006000000}" name="Περιγραφή" dataDxfId="9"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight12" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{124B803E-62B7-4DF6-97EB-31E33393CFE8}" name="Πίνακας3" displayName="Πίνακας3" ref="A1:G42" totalsRowShown="0" dataDxfId="1">
-  <autoFilter ref="A1:G42" xr:uid="{89C5C1E3-CE08-4CF4-BF51-207D1F88BF61}"/>
-  <tableColumns count="7">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{124B803E-62B7-4DF6-97EB-31E33393CFE8}" name="Πίνακας3" displayName="Πίνακας3" ref="A1:H42" totalsRowShown="0" dataDxfId="8">
+  <autoFilter ref="A1:H42" xr:uid="{89C5C1E3-CE08-4CF4-BF51-207D1F88BF61}"/>
+  <tableColumns count="8">
     <tableColumn id="1" xr3:uid="{310BA3A6-8BAB-4AFE-9044-3DBC1F268DB3}" name="Πεδίο" dataDxfId="7"/>
-    <tableColumn id="2" xr3:uid="{3986543B-C60B-42C6-BDEF-7981CFB32FA8}" name="Τύπος (κατανοητός)" dataDxfId="0">
+    <tableColumn id="2" xr3:uid="{3986543B-C60B-42C6-BDEF-7981CFB32FA8}" name="Τύπος (κατανοητός)" dataDxfId="6">
       <calculatedColumnFormula>VLOOKUP(Πίνακας3[[#This Row],[Τύπος SQL]],types,2,FALSE)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{BD85B841-8B4D-4BCC-B5C9-A161325437D0}" name="Τύπος SQL" dataDxfId="6"/>
-    <tableColumn id="4" xr3:uid="{72048646-56D9-4F1A-9344-EFC38B058077}" name="Υποχρεωτικό" dataDxfId="5"/>
-    <tableColumn id="5" xr3:uid="{EF472430-A112-45C0-A202-A1F958E3AB86}" name="Key" dataDxfId="4"/>
-    <tableColumn id="6" xr3:uid="{7A28CF5F-9508-41CD-A516-6F0B3FB0681E}" name="Default value" dataDxfId="3"/>
-    <tableColumn id="7" xr3:uid="{A4C62788-3491-4A41-9F8A-B8B83DEFB0B7}" name="Extra" dataDxfId="2"/>
+    <tableColumn id="3" xr3:uid="{BD85B841-8B4D-4BCC-B5C9-A161325437D0}" name="Τύπος SQL" dataDxfId="5"/>
+    <tableColumn id="4" xr3:uid="{72048646-56D9-4F1A-9344-EFC38B058077}" name="Υποχρεωτικό" dataDxfId="4"/>
+    <tableColumn id="5" xr3:uid="{EF472430-A112-45C0-A202-A1F958E3AB86}" name="Key" dataDxfId="3"/>
+    <tableColumn id="6" xr3:uid="{7A28CF5F-9508-41CD-A516-6F0B3FB0681E}" name="Default value" dataDxfId="2"/>
+    <tableColumn id="7" xr3:uid="{A4C62788-3491-4A41-9F8A-B8B83DEFB0B7}" name="Extra" dataDxfId="1"/>
+    <tableColumn id="8" xr3:uid="{FB2D05D5-FCD5-4649-95BD-DC58D8DC278B}" name="SQL view" dataDxfId="0">
+      <calculatedColumnFormula>"`cases`.`"&amp;Πίνακας3[[#This Row],[Πεδίο]]&amp;"` AS `"&amp;Πίνακας3[[#This Row],[Πεδίο]]&amp;"`,"</calculatedColumnFormula>
+    </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight14" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2027,7 +2037,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{13E70851-83B8-43A0-B14E-A8B2D42B9ED9}">
   <dimension ref="A1:T42"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="H7" sqref="H7:H41"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="25.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -2037,6 +2049,7 @@
     <col min="4" max="4" width="15.140625" bestFit="1" customWidth="1"/>
     <col min="5" max="6" width="9.28515625" customWidth="1"/>
     <col min="7" max="7" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="41.28515625" customWidth="1"/>
     <col min="12" max="12" width="33.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -2062,6 +2075,9 @@
       <c r="G1" t="s">
         <v>151</v>
       </c>
+      <c r="H1" t="s">
+        <v>158</v>
+      </c>
       <c r="K1" s="12" t="s">
         <v>148</v>
       </c>
@@ -2096,6 +2112,10 @@
       <c r="G2" s="11" t="s">
         <v>126</v>
       </c>
+      <c r="H2" s="11" t="str">
+        <f>"`cases`.`"&amp;Πίνακας3[[#This Row],[Πεδίο]]&amp;"` AS `"&amp;Πίνακας3[[#This Row],[Πεδίο]]&amp;"`,"</f>
+        <v>`cases`.`id` AS `id`,</v>
+      </c>
       <c r="I2" s="11"/>
       <c r="K2" s="13" t="s">
         <v>123</v>
@@ -2129,6 +2149,10 @@
         <v>0</v>
       </c>
       <c r="G3" s="11"/>
+      <c r="H3" s="11" t="str">
+        <f>"`cases`.`"&amp;Πίνακας3[[#This Row],[Πεδίο]]&amp;"` AS `"&amp;Πίνακας3[[#This Row],[Πεδίο]]&amp;"`,"</f>
+        <v>`cases`.`testPatient` AS `testPatient`,</v>
+      </c>
       <c r="I3" s="11"/>
       <c r="K3" s="13" t="s">
         <v>127</v>
@@ -2162,6 +2186,10 @@
       </c>
       <c r="F4" s="11"/>
       <c r="G4" s="11"/>
+      <c r="H4" s="11" t="str">
+        <f>"`cases`.`"&amp;Πίνακας3[[#This Row],[Πεδίο]]&amp;"` AS `"&amp;Πίνακας3[[#This Row],[Πεδίο]]&amp;"`,"</f>
+        <v>`cases`.`patientId` AS `patientId`,</v>
+      </c>
       <c r="I4" s="11"/>
       <c r="K4" s="13" t="s">
         <v>129</v>
@@ -2193,6 +2221,10 @@
       <c r="E5" s="11"/>
       <c r="F5" s="11"/>
       <c r="G5" s="11"/>
+      <c r="H5" s="11" t="str">
+        <f>"`cases`.`"&amp;Πίνακας3[[#This Row],[Πεδίο]]&amp;"` AS `"&amp;Πίνακας3[[#This Row],[Πεδίο]]&amp;"`,"</f>
+        <v>`cases`.`gender` AS `gender`,</v>
+      </c>
       <c r="I5" s="11"/>
       <c r="K5" s="13" t="s">
         <v>131</v>
@@ -2224,6 +2256,10 @@
       <c r="E6" s="11"/>
       <c r="F6" s="11"/>
       <c r="G6" s="11"/>
+      <c r="H6" s="11" t="str">
+        <f>"`cases`.`"&amp;Πίνακας3[[#This Row],[Πεδίο]]&amp;"` AS `"&amp;Πίνακας3[[#This Row],[Πεδίο]]&amp;"`,"</f>
+        <v>`cases`.`age` AS `age`,</v>
+      </c>
       <c r="I6" s="11"/>
       <c r="K6" s="13" t="s">
         <v>135</v>
@@ -2255,6 +2291,10 @@
       <c r="E7" s="11"/>
       <c r="F7" s="11"/>
       <c r="G7" s="11"/>
+      <c r="H7" s="11" t="str">
+        <f>"`cases`.`"&amp;Πίνακας3[[#This Row],[Πεδίο]]&amp;"` AS `"&amp;Πίνακας3[[#This Row],[Πεδίο]]&amp;"`,"</f>
+        <v>`cases`.`drugbp` AS `drugbp`,</v>
+      </c>
       <c r="I7" s="11"/>
       <c r="K7" s="13" t="s">
         <v>142</v>
@@ -2286,6 +2326,10 @@
       <c r="E8" s="11"/>
       <c r="F8" s="11"/>
       <c r="G8" s="11"/>
+      <c r="H8" s="11" t="str">
+        <f>"`cases`.`"&amp;Πίνακας3[[#This Row],[Πεδίο]]&amp;"` AS `"&amp;Πίνακας3[[#This Row],[Πεδίο]]&amp;"`,"</f>
+        <v>`cases`.`sbp` AS `sbp`,</v>
+      </c>
       <c r="I8" s="11"/>
       <c r="K8" s="13" t="s">
         <v>144</v>
@@ -2317,6 +2361,10 @@
       <c r="E9" s="11"/>
       <c r="F9" s="11"/>
       <c r="G9" s="11"/>
+      <c r="H9" s="11" t="str">
+        <f>"`cases`.`"&amp;Πίνακας3[[#This Row],[Πεδίο]]&amp;"` AS `"&amp;Πίνακας3[[#This Row],[Πεδίο]]&amp;"`,"</f>
+        <v>`cases`.`dbp` AS `dbp`,</v>
+      </c>
       <c r="I9" s="11"/>
       <c r="K9" s="13" t="s">
         <v>145</v>
@@ -2348,6 +2396,10 @@
       <c r="E10" s="11"/>
       <c r="F10" s="11"/>
       <c r="G10" s="11"/>
+      <c r="H10" s="11" t="str">
+        <f>"`cases`.`"&amp;Πίνακας3[[#This Row],[Πεδίο]]&amp;"` AS `"&amp;Πίνακας3[[#This Row],[Πεδίο]]&amp;"`,"</f>
+        <v>`cases`.`glucose` AS `glucose`,</v>
+      </c>
       <c r="I10" s="11"/>
       <c r="O10" s="11"/>
       <c r="P10" s="11"/>
@@ -2373,6 +2425,10 @@
       <c r="E11" s="11"/>
       <c r="F11" s="11"/>
       <c r="G11" s="11"/>
+      <c r="H11" s="11" t="str">
+        <f>"`cases`.`"&amp;Πίνακας3[[#This Row],[Πεδίο]]&amp;"` AS `"&amp;Πίνακας3[[#This Row],[Πεδίο]]&amp;"`,"</f>
+        <v>`cases`.`hba1c` AS `hba1c`,</v>
+      </c>
       <c r="I11" s="11"/>
       <c r="O11" s="11"/>
       <c r="P11" s="11"/>
@@ -2398,6 +2454,10 @@
       <c r="E12" s="11"/>
       <c r="F12" s="11"/>
       <c r="G12" s="11"/>
+      <c r="H12" s="11" t="str">
+        <f>"`cases`.`"&amp;Πίνακας3[[#This Row],[Πεδίο]]&amp;"` AS `"&amp;Πίνακας3[[#This Row],[Πεδίο]]&amp;"`,"</f>
+        <v>`cases`.`diebetes` AS `diebetes`,</v>
+      </c>
       <c r="I12" s="11"/>
       <c r="O12" s="11"/>
       <c r="P12" s="11"/>
@@ -2423,6 +2483,10 @@
       <c r="E13" s="11"/>
       <c r="F13" s="11"/>
       <c r="G13" s="11"/>
+      <c r="H13" s="11" t="str">
+        <f>"`cases`.`"&amp;Πίνακας3[[#This Row],[Πεδίο]]&amp;"` AS `"&amp;Πίνακας3[[#This Row],[Πεδίο]]&amp;"`,"</f>
+        <v>`cases`.`activity` AS `activity`,</v>
+      </c>
       <c r="I13" s="11"/>
       <c r="O13" s="11"/>
       <c r="P13" s="11"/>
@@ -2448,6 +2512,10 @@
       <c r="E14" s="11"/>
       <c r="F14" s="11"/>
       <c r="G14" s="11"/>
+      <c r="H14" s="11" t="str">
+        <f>"`cases`.`"&amp;Πίνακας3[[#This Row],[Πεδίο]]&amp;"` AS `"&amp;Πίνακας3[[#This Row],[Πεδίο]]&amp;"`,"</f>
+        <v>`cases`.`diet` AS `diet`,</v>
+      </c>
       <c r="I14" s="11"/>
       <c r="O14" s="11"/>
       <c r="P14" s="11"/>
@@ -2473,6 +2541,10 @@
       <c r="E15" s="11"/>
       <c r="F15" s="11"/>
       <c r="G15" s="11"/>
+      <c r="H15" s="11" t="str">
+        <f>"`cases`.`"&amp;Πίνακας3[[#This Row],[Πεδίο]]&amp;"` AS `"&amp;Πίνακας3[[#This Row],[Πεδίο]]&amp;"`,"</f>
+        <v>`cases`.`alcohol` AS `alcohol`,</v>
+      </c>
       <c r="I15" s="11"/>
       <c r="O15" s="11"/>
       <c r="P15" s="11"/>
@@ -2498,6 +2570,10 @@
       <c r="E16" s="11"/>
       <c r="F16" s="11"/>
       <c r="G16" s="11"/>
+      <c r="H16" s="11" t="str">
+        <f>"`cases`.`"&amp;Πίνακας3[[#This Row],[Πεδίο]]&amp;"` AS `"&amp;Πίνακας3[[#This Row],[Πεδίο]]&amp;"`,"</f>
+        <v>`cases`.`smoking` AS `smoking`,</v>
+      </c>
       <c r="I16" s="11"/>
       <c r="O16" s="11"/>
       <c r="P16" s="11"/>
@@ -2523,6 +2599,10 @@
       <c r="E17" s="11"/>
       <c r="F17" s="11"/>
       <c r="G17" s="11"/>
+      <c r="H17" s="11" t="str">
+        <f>"`cases`.`"&amp;Πίνακας3[[#This Row],[Πεδίο]]&amp;"` AS `"&amp;Πίνακας3[[#This Row],[Πεδίο]]&amp;"`,"</f>
+        <v>`cases`.`druglipids` AS `druglipids`,</v>
+      </c>
       <c r="I17" s="11"/>
       <c r="O17" s="11"/>
       <c r="P17" s="11"/>
@@ -2548,6 +2628,10 @@
       <c r="E18" s="11"/>
       <c r="F18" s="11"/>
       <c r="G18" s="11"/>
+      <c r="H18" s="11" t="str">
+        <f>"`cases`.`"&amp;Πίνακας3[[#This Row],[Πεδίο]]&amp;"` AS `"&amp;Πίνακας3[[#This Row],[Πεδίο]]&amp;"`,"</f>
+        <v>`cases`.`triglycerides` AS `triglycerides`,</v>
+      </c>
       <c r="I18" s="11"/>
       <c r="O18" s="11"/>
       <c r="P18" s="11"/>
@@ -2573,6 +2657,10 @@
       <c r="E19" s="11"/>
       <c r="F19" s="11"/>
       <c r="G19" s="11"/>
+      <c r="H19" s="11" t="str">
+        <f>"`cases`.`"&amp;Πίνακας3[[#This Row],[Πεδίο]]&amp;"` AS `"&amp;Πίνακας3[[#This Row],[Πεδίο]]&amp;"`,"</f>
+        <v>`cases`.`cholesterol` AS `cholesterol`,</v>
+      </c>
       <c r="I19" s="11"/>
       <c r="O19" s="11"/>
       <c r="P19" s="11"/>
@@ -2598,6 +2686,10 @@
       <c r="E20" s="11"/>
       <c r="F20" s="11"/>
       <c r="G20" s="11"/>
+      <c r="H20" s="11" t="str">
+        <f>"`cases`.`"&amp;Πίνακας3[[#This Row],[Πεδίο]]&amp;"` AS `"&amp;Πίνακας3[[#This Row],[Πεδίο]]&amp;"`,"</f>
+        <v>`cases`.`ldl` AS `ldl`,</v>
+      </c>
       <c r="I20" s="11"/>
       <c r="O20" s="11"/>
       <c r="P20" s="11"/>
@@ -2623,6 +2715,10 @@
       <c r="E21" s="11"/>
       <c r="F21" s="11"/>
       <c r="G21" s="11"/>
+      <c r="H21" s="11" t="str">
+        <f>"`cases`.`"&amp;Πίνακας3[[#This Row],[Πεδίο]]&amp;"` AS `"&amp;Πίνακας3[[#This Row],[Πεδίο]]&amp;"`,"</f>
+        <v>`cases`.`hdl` AS `hdl`,</v>
+      </c>
       <c r="I21" s="11"/>
       <c r="O21" s="11"/>
       <c r="P21" s="11"/>
@@ -2648,6 +2744,10 @@
       <c r="E22" s="11"/>
       <c r="F22" s="11"/>
       <c r="G22" s="11"/>
+      <c r="H22" s="11" t="str">
+        <f>"`cases`.`"&amp;Πίνακας3[[#This Row],[Πεδίο]]&amp;"` AS `"&amp;Πίνακας3[[#This Row],[Πεδίο]]&amp;"`,"</f>
+        <v>`cases`.`bmi` AS `bmi`,</v>
+      </c>
       <c r="I22" s="11"/>
       <c r="O22" s="11"/>
       <c r="P22" s="11"/>
@@ -2673,6 +2773,10 @@
       <c r="E23" s="11"/>
       <c r="F23" s="11"/>
       <c r="G23" s="11"/>
+      <c r="H23" s="11" t="str">
+        <f>"`cases`.`"&amp;Πίνακας3[[#This Row],[Πεδίο]]&amp;"` AS `"&amp;Πίνακας3[[#This Row],[Πεδίο]]&amp;"`,"</f>
+        <v>`cases`.`crp` AS `crp`,</v>
+      </c>
       <c r="I23" s="11"/>
       <c r="O23" s="11"/>
       <c r="P23" s="11"/>
@@ -2698,6 +2802,10 @@
       <c r="E24" s="11"/>
       <c r="F24" s="11"/>
       <c r="G24" s="11"/>
+      <c r="H24" s="11" t="str">
+        <f>"`cases`.`"&amp;Πίνακας3[[#This Row],[Πεδίο]]&amp;"` AS `"&amp;Πίνακας3[[#This Row],[Πεδίο]]&amp;"`,"</f>
+        <v>`cases`.`wbc` AS `wbc`,</v>
+      </c>
       <c r="I24" s="11"/>
       <c r="O24" s="11"/>
       <c r="P24" s="11"/>
@@ -2723,6 +2831,10 @@
       <c r="E25" s="11"/>
       <c r="F25" s="11"/>
       <c r="G25" s="11"/>
+      <c r="H25" s="11" t="str">
+        <f>"`cases`.`"&amp;Πίνακας3[[#This Row],[Πεδίο]]&amp;"` AS `"&amp;Πίνακας3[[#This Row],[Πεδίο]]&amp;"`,"</f>
+        <v>`cases`.`imt` AS `imt`,</v>
+      </c>
       <c r="I25" s="11"/>
       <c r="O25" s="11"/>
       <c r="P25" s="11"/>
@@ -2748,6 +2860,10 @@
       <c r="E26" s="11"/>
       <c r="F26" s="11"/>
       <c r="G26" s="11"/>
+      <c r="H26" s="11" t="str">
+        <f>"`cases`.`"&amp;Πίνακας3[[#This Row],[Πεδίο]]&amp;"` AS `"&amp;Πίνακας3[[#This Row],[Πεδίο]]&amp;"`,"</f>
+        <v>`cases`.`ef` AS `ef`,</v>
+      </c>
       <c r="I26" s="11"/>
       <c r="O26" s="11"/>
       <c r="P26" s="11"/>
@@ -2773,6 +2889,10 @@
       <c r="E27" s="11"/>
       <c r="F27" s="11"/>
       <c r="G27" s="11"/>
+      <c r="H27" s="11" t="str">
+        <f>"`cases`.`"&amp;Πίνακας3[[#This Row],[Πεδίο]]&amp;"` AS `"&amp;Πίνακας3[[#This Row],[Πεδίο]]&amp;"`,"</f>
+        <v>`cases`.`calciumscore` AS `calciumscore`,</v>
+      </c>
       <c r="I27" s="11"/>
       <c r="O27" s="11"/>
       <c r="P27" s="11"/>
@@ -2798,6 +2918,10 @@
       <c r="E28" s="11"/>
       <c r="F28" s="11"/>
       <c r="G28" s="11"/>
+      <c r="H28" s="11" t="str">
+        <f>"`cases`.`"&amp;Πίνακας3[[#This Row],[Πεδίο]]&amp;"` AS `"&amp;Πίνακας3[[#This Row],[Πεδίο]]&amp;"`,"</f>
+        <v>`cases`.`lpa` AS `lpa`,</v>
+      </c>
       <c r="I28" s="11"/>
       <c r="O28" s="11"/>
       <c r="P28" s="11"/>
@@ -2823,6 +2947,10 @@
       <c r="E29" s="11"/>
       <c r="F29" s="11"/>
       <c r="G29" s="11"/>
+      <c r="H29" s="11" t="str">
+        <f>"`cases`.`"&amp;Πίνακας3[[#This Row],[Πεδίο]]&amp;"` AS `"&amp;Πίνακας3[[#This Row],[Πεδίο]]&amp;"`,"</f>
+        <v>`cases`.`creatinine` AS `creatinine`,</v>
+      </c>
       <c r="I29" s="11"/>
       <c r="O29" s="11"/>
       <c r="P29" s="11"/>
@@ -2848,6 +2976,10 @@
       <c r="E30" s="11"/>
       <c r="F30" s="11"/>
       <c r="G30" s="11"/>
+      <c r="H30" s="11" t="str">
+        <f>"`cases`.`"&amp;Πίνακας3[[#This Row],[Πεδίο]]&amp;"` AS `"&amp;Πίνακας3[[#This Row],[Πεδίο]]&amp;"`,"</f>
+        <v>`cases`.`artialfibrillation` AS `artialfibrillation`,</v>
+      </c>
       <c r="I30" s="11"/>
       <c r="O30" s="11"/>
       <c r="P30" s="11"/>
@@ -2873,6 +3005,10 @@
       <c r="E31" s="11"/>
       <c r="F31" s="11"/>
       <c r="G31" s="11"/>
+      <c r="H31" s="11" t="str">
+        <f>"`cases`.`"&amp;Πίνακας3[[#This Row],[Πεδίο]]&amp;"` AS `"&amp;Πίνακας3[[#This Row],[Πεδίο]]&amp;"`,"</f>
+        <v>`cases`.`heartfailure` AS `heartfailure`,</v>
+      </c>
       <c r="I31" s="11"/>
       <c r="O31" s="11"/>
       <c r="P31" s="11"/>
@@ -2898,6 +3034,10 @@
       <c r="E32" s="11"/>
       <c r="F32" s="11"/>
       <c r="G32" s="11"/>
+      <c r="H32" s="11" t="str">
+        <f>"`cases`.`"&amp;Πίνακας3[[#This Row],[Πεδίο]]&amp;"` AS `"&amp;Πίνακας3[[#This Row],[Πεδίο]]&amp;"`,"</f>
+        <v>`cases`.`cvd` AS `cvd`,</v>
+      </c>
       <c r="I32" s="11"/>
       <c r="O32" s="11"/>
       <c r="P32" s="11"/>
@@ -2923,6 +3063,10 @@
       <c r="E33" s="11"/>
       <c r="F33" s="11"/>
       <c r="G33" s="11"/>
+      <c r="H33" s="11" t="str">
+        <f>"`cases`.`"&amp;Πίνακας3[[#This Row],[Πεδίο]]&amp;"` AS `"&amp;Πίνακας3[[#This Row],[Πεδίο]]&amp;"`,"</f>
+        <v>`cases`.`yrcvd` AS `yrcvd`,</v>
+      </c>
       <c r="I33" s="11"/>
       <c r="O33" s="11"/>
       <c r="P33" s="11"/>
@@ -2948,6 +3092,10 @@
       <c r="E34" s="11"/>
       <c r="F34" s="11"/>
       <c r="G34" s="11"/>
+      <c r="H34" s="11" t="str">
+        <f>"`cases`.`"&amp;Πίνακας3[[#This Row],[Πεδίο]]&amp;"` AS `"&amp;Πίνακας3[[#This Row],[Πεδίο]]&amp;"`,"</f>
+        <v>`cases`.`deathcvd` AS `deathcvd`,</v>
+      </c>
       <c r="I34" s="11"/>
       <c r="O34" s="11"/>
       <c r="P34" s="11"/>
@@ -2973,6 +3121,10 @@
       <c r="E35" s="11"/>
       <c r="F35" s="11"/>
       <c r="G35" s="11"/>
+      <c r="H35" s="11" t="str">
+        <f>"`cases`.`"&amp;Πίνακας3[[#This Row],[Πεδίο]]&amp;"` AS `"&amp;Πίνακας3[[#This Row],[Πεδίο]]&amp;"`,"</f>
+        <v>`cases`.`yrcvddeath` AS `yrcvddeath`,</v>
+      </c>
       <c r="I35" s="11"/>
       <c r="O35" s="11"/>
       <c r="P35" s="11"/>
@@ -2998,6 +3150,10 @@
       <c r="E36" s="11"/>
       <c r="F36" s="11"/>
       <c r="G36" s="11"/>
+      <c r="H36" s="11" t="str">
+        <f>"`cases`.`"&amp;Πίνακας3[[#This Row],[Πεδίο]]&amp;"` AS `"&amp;Πίνακας3[[#This Row],[Πεδίο]]&amp;"`,"</f>
+        <v>`cases`.`familyhistory` AS `familyhistory`,</v>
+      </c>
       <c r="I36" s="11"/>
       <c r="O36" s="11"/>
       <c r="P36" s="11"/>
@@ -3023,6 +3179,10 @@
       <c r="E37" s="11"/>
       <c r="F37" s="11"/>
       <c r="G37" s="11"/>
+      <c r="H37" s="11" t="str">
+        <f>"`cases`.`"&amp;Πίνακας3[[#This Row],[Πεδίο]]&amp;"` AS `"&amp;Πίνακας3[[#This Row],[Πεδίο]]&amp;"`,"</f>
+        <v>`cases`.`cancer` AS `cancer`,</v>
+      </c>
       <c r="I37" s="11"/>
       <c r="O37" s="11"/>
       <c r="P37" s="11"/>
@@ -3048,6 +3208,10 @@
       <c r="E38" s="11"/>
       <c r="F38" s="11"/>
       <c r="G38" s="11"/>
+      <c r="H38" s="11" t="str">
+        <f>"`cases`.`"&amp;Πίνακας3[[#This Row],[Πεδίο]]&amp;"` AS `"&amp;Πίνακας3[[#This Row],[Πεδίο]]&amp;"`,"</f>
+        <v>`cases`.`yrcancer` AS `yrcancer`,</v>
+      </c>
       <c r="I38" s="11"/>
       <c r="O38" s="11"/>
       <c r="P38" s="11"/>
@@ -3073,6 +3237,10 @@
       <c r="E39" s="11"/>
       <c r="F39" s="11"/>
       <c r="G39" s="11"/>
+      <c r="H39" s="11" t="str">
+        <f>"`cases`.`"&amp;Πίνακας3[[#This Row],[Πεδίο]]&amp;"` AS `"&amp;Πίνακας3[[#This Row],[Πεδίο]]&amp;"`,"</f>
+        <v>`cases`.`comments` AS `comments`,</v>
+      </c>
       <c r="I39" s="11"/>
       <c r="O39" s="11"/>
       <c r="P39" s="11"/>
@@ -3098,6 +3266,10 @@
       <c r="E40" s="11"/>
       <c r="F40" s="11"/>
       <c r="G40" s="11"/>
+      <c r="H40" s="11" t="str">
+        <f>"`cases`.`"&amp;Πίνακας3[[#This Row],[Πεδίο]]&amp;"` AS `"&amp;Πίνακας3[[#This Row],[Πεδίο]]&amp;"`,"</f>
+        <v>`cases`.`createdAt` AS `createdAt`,</v>
+      </c>
       <c r="I40" s="11"/>
       <c r="O40" s="11"/>
       <c r="P40" s="11"/>
@@ -3123,6 +3295,10 @@
       <c r="E41" s="11"/>
       <c r="F41" s="11"/>
       <c r="G41" s="11"/>
+      <c r="H41" s="11" t="str">
+        <f>"`cases`.`"&amp;Πίνακας3[[#This Row],[Πεδίο]]&amp;"` AS `"&amp;Πίνακας3[[#This Row],[Πεδίο]]&amp;"`,"</f>
+        <v>`cases`.`updatedAt` AS `updatedAt`,</v>
+      </c>
       <c r="I41" s="11"/>
       <c r="O41" s="11"/>
       <c r="P41" s="11"/>
@@ -3150,6 +3326,10 @@
       </c>
       <c r="F42" s="11"/>
       <c r="G42" s="11"/>
+      <c r="H42" s="11" t="str">
+        <f>"`cases`.`"&amp;Πίνακας3[[#This Row],[Πεδίο]]&amp;"` AS `"&amp;Πίνακας3[[#This Row],[Πεδίο]]&amp;"`,"</f>
+        <v>`cases`.`author` AS `author`,</v>
+      </c>
       <c r="I42" s="11"/>
       <c r="O42" s="11"/>
       <c r="P42" s="11"/>

</xml_diff>

<commit_message>
0.81 - fields correction
</commit_message>
<xml_diff>
--- a/Docs/ΕΥΚΑΡΔΙΑ Πεδία Βάσης Δεδομένων.xlsx
+++ b/Docs/ΕΥΚΑΡΔΙΑ Πεδία Βάσης Δεδομένων.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Development\Eukardia\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4207EED7-8749-4426-82D8-7DC791F4DFE9}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{316A7888-4239-43FB-BBC9-838182C06A55}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11625" tabRatio="481" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="354" uniqueCount="159">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="354" uniqueCount="158">
   <si>
     <t>Όνομα πεδίου</t>
   </si>
@@ -441,9 +441,6 @@
   </si>
   <si>
     <t>dbp</t>
-  </si>
-  <si>
-    <t>diebetes</t>
   </si>
   <si>
     <t>druglipids</t>
@@ -591,7 +588,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -626,11 +623,20 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="8"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -655,6 +661,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Κανονικό" xfId="0" builtinId="0"/>
@@ -1287,7 +1294,7 @@
   <dimension ref="A1:G46"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2035,10 +2042,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{13E70851-83B8-43A0-B14E-A8B2D42B9ED9}">
-  <dimension ref="A1:T42"/>
+  <dimension ref="A1:T52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="H7" sqref="H7:H41"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="25.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2055,34 +2062,34 @@
   <sheetData>
     <row r="1" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>145</v>
+      </c>
+      <c r="B1" t="s">
         <v>146</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>147</v>
-      </c>
-      <c r="C1" t="s">
-        <v>148</v>
       </c>
       <c r="D1" t="s">
         <v>3</v>
       </c>
       <c r="E1" t="s">
+        <v>148</v>
+      </c>
+      <c r="F1" t="s">
         <v>149</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>150</v>
       </c>
-      <c r="G1" t="s">
-        <v>151</v>
-      </c>
       <c r="H1" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="K1" s="12" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="L1" s="12" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="O1" s="11"/>
       <c r="P1" s="11"/>
@@ -2121,7 +2128,7 @@
         <v>123</v>
       </c>
       <c r="L2" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="O2" s="11"/>
       <c r="P2" s="11"/>
@@ -2230,7 +2237,7 @@
         <v>131</v>
       </c>
       <c r="L5" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="O5" s="11"/>
       <c r="P5" s="11"/>
@@ -2265,7 +2272,7 @@
         <v>135</v>
       </c>
       <c r="L6" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="O6" s="11"/>
       <c r="P6" s="11"/>
@@ -2297,10 +2304,10 @@
       </c>
       <c r="I7" s="11"/>
       <c r="K7" s="13" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="L7" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="O7" s="11"/>
       <c r="P7" s="11"/>
@@ -2332,10 +2339,10 @@
       </c>
       <c r="I8" s="11"/>
       <c r="K8" s="13" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="L8" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="O8" s="11"/>
       <c r="P8" s="11"/>
@@ -2367,10 +2374,10 @@
       </c>
       <c r="I9" s="11"/>
       <c r="K9" s="13" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="L9" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="O9" s="11"/>
       <c r="P9" s="11"/>
@@ -2439,7 +2446,7 @@
     </row>
     <row r="12" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A12" s="11" t="s">
-        <v>137</v>
+        <v>83</v>
       </c>
       <c r="B12" s="11" t="str">
         <f>VLOOKUP(Πίνακας3[[#This Row],[Τύπος SQL]],types,2,FALSE)</f>
@@ -2456,7 +2463,7 @@
       <c r="G12" s="11"/>
       <c r="H12" s="11" t="str">
         <f>"`cases`.`"&amp;Πίνακας3[[#This Row],[Πεδίο]]&amp;"` AS `"&amp;Πίνακας3[[#This Row],[Πεδίο]]&amp;"`,"</f>
-        <v>`cases`.`diebetes` AS `diebetes`,</v>
+        <v>`cases`.`diabetes` AS `diabetes`,</v>
       </c>
       <c r="I12" s="11"/>
       <c r="O12" s="11"/>
@@ -2584,7 +2591,7 @@
     </row>
     <row r="17" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A17" s="11" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B17" s="11" t="str">
         <f>VLOOKUP(Πίνακας3[[#This Row],[Τύπος SQL]],types,2,FALSE)</f>
@@ -2959,9 +2966,9 @@
       <c r="S29" s="11"/>
       <c r="T29" s="11"/>
     </row>
-    <row r="30" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:20" ht="30" x14ac:dyDescent="0.25">
       <c r="A30" s="11" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B30" s="11" t="str">
         <f>VLOOKUP(Πίνακας3[[#This Row],[Τύπος SQL]],types,2,FALSE)</f>
@@ -3019,7 +3026,7 @@
     </row>
     <row r="32" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A32" s="11" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B32" s="11" t="str">
         <f>VLOOKUP(Πίνακας3[[#This Row],[Τύπος SQL]],types,2,FALSE)</f>
@@ -3048,14 +3055,14 @@
     </row>
     <row r="33" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A33" s="11" t="s">
+        <v>140</v>
+      </c>
+      <c r="B33" s="11" t="str">
+        <f>VLOOKUP(Πίνακας3[[#This Row],[Τύπος SQL]],types,2,FALSE)</f>
+        <v>Ακέραιος μέχρι 65535</v>
+      </c>
+      <c r="C33" s="11" t="s">
         <v>141</v>
-      </c>
-      <c r="B33" s="11" t="str">
-        <f>VLOOKUP(Πίνακας3[[#This Row],[Τύπος SQL]],types,2,FALSE)</f>
-        <v>Ακέραιος μέχρι 65535</v>
-      </c>
-      <c r="C33" s="11" t="s">
-        <v>142</v>
       </c>
       <c r="D33" s="11" t="s">
         <v>132</v>
@@ -3113,7 +3120,7 @@
         <v>Ακέραιος μέχρι 65535</v>
       </c>
       <c r="C35" s="11" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="D35" s="11" t="s">
         <v>132</v>
@@ -3200,7 +3207,7 @@
         <v>Ακέραιος μέχρι 65535</v>
       </c>
       <c r="C38" s="11" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="D38" s="11" t="s">
         <v>132</v>
@@ -3222,14 +3229,14 @@
     </row>
     <row r="39" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A39" s="11" t="s">
+        <v>142</v>
+      </c>
+      <c r="B39" s="11" t="str">
+        <f>VLOOKUP(Πίνακας3[[#This Row],[Τύπος SQL]],types,2,FALSE)</f>
+        <v>Μεγάλο κείμενο</v>
+      </c>
+      <c r="C39" s="11" t="s">
         <v>143</v>
-      </c>
-      <c r="B39" s="11" t="str">
-        <f>VLOOKUP(Πίνακας3[[#This Row],[Τύπος SQL]],types,2,FALSE)</f>
-        <v>Μεγάλο κείμενο</v>
-      </c>
-      <c r="C39" s="11" t="s">
-        <v>144</v>
       </c>
       <c r="D39" s="11" t="s">
         <v>132</v>
@@ -3258,7 +3265,7 @@
         <v>Ημερομηνία και Ώρα</v>
       </c>
       <c r="C40" s="11" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="D40" s="11" t="s">
         <v>124</v>
@@ -3287,7 +3294,7 @@
         <v>Ημερομηνία και Ώρα</v>
       </c>
       <c r="C41" s="11" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="D41" s="11" t="s">
         <v>124</v>
@@ -3337,6 +3344,9 @@
       <c r="R42" s="11"/>
       <c r="S42" s="11"/>
       <c r="T42" s="11"/>
+    </row>
+    <row r="52" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B52" s="14"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
0.83 - fields correction
</commit_message>
<xml_diff>
--- a/Docs/ΕΥΚΑΡΔΙΑ Πεδία Βάσης Δεδομένων.xlsx
+++ b/Docs/ΕΥΚΑΡΔΙΑ Πεδία Βάσης Δεδομένων.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Development\Eukardia\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{316A7888-4239-43FB-BBC9-838182C06A55}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22189EC9-685F-423C-82A1-46B659A96DBE}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11625" tabRatio="481" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="354" uniqueCount="158">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="354" uniqueCount="157">
   <si>
     <t>Όνομα πεδίου</t>
   </si>
@@ -444,9 +444,6 @@
   </si>
   <si>
     <t>druglipids</t>
-  </si>
-  <si>
-    <t>artialfibrillation</t>
   </si>
   <si>
     <t>cvd</t>
@@ -510,7 +507,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -566,6 +563,13 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFCE9178"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+      <charset val="161"/>
     </font>
   </fonts>
   <fills count="4">
@@ -636,7 +640,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -662,6 +666,9 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Κανονικό" xfId="0" builtinId="0"/>
@@ -1294,7 +1301,7 @@
   <dimension ref="A1:G46"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+      <selection activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2044,8 +2051,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{13E70851-83B8-43A0-B14E-A8B2D42B9ED9}">
   <dimension ref="A1:T52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="A50" sqref="A50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="25.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2062,34 +2069,34 @@
   <sheetData>
     <row r="1" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>144</v>
+      </c>
+      <c r="B1" t="s">
         <v>145</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>146</v>
-      </c>
-      <c r="C1" t="s">
-        <v>147</v>
       </c>
       <c r="D1" t="s">
         <v>3</v>
       </c>
       <c r="E1" t="s">
+        <v>147</v>
+      </c>
+      <c r="F1" t="s">
         <v>148</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>149</v>
       </c>
-      <c r="G1" t="s">
-        <v>150</v>
-      </c>
       <c r="H1" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="K1" s="12" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="L1" s="12" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="O1" s="11"/>
       <c r="P1" s="11"/>
@@ -2128,7 +2135,7 @@
         <v>123</v>
       </c>
       <c r="L2" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="O2" s="11"/>
       <c r="P2" s="11"/>
@@ -2237,7 +2244,7 @@
         <v>131</v>
       </c>
       <c r="L5" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="O5" s="11"/>
       <c r="P5" s="11"/>
@@ -2272,7 +2279,7 @@
         <v>135</v>
       </c>
       <c r="L6" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="O6" s="11"/>
       <c r="P6" s="11"/>
@@ -2304,10 +2311,10 @@
       </c>
       <c r="I7" s="11"/>
       <c r="K7" s="13" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="L7" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="O7" s="11"/>
       <c r="P7" s="11"/>
@@ -2339,10 +2346,10 @@
       </c>
       <c r="I8" s="11"/>
       <c r="K8" s="13" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="L8" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="O8" s="11"/>
       <c r="P8" s="11"/>
@@ -2374,10 +2381,10 @@
       </c>
       <c r="I9" s="11"/>
       <c r="K9" s="13" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="L9" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="O9" s="11"/>
       <c r="P9" s="11"/>
@@ -2968,7 +2975,7 @@
     </row>
     <row r="30" spans="1:20" ht="30" x14ac:dyDescent="0.25">
       <c r="A30" s="11" t="s">
-        <v>138</v>
+        <v>85</v>
       </c>
       <c r="B30" s="11" t="str">
         <f>VLOOKUP(Πίνακας3[[#This Row],[Τύπος SQL]],types,2,FALSE)</f>
@@ -2985,7 +2992,7 @@
       <c r="G30" s="11"/>
       <c r="H30" s="11" t="str">
         <f>"`cases`.`"&amp;Πίνακας3[[#This Row],[Πεδίο]]&amp;"` AS `"&amp;Πίνακας3[[#This Row],[Πεδίο]]&amp;"`,"</f>
-        <v>`cases`.`artialfibrillation` AS `artialfibrillation`,</v>
+        <v>`cases`.`atrialfibrillation` AS `atrialfibrillation`,</v>
       </c>
       <c r="I30" s="11"/>
       <c r="O30" s="11"/>
@@ -3026,7 +3033,7 @@
     </row>
     <row r="32" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A32" s="11" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B32" s="11" t="str">
         <f>VLOOKUP(Πίνακας3[[#This Row],[Τύπος SQL]],types,2,FALSE)</f>
@@ -3055,14 +3062,14 @@
     </row>
     <row r="33" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A33" s="11" t="s">
+        <v>139</v>
+      </c>
+      <c r="B33" s="11" t="str">
+        <f>VLOOKUP(Πίνακας3[[#This Row],[Τύπος SQL]],types,2,FALSE)</f>
+        <v>Ακέραιος μέχρι 65535</v>
+      </c>
+      <c r="C33" s="11" t="s">
         <v>140</v>
-      </c>
-      <c r="B33" s="11" t="str">
-        <f>VLOOKUP(Πίνακας3[[#This Row],[Τύπος SQL]],types,2,FALSE)</f>
-        <v>Ακέραιος μέχρι 65535</v>
-      </c>
-      <c r="C33" s="11" t="s">
-        <v>141</v>
       </c>
       <c r="D33" s="11" t="s">
         <v>132</v>
@@ -3120,7 +3127,7 @@
         <v>Ακέραιος μέχρι 65535</v>
       </c>
       <c r="C35" s="11" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D35" s="11" t="s">
         <v>132</v>
@@ -3207,7 +3214,7 @@
         <v>Ακέραιος μέχρι 65535</v>
       </c>
       <c r="C38" s="11" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D38" s="11" t="s">
         <v>132</v>
@@ -3229,14 +3236,14 @@
     </row>
     <row r="39" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A39" s="11" t="s">
+        <v>141</v>
+      </c>
+      <c r="B39" s="11" t="str">
+        <f>VLOOKUP(Πίνακας3[[#This Row],[Τύπος SQL]],types,2,FALSE)</f>
+        <v>Μεγάλο κείμενο</v>
+      </c>
+      <c r="C39" s="11" t="s">
         <v>142</v>
-      </c>
-      <c r="B39" s="11" t="str">
-        <f>VLOOKUP(Πίνακας3[[#This Row],[Τύπος SQL]],types,2,FALSE)</f>
-        <v>Μεγάλο κείμενο</v>
-      </c>
-      <c r="C39" s="11" t="s">
-        <v>143</v>
       </c>
       <c r="D39" s="11" t="s">
         <v>132</v>
@@ -3265,7 +3272,7 @@
         <v>Ημερομηνία και Ώρα</v>
       </c>
       <c r="C40" s="11" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="D40" s="11" t="s">
         <v>124</v>
@@ -3294,7 +3301,7 @@
         <v>Ημερομηνία και Ώρα</v>
       </c>
       <c r="C41" s="11" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="D41" s="11" t="s">
         <v>124</v>
@@ -3344,6 +3351,12 @@
       <c r="R42" s="11"/>
       <c r="S42" s="11"/>
       <c r="T42" s="11"/>
+    </row>
+    <row r="50" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B50" s="14"/>
+    </row>
+    <row r="51" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B51" s="15"/>
     </row>
     <row r="52" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B52" s="14"/>

</xml_diff>

<commit_message>
0..91 - test sequelize config
</commit_message>
<xml_diff>
--- a/Docs/ΕΥΚΑΡΔΙΑ Πεδία Βάσης Δεδομένων.xlsx
+++ b/Docs/ΕΥΚΑΡΔΙΑ Πεδία Βάσης Δεδομένων.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Development\Eukardia\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22189EC9-685F-423C-82A1-46B659A96DBE}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E714EDF-A7C3-42B3-93AE-B38F17E81AE7}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11625" tabRatio="481" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2051,8 +2051,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{13E70851-83B8-43A0-B14E-A8B2D42B9ED9}">
   <dimension ref="A1:T52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="A50" sqref="A50"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="25.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
0.18.3. - vercel redeploy
</commit_message>
<xml_diff>
--- a/Docs/ΕΥΚΑΡΔΙΑ Πεδία Βάσης Δεδομένων.xlsx
+++ b/Docs/ΕΥΚΑΡΔΙΑ Πεδία Βάσης Δεδομένων.xlsx
@@ -8,17 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Development\Eukardia\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E714EDF-A7C3-42B3-93AE-B38F17E81AE7}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34582209-90B0-4A04-B843-107CE28D85B5}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11625" tabRatio="481" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Πεδία" sheetId="1" r:id="rId1"/>
-    <sheet name="dim" sheetId="2" r:id="rId2"/>
+    <sheet name="sql πεδία" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm.Print_Area" localSheetId="0">Πίνακας1[[#All],[Περιγραφή πεδίου]:[Επιτρεπόμενες τιμές ή εύρος τιμών]]</definedName>
-    <definedName name="types">dim!$K$1:$L$9</definedName>
+    <definedName name="types">'sql πεδία'!$K$1:$L$9</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -640,7 +640,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -648,9 +648,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -1028,7 +1025,7 @@
       <calculatedColumnFormula>"`cases`.`"&amp;Πίνακας3[[#This Row],[Πεδίο]]&amp;"` AS `"&amp;Πίνακας3[[#This Row],[Πεδίο]]&amp;"`,"</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
-  <tableStyleInfo name="TableStyleLight14" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+  <tableStyleInfo name="TableStyleLight10" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
@@ -1296,12 +1293,13 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
+    <tabColor rgb="FF00B0F0"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:G46"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C29" sqref="C29"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1319,7 +1317,7 @@
       <c r="A1" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="B1" s="9" t="s">
+      <c r="B1" s="8" t="s">
         <v>51</v>
       </c>
       <c r="C1" s="1" t="s">
@@ -1339,19 +1337,19 @@
       </c>
     </row>
     <row r="2" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="10" t="s">
+      <c r="A2" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="B2" s="10"/>
-      <c r="C2" s="10" t="s">
+      <c r="B2" s="9"/>
+      <c r="C2" s="9" t="s">
         <v>52</v>
       </c>
-      <c r="D2" s="10" t="s">
+      <c r="D2" s="9" t="s">
         <v>118</v>
       </c>
-      <c r="E2" s="10"/>
-      <c r="F2" s="10"/>
-      <c r="G2" s="10" t="s">
+      <c r="E2" s="9"/>
+      <c r="F2" s="9"/>
+      <c r="G2" s="9" t="s">
         <v>43</v>
       </c>
     </row>
@@ -1489,7 +1487,7 @@
       <c r="C11" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="D11" s="10" t="s">
+      <c r="D11" s="9" t="s">
         <v>118</v>
       </c>
       <c r="E11" s="3" t="s">
@@ -1532,7 +1530,7 @@
       <c r="E13" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="F13" s="5" t="s">
+      <c r="F13" s="1" t="s">
         <v>119</v>
       </c>
       <c r="G13" s="1" t="s">
@@ -1581,7 +1579,7 @@
       <c r="C16" s="3" t="s">
         <v>90</v>
       </c>
-      <c r="D16" s="10" t="s">
+      <c r="D16" s="9" t="s">
         <v>118</v>
       </c>
       <c r="E16" s="4"/>
@@ -1778,7 +1776,7 @@
       <c r="C29" s="3" t="s">
         <v>85</v>
       </c>
-      <c r="D29" s="10" t="s">
+      <c r="D29" s="9" t="s">
         <v>118</v>
       </c>
       <c r="E29" s="4" t="s">
@@ -1796,7 +1794,7 @@
       <c r="C30" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="D30" s="10" t="s">
+      <c r="D30" s="9" t="s">
         <v>118</v>
       </c>
       <c r="E30" s="4" t="s">
@@ -1814,7 +1812,7 @@
       <c r="C31" s="3" t="s">
         <v>95</v>
       </c>
-      <c r="D31" s="10" t="s">
+      <c r="D31" s="9" t="s">
         <v>118</v>
       </c>
       <c r="E31" s="4" t="s">
@@ -1847,7 +1845,7 @@
       <c r="C33" s="3" t="s">
         <v>121</v>
       </c>
-      <c r="D33" s="10" t="s">
+      <c r="D33" s="9" t="s">
         <v>118</v>
       </c>
       <c r="F33" s="3" t="s">
@@ -1877,7 +1875,7 @@
       <c r="C35" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="D35" s="10" t="s">
+      <c r="D35" s="9" t="s">
         <v>118</v>
       </c>
       <c r="E35" s="4" t="s">
@@ -1895,7 +1893,7 @@
       <c r="C36" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="D36" s="10" t="s">
+      <c r="D36" s="9" t="s">
         <v>118</v>
       </c>
       <c r="E36" s="4" t="s">
@@ -1928,25 +1926,25 @@
       </c>
     </row>
     <row r="42" spans="1:7" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="6" t="s">
+      <c r="A42" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B42" s="6" t="s">
+      <c r="B42" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="C42" s="6" t="s">
+      <c r="C42" s="5" t="s">
         <v>76</v>
       </c>
-      <c r="D42" s="7" t="s">
+      <c r="D42" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="E42" s="7" t="s">
+      <c r="E42" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="F42" s="8" t="s">
+      <c r="F42" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="G42" s="7" t="s">
+      <c r="G42" s="6" t="s">
         <v>39</v>
       </c>
     </row>
@@ -2049,11 +2047,12 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{13E70851-83B8-43A0-B14E-A8B2D42B9ED9}">
+  <sheetPr>
+    <tabColor rgb="FF7030A0"/>
+  </sheetPr>
   <dimension ref="A1:T52"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="25.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -2063,7 +2062,7 @@
     <col min="4" max="4" width="15.140625" bestFit="1" customWidth="1"/>
     <col min="5" max="6" width="9.28515625" customWidth="1"/>
     <col min="7" max="7" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="41.28515625" customWidth="1"/>
+    <col min="8" max="8" width="44.5703125" customWidth="1"/>
     <col min="12" max="12" width="33.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -2092,1274 +2091,1274 @@
       <c r="H1" t="s">
         <v>156</v>
       </c>
-      <c r="K1" s="12" t="s">
+      <c r="K1" s="11" t="s">
         <v>146</v>
       </c>
-      <c r="L1" s="12" t="s">
+      <c r="L1" s="11" t="s">
         <v>145</v>
       </c>
-      <c r="O1" s="11"/>
-      <c r="P1" s="11"/>
-      <c r="Q1" s="11"/>
-      <c r="R1" s="11"/>
-      <c r="S1" s="11"/>
-      <c r="T1" s="11"/>
+      <c r="O1" s="10"/>
+      <c r="P1" s="10"/>
+      <c r="Q1" s="10"/>
+      <c r="R1" s="10"/>
+      <c r="S1" s="10"/>
+      <c r="T1" s="10"/>
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A2" s="11" t="s">
+      <c r="A2" s="10" t="s">
         <v>72</v>
       </c>
-      <c r="B2" s="11" t="str">
+      <c r="B2" s="10" t="str">
         <f>VLOOKUP(Πίνακας3[[#This Row],[Τύπος SQL]],types,2,FALSE)</f>
         <v>Ακέραιος μέχρι 2147483647</v>
       </c>
-      <c r="C2" s="11" t="s">
+      <c r="C2" s="10" t="s">
         <v>123</v>
       </c>
-      <c r="D2" s="11" t="s">
+      <c r="D2" s="10" t="s">
         <v>124</v>
       </c>
-      <c r="E2" s="11" t="s">
+      <c r="E2" s="10" t="s">
         <v>125</v>
       </c>
-      <c r="F2" s="11"/>
-      <c r="G2" s="11" t="s">
+      <c r="F2" s="10"/>
+      <c r="G2" s="10" t="s">
         <v>126</v>
       </c>
-      <c r="H2" s="11" t="str">
+      <c r="H2" s="10" t="str">
         <f>"`cases`.`"&amp;Πίνακας3[[#This Row],[Πεδίο]]&amp;"` AS `"&amp;Πίνακας3[[#This Row],[Πεδίο]]&amp;"`,"</f>
         <v>`cases`.`id` AS `id`,</v>
       </c>
-      <c r="I2" s="11"/>
-      <c r="K2" s="13" t="s">
+      <c r="I2" s="10"/>
+      <c r="K2" s="12" t="s">
         <v>123</v>
       </c>
       <c r="L2" t="s">
         <v>154</v>
       </c>
-      <c r="O2" s="11"/>
-      <c r="P2" s="11"/>
-      <c r="Q2" s="11"/>
-      <c r="R2" s="11"/>
-      <c r="S2" s="11"/>
-      <c r="T2" s="11"/>
+      <c r="O2" s="10"/>
+      <c r="P2" s="10"/>
+      <c r="Q2" s="10"/>
+      <c r="R2" s="10"/>
+      <c r="S2" s="10"/>
+      <c r="T2" s="10"/>
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A3" s="11" t="s">
+      <c r="A3" s="10" t="s">
         <v>52</v>
       </c>
-      <c r="B3" s="11" t="str">
+      <c r="B3" s="10" t="str">
         <f>VLOOKUP(Πίνακας3[[#This Row],[Τύπος SQL]],types,2,FALSE)</f>
         <v>Ναι/Όχι</v>
       </c>
-      <c r="C3" s="11" t="s">
+      <c r="C3" s="10" t="s">
         <v>127</v>
       </c>
-      <c r="D3" s="11" t="s">
+      <c r="D3" s="10" t="s">
         <v>124</v>
       </c>
-      <c r="E3" s="11"/>
-      <c r="F3" s="11">
+      <c r="E3" s="10"/>
+      <c r="F3" s="10">
         <v>0</v>
       </c>
-      <c r="G3" s="11"/>
-      <c r="H3" s="11" t="str">
+      <c r="G3" s="10"/>
+      <c r="H3" s="10" t="str">
         <f>"`cases`.`"&amp;Πίνακας3[[#This Row],[Πεδίο]]&amp;"` AS `"&amp;Πίνακας3[[#This Row],[Πεδίο]]&amp;"`,"</f>
         <v>`cases`.`testPatient` AS `testPatient`,</v>
       </c>
-      <c r="I3" s="11"/>
-      <c r="K3" s="13" t="s">
+      <c r="I3" s="10"/>
+      <c r="K3" s="12" t="s">
         <v>127</v>
       </c>
       <c r="L3" t="s">
         <v>118</v>
       </c>
-      <c r="O3" s="11"/>
-      <c r="P3" s="11"/>
-      <c r="Q3" s="11"/>
-      <c r="R3" s="11"/>
-      <c r="S3" s="11"/>
-      <c r="T3" s="11"/>
+      <c r="O3" s="10"/>
+      <c r="P3" s="10"/>
+      <c r="Q3" s="10"/>
+      <c r="R3" s="10"/>
+      <c r="S3" s="10"/>
+      <c r="T3" s="10"/>
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A4" s="11" t="s">
+      <c r="A4" s="10" t="s">
         <v>128</v>
       </c>
-      <c r="B4" s="11" t="str">
+      <c r="B4" s="10" t="str">
         <f>VLOOKUP(Πίνακας3[[#This Row],[Τύπος SQL]],types,2,FALSE)</f>
         <v>Σύντομο κείμενο</v>
       </c>
-      <c r="C4" s="11" t="s">
+      <c r="C4" s="10" t="s">
         <v>129</v>
       </c>
-      <c r="D4" s="11" t="s">
+      <c r="D4" s="10" t="s">
         <v>124</v>
       </c>
-      <c r="E4" s="11" t="s">
+      <c r="E4" s="10" t="s">
         <v>130</v>
       </c>
-      <c r="F4" s="11"/>
-      <c r="G4" s="11"/>
-      <c r="H4" s="11" t="str">
+      <c r="F4" s="10"/>
+      <c r="G4" s="10"/>
+      <c r="H4" s="10" t="str">
         <f>"`cases`.`"&amp;Πίνακας3[[#This Row],[Πεδίο]]&amp;"` AS `"&amp;Πίνακας3[[#This Row],[Πεδίο]]&amp;"`,"</f>
         <v>`cases`.`patientId` AS `patientId`,</v>
       </c>
-      <c r="I4" s="11"/>
-      <c r="K4" s="13" t="s">
+      <c r="I4" s="10"/>
+      <c r="K4" s="12" t="s">
         <v>129</v>
       </c>
       <c r="L4" t="s">
         <v>35</v>
       </c>
-      <c r="O4" s="11"/>
-      <c r="P4" s="11"/>
-      <c r="Q4" s="11"/>
-      <c r="R4" s="11"/>
-      <c r="S4" s="11"/>
-      <c r="T4" s="11"/>
+      <c r="O4" s="10"/>
+      <c r="P4" s="10"/>
+      <c r="Q4" s="10"/>
+      <c r="R4" s="10"/>
+      <c r="S4" s="10"/>
+      <c r="T4" s="10"/>
     </row>
     <row r="5" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A5" s="11" t="s">
+      <c r="A5" s="10" t="s">
         <v>54</v>
       </c>
-      <c r="B5" s="11" t="str">
+      <c r="B5" s="10" t="str">
         <f>VLOOKUP(Πίνακας3[[#This Row],[Τύπος SQL]],types,2,FALSE)</f>
         <v xml:space="preserve">Ακέραιος ή λίστα μέχρι 127 </v>
       </c>
-      <c r="C5" s="11" t="s">
+      <c r="C5" s="10" t="s">
         <v>131</v>
       </c>
-      <c r="D5" s="11" t="s">
-        <v>132</v>
-      </c>
-      <c r="E5" s="11"/>
-      <c r="F5" s="11"/>
-      <c r="G5" s="11"/>
-      <c r="H5" s="11" t="str">
+      <c r="D5" s="10" t="s">
+        <v>132</v>
+      </c>
+      <c r="E5" s="10"/>
+      <c r="F5" s="10"/>
+      <c r="G5" s="10"/>
+      <c r="H5" s="10" t="str">
         <f>"`cases`.`"&amp;Πίνακας3[[#This Row],[Πεδίο]]&amp;"` AS `"&amp;Πίνακας3[[#This Row],[Πεδίο]]&amp;"`,"</f>
         <v>`cases`.`gender` AS `gender`,</v>
       </c>
-      <c r="I5" s="11"/>
-      <c r="K5" s="13" t="s">
+      <c r="I5" s="10"/>
+      <c r="K5" s="12" t="s">
         <v>131</v>
       </c>
       <c r="L5" t="s">
         <v>155</v>
       </c>
-      <c r="O5" s="11"/>
-      <c r="P5" s="11"/>
-      <c r="Q5" s="11"/>
-      <c r="R5" s="11"/>
-      <c r="S5" s="11"/>
-      <c r="T5" s="11"/>
+      <c r="O5" s="10"/>
+      <c r="P5" s="10"/>
+      <c r="Q5" s="10"/>
+      <c r="R5" s="10"/>
+      <c r="S5" s="10"/>
+      <c r="T5" s="10"/>
     </row>
     <row r="6" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A6" s="11" t="s">
+      <c r="A6" s="10" t="s">
         <v>55</v>
       </c>
-      <c r="B6" s="11" t="str">
+      <c r="B6" s="10" t="str">
         <f>VLOOKUP(Πίνακας3[[#This Row],[Τύπος SQL]],types,2,FALSE)</f>
         <v xml:space="preserve">Ακέραιος ή λίστα μέχρι 127 </v>
       </c>
-      <c r="C6" s="11" t="s">
+      <c r="C6" s="10" t="s">
         <v>131</v>
       </c>
-      <c r="D6" s="11" t="s">
-        <v>132</v>
-      </c>
-      <c r="E6" s="11"/>
-      <c r="F6" s="11"/>
-      <c r="G6" s="11"/>
-      <c r="H6" s="11" t="str">
+      <c r="D6" s="10" t="s">
+        <v>132</v>
+      </c>
+      <c r="E6" s="10"/>
+      <c r="F6" s="10"/>
+      <c r="G6" s="10"/>
+      <c r="H6" s="10" t="str">
         <f>"`cases`.`"&amp;Πίνακας3[[#This Row],[Πεδίο]]&amp;"` AS `"&amp;Πίνακας3[[#This Row],[Πεδίο]]&amp;"`,"</f>
         <v>`cases`.`age` AS `age`,</v>
       </c>
-      <c r="I6" s="11"/>
-      <c r="K6" s="13" t="s">
+      <c r="I6" s="10"/>
+      <c r="K6" s="12" t="s">
         <v>135</v>
       </c>
       <c r="L6" t="s">
         <v>152</v>
       </c>
-      <c r="O6" s="11"/>
-      <c r="P6" s="11"/>
-      <c r="Q6" s="11"/>
-      <c r="R6" s="11"/>
-      <c r="S6" s="11"/>
-      <c r="T6" s="11"/>
+      <c r="O6" s="10"/>
+      <c r="P6" s="10"/>
+      <c r="Q6" s="10"/>
+      <c r="R6" s="10"/>
+      <c r="S6" s="10"/>
+      <c r="T6" s="10"/>
     </row>
     <row r="7" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A7" s="11" t="s">
+      <c r="A7" s="10" t="s">
         <v>133</v>
       </c>
-      <c r="B7" s="11" t="str">
+      <c r="B7" s="10" t="str">
         <f>VLOOKUP(Πίνακας3[[#This Row],[Τύπος SQL]],types,2,FALSE)</f>
         <v>Ναι/Όχι</v>
       </c>
-      <c r="C7" s="11" t="s">
+      <c r="C7" s="10" t="s">
         <v>127</v>
       </c>
-      <c r="D7" s="11" t="s">
-        <v>132</v>
-      </c>
-      <c r="E7" s="11"/>
-      <c r="F7" s="11"/>
-      <c r="G7" s="11"/>
-      <c r="H7" s="11" t="str">
+      <c r="D7" s="10" t="s">
+        <v>132</v>
+      </c>
+      <c r="E7" s="10"/>
+      <c r="F7" s="10"/>
+      <c r="G7" s="10"/>
+      <c r="H7" s="10" t="str">
         <f>"`cases`.`"&amp;Πίνακας3[[#This Row],[Πεδίο]]&amp;"` AS `"&amp;Πίνακας3[[#This Row],[Πεδίο]]&amp;"`,"</f>
         <v>`cases`.`drugbp` AS `drugbp`,</v>
       </c>
-      <c r="I7" s="11"/>
-      <c r="K7" s="13" t="s">
+      <c r="I7" s="10"/>
+      <c r="K7" s="12" t="s">
         <v>140</v>
       </c>
       <c r="L7" t="s">
         <v>153</v>
       </c>
-      <c r="O7" s="11"/>
-      <c r="P7" s="11"/>
-      <c r="Q7" s="11"/>
-      <c r="R7" s="11"/>
-      <c r="S7" s="11"/>
-      <c r="T7" s="11"/>
+      <c r="O7" s="10"/>
+      <c r="P7" s="10"/>
+      <c r="Q7" s="10"/>
+      <c r="R7" s="10"/>
+      <c r="S7" s="10"/>
+      <c r="T7" s="10"/>
     </row>
     <row r="8" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A8" s="11" t="s">
+      <c r="A8" s="10" t="s">
         <v>134</v>
       </c>
-      <c r="B8" s="11" t="str">
+      <c r="B8" s="10" t="str">
         <f>VLOOKUP(Πίνακας3[[#This Row],[Τύπος SQL]],types,2,FALSE)</f>
         <v>Δεκαδικός αριθμός</v>
       </c>
-      <c r="C8" s="11" t="s">
+      <c r="C8" s="10" t="s">
         <v>135</v>
       </c>
-      <c r="D8" s="11" t="s">
-        <v>132</v>
-      </c>
-      <c r="E8" s="11"/>
-      <c r="F8" s="11"/>
-      <c r="G8" s="11"/>
-      <c r="H8" s="11" t="str">
+      <c r="D8" s="10" t="s">
+        <v>132</v>
+      </c>
+      <c r="E8" s="10"/>
+      <c r="F8" s="10"/>
+      <c r="G8" s="10"/>
+      <c r="H8" s="10" t="str">
         <f>"`cases`.`"&amp;Πίνακας3[[#This Row],[Πεδίο]]&amp;"` AS `"&amp;Πίνακας3[[#This Row],[Πεδίο]]&amp;"`,"</f>
         <v>`cases`.`sbp` AS `sbp`,</v>
       </c>
-      <c r="I8" s="11"/>
-      <c r="K8" s="13" t="s">
+      <c r="I8" s="10"/>
+      <c r="K8" s="12" t="s">
         <v>142</v>
       </c>
       <c r="L8" t="s">
         <v>150</v>
       </c>
-      <c r="O8" s="11"/>
-      <c r="P8" s="11"/>
-      <c r="Q8" s="11"/>
-      <c r="R8" s="11"/>
-      <c r="S8" s="11"/>
-      <c r="T8" s="11"/>
+      <c r="O8" s="10"/>
+      <c r="P8" s="10"/>
+      <c r="Q8" s="10"/>
+      <c r="R8" s="10"/>
+      <c r="S8" s="10"/>
+      <c r="T8" s="10"/>
     </row>
     <row r="9" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A9" s="11" t="s">
+      <c r="A9" s="10" t="s">
         <v>136</v>
       </c>
-      <c r="B9" s="11" t="str">
+      <c r="B9" s="10" t="str">
         <f>VLOOKUP(Πίνακας3[[#This Row],[Τύπος SQL]],types,2,FALSE)</f>
         <v>Δεκαδικός αριθμός</v>
       </c>
-      <c r="C9" s="11" t="s">
+      <c r="C9" s="10" t="s">
         <v>135</v>
       </c>
-      <c r="D9" s="11" t="s">
-        <v>132</v>
-      </c>
-      <c r="E9" s="11"/>
-      <c r="F9" s="11"/>
-      <c r="G9" s="11"/>
-      <c r="H9" s="11" t="str">
+      <c r="D9" s="10" t="s">
+        <v>132</v>
+      </c>
+      <c r="E9" s="10"/>
+      <c r="F9" s="10"/>
+      <c r="G9" s="10"/>
+      <c r="H9" s="10" t="str">
         <f>"`cases`.`"&amp;Πίνακας3[[#This Row],[Πεδίο]]&amp;"` AS `"&amp;Πίνακας3[[#This Row],[Πεδίο]]&amp;"`,"</f>
         <v>`cases`.`dbp` AS `dbp`,</v>
       </c>
-      <c r="I9" s="11"/>
-      <c r="K9" s="13" t="s">
+      <c r="I9" s="10"/>
+      <c r="K9" s="12" t="s">
         <v>143</v>
       </c>
       <c r="L9" t="s">
         <v>151</v>
       </c>
-      <c r="O9" s="11"/>
-      <c r="P9" s="11"/>
-      <c r="Q9" s="11"/>
-      <c r="R9" s="11"/>
-      <c r="S9" s="11"/>
-      <c r="T9" s="11"/>
+      <c r="O9" s="10"/>
+      <c r="P9" s="10"/>
+      <c r="Q9" s="10"/>
+      <c r="R9" s="10"/>
+      <c r="S9" s="10"/>
+      <c r="T9" s="10"/>
     </row>
     <row r="10" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A10" s="11" t="s">
+      <c r="A10" s="10" t="s">
         <v>56</v>
       </c>
-      <c r="B10" s="11" t="str">
+      <c r="B10" s="10" t="str">
         <f>VLOOKUP(Πίνακας3[[#This Row],[Τύπος SQL]],types,2,FALSE)</f>
         <v>Δεκαδικός αριθμός</v>
       </c>
-      <c r="C10" s="11" t="s">
+      <c r="C10" s="10" t="s">
         <v>135</v>
       </c>
-      <c r="D10" s="11" t="s">
-        <v>132</v>
-      </c>
-      <c r="E10" s="11"/>
-      <c r="F10" s="11"/>
-      <c r="G10" s="11"/>
-      <c r="H10" s="11" t="str">
+      <c r="D10" s="10" t="s">
+        <v>132</v>
+      </c>
+      <c r="E10" s="10"/>
+      <c r="F10" s="10"/>
+      <c r="G10" s="10"/>
+      <c r="H10" s="10" t="str">
         <f>"`cases`.`"&amp;Πίνακας3[[#This Row],[Πεδίο]]&amp;"` AS `"&amp;Πίνακας3[[#This Row],[Πεδίο]]&amp;"`,"</f>
         <v>`cases`.`glucose` AS `glucose`,</v>
       </c>
-      <c r="I10" s="11"/>
-      <c r="O10" s="11"/>
-      <c r="P10" s="11"/>
-      <c r="Q10" s="11"/>
-      <c r="R10" s="11"/>
-      <c r="S10" s="11"/>
-      <c r="T10" s="11"/>
+      <c r="I10" s="10"/>
+      <c r="O10" s="10"/>
+      <c r="P10" s="10"/>
+      <c r="Q10" s="10"/>
+      <c r="R10" s="10"/>
+      <c r="S10" s="10"/>
+      <c r="T10" s="10"/>
     </row>
     <row r="11" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A11" s="11" t="s">
+      <c r="A11" s="10" t="s">
         <v>68</v>
       </c>
-      <c r="B11" s="11" t="str">
+      <c r="B11" s="10" t="str">
         <f>VLOOKUP(Πίνακας3[[#This Row],[Τύπος SQL]],types,2,FALSE)</f>
         <v>Δεκαδικός αριθμός</v>
       </c>
-      <c r="C11" s="11" t="s">
+      <c r="C11" s="10" t="s">
         <v>135</v>
       </c>
-      <c r="D11" s="11" t="s">
-        <v>132</v>
-      </c>
-      <c r="E11" s="11"/>
-      <c r="F11" s="11"/>
-      <c r="G11" s="11"/>
-      <c r="H11" s="11" t="str">
+      <c r="D11" s="10" t="s">
+        <v>132</v>
+      </c>
+      <c r="E11" s="10"/>
+      <c r="F11" s="10"/>
+      <c r="G11" s="10"/>
+      <c r="H11" s="10" t="str">
         <f>"`cases`.`"&amp;Πίνακας3[[#This Row],[Πεδίο]]&amp;"` AS `"&amp;Πίνακας3[[#This Row],[Πεδίο]]&amp;"`,"</f>
         <v>`cases`.`hba1c` AS `hba1c`,</v>
       </c>
-      <c r="I11" s="11"/>
-      <c r="O11" s="11"/>
-      <c r="P11" s="11"/>
-      <c r="Q11" s="11"/>
-      <c r="R11" s="11"/>
-      <c r="S11" s="11"/>
-      <c r="T11" s="11"/>
+      <c r="I11" s="10"/>
+      <c r="O11" s="10"/>
+      <c r="P11" s="10"/>
+      <c r="Q11" s="10"/>
+      <c r="R11" s="10"/>
+      <c r="S11" s="10"/>
+      <c r="T11" s="10"/>
     </row>
     <row r="12" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A12" s="11" t="s">
+      <c r="A12" s="10" t="s">
         <v>83</v>
       </c>
-      <c r="B12" s="11" t="str">
+      <c r="B12" s="10" t="str">
         <f>VLOOKUP(Πίνακας3[[#This Row],[Τύπος SQL]],types,2,FALSE)</f>
         <v>Ναι/Όχι</v>
       </c>
-      <c r="C12" s="11" t="s">
+      <c r="C12" s="10" t="s">
         <v>127</v>
       </c>
-      <c r="D12" s="11" t="s">
-        <v>132</v>
-      </c>
-      <c r="E12" s="11"/>
-      <c r="F12" s="11"/>
-      <c r="G12" s="11"/>
-      <c r="H12" s="11" t="str">
+      <c r="D12" s="10" t="s">
+        <v>132</v>
+      </c>
+      <c r="E12" s="10"/>
+      <c r="F12" s="10"/>
+      <c r="G12" s="10"/>
+      <c r="H12" s="10" t="str">
         <f>"`cases`.`"&amp;Πίνακας3[[#This Row],[Πεδίο]]&amp;"` AS `"&amp;Πίνακας3[[#This Row],[Πεδίο]]&amp;"`,"</f>
         <v>`cases`.`diabetes` AS `diabetes`,</v>
       </c>
-      <c r="I12" s="11"/>
-      <c r="O12" s="11"/>
-      <c r="P12" s="11"/>
-      <c r="Q12" s="11"/>
-      <c r="R12" s="11"/>
-      <c r="S12" s="11"/>
-      <c r="T12" s="11"/>
+      <c r="I12" s="10"/>
+      <c r="O12" s="10"/>
+      <c r="P12" s="10"/>
+      <c r="Q12" s="10"/>
+      <c r="R12" s="10"/>
+      <c r="S12" s="10"/>
+      <c r="T12" s="10"/>
     </row>
     <row r="13" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A13" s="11" t="s">
+      <c r="A13" s="10" t="s">
         <v>58</v>
       </c>
-      <c r="B13" s="11" t="str">
+      <c r="B13" s="10" t="str">
         <f>VLOOKUP(Πίνακας3[[#This Row],[Τύπος SQL]],types,2,FALSE)</f>
         <v xml:space="preserve">Ακέραιος ή λίστα μέχρι 127 </v>
       </c>
-      <c r="C13" s="11" t="s">
+      <c r="C13" s="10" t="s">
         <v>131</v>
       </c>
-      <c r="D13" s="11" t="s">
-        <v>132</v>
-      </c>
-      <c r="E13" s="11"/>
-      <c r="F13" s="11"/>
-      <c r="G13" s="11"/>
-      <c r="H13" s="11" t="str">
+      <c r="D13" s="10" t="s">
+        <v>132</v>
+      </c>
+      <c r="E13" s="10"/>
+      <c r="F13" s="10"/>
+      <c r="G13" s="10"/>
+      <c r="H13" s="10" t="str">
         <f>"`cases`.`"&amp;Πίνακας3[[#This Row],[Πεδίο]]&amp;"` AS `"&amp;Πίνακας3[[#This Row],[Πεδίο]]&amp;"`,"</f>
         <v>`cases`.`activity` AS `activity`,</v>
       </c>
-      <c r="I13" s="11"/>
-      <c r="O13" s="11"/>
-      <c r="P13" s="11"/>
-      <c r="Q13" s="11"/>
-      <c r="R13" s="11"/>
-      <c r="S13" s="11"/>
-      <c r="T13" s="11"/>
+      <c r="I13" s="10"/>
+      <c r="O13" s="10"/>
+      <c r="P13" s="10"/>
+      <c r="Q13" s="10"/>
+      <c r="R13" s="10"/>
+      <c r="S13" s="10"/>
+      <c r="T13" s="10"/>
     </row>
     <row r="14" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A14" s="11" t="s">
+      <c r="A14" s="10" t="s">
         <v>59</v>
       </c>
-      <c r="B14" s="11" t="str">
+      <c r="B14" s="10" t="str">
         <f>VLOOKUP(Πίνακας3[[#This Row],[Τύπος SQL]],types,2,FALSE)</f>
         <v xml:space="preserve">Ακέραιος ή λίστα μέχρι 127 </v>
       </c>
-      <c r="C14" s="11" t="s">
+      <c r="C14" s="10" t="s">
         <v>131</v>
       </c>
-      <c r="D14" s="11" t="s">
-        <v>132</v>
-      </c>
-      <c r="E14" s="11"/>
-      <c r="F14" s="11"/>
-      <c r="G14" s="11"/>
-      <c r="H14" s="11" t="str">
+      <c r="D14" s="10" t="s">
+        <v>132</v>
+      </c>
+      <c r="E14" s="10"/>
+      <c r="F14" s="10"/>
+      <c r="G14" s="10"/>
+      <c r="H14" s="10" t="str">
         <f>"`cases`.`"&amp;Πίνακας3[[#This Row],[Πεδίο]]&amp;"` AS `"&amp;Πίνακας3[[#This Row],[Πεδίο]]&amp;"`,"</f>
         <v>`cases`.`diet` AS `diet`,</v>
       </c>
-      <c r="I14" s="11"/>
-      <c r="O14" s="11"/>
-      <c r="P14" s="11"/>
-      <c r="Q14" s="11"/>
-      <c r="R14" s="11"/>
-      <c r="S14" s="11"/>
-      <c r="T14" s="11"/>
+      <c r="I14" s="10"/>
+      <c r="O14" s="10"/>
+      <c r="P14" s="10"/>
+      <c r="Q14" s="10"/>
+      <c r="R14" s="10"/>
+      <c r="S14" s="10"/>
+      <c r="T14" s="10"/>
     </row>
     <row r="15" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A15" s="11" t="s">
+      <c r="A15" s="10" t="s">
         <v>109</v>
       </c>
-      <c r="B15" s="11" t="str">
+      <c r="B15" s="10" t="str">
         <f>VLOOKUP(Πίνακας3[[#This Row],[Τύπος SQL]],types,2,FALSE)</f>
         <v xml:space="preserve">Ακέραιος ή λίστα μέχρι 127 </v>
       </c>
-      <c r="C15" s="11" t="s">
+      <c r="C15" s="10" t="s">
         <v>131</v>
       </c>
-      <c r="D15" s="11" t="s">
-        <v>132</v>
-      </c>
-      <c r="E15" s="11"/>
-      <c r="F15" s="11"/>
-      <c r="G15" s="11"/>
-      <c r="H15" s="11" t="str">
+      <c r="D15" s="10" t="s">
+        <v>132</v>
+      </c>
+      <c r="E15" s="10"/>
+      <c r="F15" s="10"/>
+      <c r="G15" s="10"/>
+      <c r="H15" s="10" t="str">
         <f>"`cases`.`"&amp;Πίνακας3[[#This Row],[Πεδίο]]&amp;"` AS `"&amp;Πίνακας3[[#This Row],[Πεδίο]]&amp;"`,"</f>
         <v>`cases`.`alcohol` AS `alcohol`,</v>
       </c>
-      <c r="I15" s="11"/>
-      <c r="O15" s="11"/>
-      <c r="P15" s="11"/>
-      <c r="Q15" s="11"/>
-      <c r="R15" s="11"/>
-      <c r="S15" s="11"/>
-      <c r="T15" s="11"/>
+      <c r="I15" s="10"/>
+      <c r="O15" s="10"/>
+      <c r="P15" s="10"/>
+      <c r="Q15" s="10"/>
+      <c r="R15" s="10"/>
+      <c r="S15" s="10"/>
+      <c r="T15" s="10"/>
     </row>
     <row r="16" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A16" s="11" t="s">
+      <c r="A16" s="10" t="s">
         <v>60</v>
       </c>
-      <c r="B16" s="11" t="str">
+      <c r="B16" s="10" t="str">
         <f>VLOOKUP(Πίνακας3[[#This Row],[Τύπος SQL]],types,2,FALSE)</f>
         <v xml:space="preserve">Ακέραιος ή λίστα μέχρι 127 </v>
       </c>
-      <c r="C16" s="11" t="s">
+      <c r="C16" s="10" t="s">
         <v>131</v>
       </c>
-      <c r="D16" s="11" t="s">
-        <v>132</v>
-      </c>
-      <c r="E16" s="11"/>
-      <c r="F16" s="11"/>
-      <c r="G16" s="11"/>
-      <c r="H16" s="11" t="str">
+      <c r="D16" s="10" t="s">
+        <v>132</v>
+      </c>
+      <c r="E16" s="10"/>
+      <c r="F16" s="10"/>
+      <c r="G16" s="10"/>
+      <c r="H16" s="10" t="str">
         <f>"`cases`.`"&amp;Πίνακας3[[#This Row],[Πεδίο]]&amp;"` AS `"&amp;Πίνακας3[[#This Row],[Πεδίο]]&amp;"`,"</f>
         <v>`cases`.`smoking` AS `smoking`,</v>
       </c>
-      <c r="I16" s="11"/>
-      <c r="O16" s="11"/>
-      <c r="P16" s="11"/>
-      <c r="Q16" s="11"/>
-      <c r="R16" s="11"/>
-      <c r="S16" s="11"/>
-      <c r="T16" s="11"/>
+      <c r="I16" s="10"/>
+      <c r="O16" s="10"/>
+      <c r="P16" s="10"/>
+      <c r="Q16" s="10"/>
+      <c r="R16" s="10"/>
+      <c r="S16" s="10"/>
+      <c r="T16" s="10"/>
     </row>
     <row r="17" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A17" s="11" t="s">
+      <c r="A17" s="10" t="s">
         <v>137</v>
       </c>
-      <c r="B17" s="11" t="str">
+      <c r="B17" s="10" t="str">
         <f>VLOOKUP(Πίνακας3[[#This Row],[Τύπος SQL]],types,2,FALSE)</f>
         <v>Ναι/Όχι</v>
       </c>
-      <c r="C17" s="11" t="s">
+      <c r="C17" s="10" t="s">
         <v>127</v>
       </c>
-      <c r="D17" s="11" t="s">
-        <v>132</v>
-      </c>
-      <c r="E17" s="11"/>
-      <c r="F17" s="11"/>
-      <c r="G17" s="11"/>
-      <c r="H17" s="11" t="str">
+      <c r="D17" s="10" t="s">
+        <v>132</v>
+      </c>
+      <c r="E17" s="10"/>
+      <c r="F17" s="10"/>
+      <c r="G17" s="10"/>
+      <c r="H17" s="10" t="str">
         <f>"`cases`.`"&amp;Πίνακας3[[#This Row],[Πεδίο]]&amp;"` AS `"&amp;Πίνακας3[[#This Row],[Πεδίο]]&amp;"`,"</f>
         <v>`cases`.`druglipids` AS `druglipids`,</v>
       </c>
-      <c r="I17" s="11"/>
-      <c r="O17" s="11"/>
-      <c r="P17" s="11"/>
-      <c r="Q17" s="11"/>
-      <c r="R17" s="11"/>
-      <c r="S17" s="11"/>
-      <c r="T17" s="11"/>
+      <c r="I17" s="10"/>
+      <c r="O17" s="10"/>
+      <c r="P17" s="10"/>
+      <c r="Q17" s="10"/>
+      <c r="R17" s="10"/>
+      <c r="S17" s="10"/>
+      <c r="T17" s="10"/>
     </row>
     <row r="18" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A18" s="11" t="s">
+      <c r="A18" s="10" t="s">
         <v>84</v>
       </c>
-      <c r="B18" s="11" t="str">
+      <c r="B18" s="10" t="str">
         <f>VLOOKUP(Πίνακας3[[#This Row],[Τύπος SQL]],types,2,FALSE)</f>
         <v>Δεκαδικός αριθμός</v>
       </c>
-      <c r="C18" s="11" t="s">
+      <c r="C18" s="10" t="s">
         <v>135</v>
       </c>
-      <c r="D18" s="11" t="s">
-        <v>132</v>
-      </c>
-      <c r="E18" s="11"/>
-      <c r="F18" s="11"/>
-      <c r="G18" s="11"/>
-      <c r="H18" s="11" t="str">
+      <c r="D18" s="10" t="s">
+        <v>132</v>
+      </c>
+      <c r="E18" s="10"/>
+      <c r="F18" s="10"/>
+      <c r="G18" s="10"/>
+      <c r="H18" s="10" t="str">
         <f>"`cases`.`"&amp;Πίνακας3[[#This Row],[Πεδίο]]&amp;"` AS `"&amp;Πίνακας3[[#This Row],[Πεδίο]]&amp;"`,"</f>
         <v>`cases`.`triglycerides` AS `triglycerides`,</v>
       </c>
-      <c r="I18" s="11"/>
-      <c r="O18" s="11"/>
-      <c r="P18" s="11"/>
-      <c r="Q18" s="11"/>
-      <c r="R18" s="11"/>
-      <c r="S18" s="11"/>
-      <c r="T18" s="11"/>
+      <c r="I18" s="10"/>
+      <c r="O18" s="10"/>
+      <c r="P18" s="10"/>
+      <c r="Q18" s="10"/>
+      <c r="R18" s="10"/>
+      <c r="S18" s="10"/>
+      <c r="T18" s="10"/>
     </row>
     <row r="19" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A19" s="11" t="s">
+      <c r="A19" s="10" t="s">
         <v>61</v>
       </c>
-      <c r="B19" s="11" t="str">
+      <c r="B19" s="10" t="str">
         <f>VLOOKUP(Πίνακας3[[#This Row],[Τύπος SQL]],types,2,FALSE)</f>
         <v>Δεκαδικός αριθμός</v>
       </c>
-      <c r="C19" s="11" t="s">
+      <c r="C19" s="10" t="s">
         <v>135</v>
       </c>
-      <c r="D19" s="11" t="s">
-        <v>132</v>
-      </c>
-      <c r="E19" s="11"/>
-      <c r="F19" s="11"/>
-      <c r="G19" s="11"/>
-      <c r="H19" s="11" t="str">
+      <c r="D19" s="10" t="s">
+        <v>132</v>
+      </c>
+      <c r="E19" s="10"/>
+      <c r="F19" s="10"/>
+      <c r="G19" s="10"/>
+      <c r="H19" s="10" t="str">
         <f>"`cases`.`"&amp;Πίνακας3[[#This Row],[Πεδίο]]&amp;"` AS `"&amp;Πίνακας3[[#This Row],[Πεδίο]]&amp;"`,"</f>
         <v>`cases`.`cholesterol` AS `cholesterol`,</v>
       </c>
-      <c r="I19" s="11"/>
-      <c r="O19" s="11"/>
-      <c r="P19" s="11"/>
-      <c r="Q19" s="11"/>
-      <c r="R19" s="11"/>
-      <c r="S19" s="11"/>
-      <c r="T19" s="11"/>
+      <c r="I19" s="10"/>
+      <c r="O19" s="10"/>
+      <c r="P19" s="10"/>
+      <c r="Q19" s="10"/>
+      <c r="R19" s="10"/>
+      <c r="S19" s="10"/>
+      <c r="T19" s="10"/>
     </row>
     <row r="20" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A20" s="11" t="s">
+      <c r="A20" s="10" t="s">
         <v>66</v>
       </c>
-      <c r="B20" s="11" t="str">
+      <c r="B20" s="10" t="str">
         <f>VLOOKUP(Πίνακας3[[#This Row],[Τύπος SQL]],types,2,FALSE)</f>
         <v>Δεκαδικός αριθμός</v>
       </c>
-      <c r="C20" s="11" t="s">
+      <c r="C20" s="10" t="s">
         <v>135</v>
       </c>
-      <c r="D20" s="11" t="s">
-        <v>132</v>
-      </c>
-      <c r="E20" s="11"/>
-      <c r="F20" s="11"/>
-      <c r="G20" s="11"/>
-      <c r="H20" s="11" t="str">
+      <c r="D20" s="10" t="s">
+        <v>132</v>
+      </c>
+      <c r="E20" s="10"/>
+      <c r="F20" s="10"/>
+      <c r="G20" s="10"/>
+      <c r="H20" s="10" t="str">
         <f>"`cases`.`"&amp;Πίνακας3[[#This Row],[Πεδίο]]&amp;"` AS `"&amp;Πίνακας3[[#This Row],[Πεδίο]]&amp;"`,"</f>
         <v>`cases`.`ldl` AS `ldl`,</v>
       </c>
-      <c r="I20" s="11"/>
-      <c r="O20" s="11"/>
-      <c r="P20" s="11"/>
-      <c r="Q20" s="11"/>
-      <c r="R20" s="11"/>
-      <c r="S20" s="11"/>
-      <c r="T20" s="11"/>
+      <c r="I20" s="10"/>
+      <c r="O20" s="10"/>
+      <c r="P20" s="10"/>
+      <c r="Q20" s="10"/>
+      <c r="R20" s="10"/>
+      <c r="S20" s="10"/>
+      <c r="T20" s="10"/>
     </row>
     <row r="21" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A21" s="11" t="s">
+      <c r="A21" s="10" t="s">
         <v>67</v>
       </c>
-      <c r="B21" s="11" t="str">
+      <c r="B21" s="10" t="str">
         <f>VLOOKUP(Πίνακας3[[#This Row],[Τύπος SQL]],types,2,FALSE)</f>
         <v>Δεκαδικός αριθμός</v>
       </c>
-      <c r="C21" s="11" t="s">
+      <c r="C21" s="10" t="s">
         <v>135</v>
       </c>
-      <c r="D21" s="11" t="s">
-        <v>132</v>
-      </c>
-      <c r="E21" s="11"/>
-      <c r="F21" s="11"/>
-      <c r="G21" s="11"/>
-      <c r="H21" s="11" t="str">
+      <c r="D21" s="10" t="s">
+        <v>132</v>
+      </c>
+      <c r="E21" s="10"/>
+      <c r="F21" s="10"/>
+      <c r="G21" s="10"/>
+      <c r="H21" s="10" t="str">
         <f>"`cases`.`"&amp;Πίνακας3[[#This Row],[Πεδίο]]&amp;"` AS `"&amp;Πίνακας3[[#This Row],[Πεδίο]]&amp;"`,"</f>
         <v>`cases`.`hdl` AS `hdl`,</v>
       </c>
-      <c r="I21" s="11"/>
-      <c r="O21" s="11"/>
-      <c r="P21" s="11"/>
-      <c r="Q21" s="11"/>
-      <c r="R21" s="11"/>
-      <c r="S21" s="11"/>
-      <c r="T21" s="11"/>
+      <c r="I21" s="10"/>
+      <c r="O21" s="10"/>
+      <c r="P21" s="10"/>
+      <c r="Q21" s="10"/>
+      <c r="R21" s="10"/>
+      <c r="S21" s="10"/>
+      <c r="T21" s="10"/>
     </row>
     <row r="22" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A22" s="11" t="s">
+      <c r="A22" s="10" t="s">
         <v>62</v>
       </c>
-      <c r="B22" s="11" t="str">
+      <c r="B22" s="10" t="str">
         <f>VLOOKUP(Πίνακας3[[#This Row],[Τύπος SQL]],types,2,FALSE)</f>
         <v>Δεκαδικός αριθμός</v>
       </c>
-      <c r="C22" s="11" t="s">
+      <c r="C22" s="10" t="s">
         <v>135</v>
       </c>
-      <c r="D22" s="11" t="s">
-        <v>132</v>
-      </c>
-      <c r="E22" s="11"/>
-      <c r="F22" s="11"/>
-      <c r="G22" s="11"/>
-      <c r="H22" s="11" t="str">
+      <c r="D22" s="10" t="s">
+        <v>132</v>
+      </c>
+      <c r="E22" s="10"/>
+      <c r="F22" s="10"/>
+      <c r="G22" s="10"/>
+      <c r="H22" s="10" t="str">
         <f>"`cases`.`"&amp;Πίνακας3[[#This Row],[Πεδίο]]&amp;"` AS `"&amp;Πίνακας3[[#This Row],[Πεδίο]]&amp;"`,"</f>
         <v>`cases`.`bmi` AS `bmi`,</v>
       </c>
-      <c r="I22" s="11"/>
-      <c r="O22" s="11"/>
-      <c r="P22" s="11"/>
-      <c r="Q22" s="11"/>
-      <c r="R22" s="11"/>
-      <c r="S22" s="11"/>
-      <c r="T22" s="11"/>
+      <c r="I22" s="10"/>
+      <c r="O22" s="10"/>
+      <c r="P22" s="10"/>
+      <c r="Q22" s="10"/>
+      <c r="R22" s="10"/>
+      <c r="S22" s="10"/>
+      <c r="T22" s="10"/>
     </row>
     <row r="23" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A23" s="11" t="s">
+      <c r="A23" s="10" t="s">
         <v>63</v>
       </c>
-      <c r="B23" s="11" t="str">
+      <c r="B23" s="10" t="str">
         <f>VLOOKUP(Πίνακας3[[#This Row],[Τύπος SQL]],types,2,FALSE)</f>
         <v>Δεκαδικός αριθμός</v>
       </c>
-      <c r="C23" s="11" t="s">
+      <c r="C23" s="10" t="s">
         <v>135</v>
       </c>
-      <c r="D23" s="11" t="s">
-        <v>132</v>
-      </c>
-      <c r="E23" s="11"/>
-      <c r="F23" s="11"/>
-      <c r="G23" s="11"/>
-      <c r="H23" s="11" t="str">
+      <c r="D23" s="10" t="s">
+        <v>132</v>
+      </c>
+      <c r="E23" s="10"/>
+      <c r="F23" s="10"/>
+      <c r="G23" s="10"/>
+      <c r="H23" s="10" t="str">
         <f>"`cases`.`"&amp;Πίνακας3[[#This Row],[Πεδίο]]&amp;"` AS `"&amp;Πίνακας3[[#This Row],[Πεδίο]]&amp;"`,"</f>
         <v>`cases`.`crp` AS `crp`,</v>
       </c>
-      <c r="I23" s="11"/>
-      <c r="O23" s="11"/>
-      <c r="P23" s="11"/>
-      <c r="Q23" s="11"/>
-      <c r="R23" s="11"/>
-      <c r="S23" s="11"/>
-      <c r="T23" s="11"/>
+      <c r="I23" s="10"/>
+      <c r="O23" s="10"/>
+      <c r="P23" s="10"/>
+      <c r="Q23" s="10"/>
+      <c r="R23" s="10"/>
+      <c r="S23" s="10"/>
+      <c r="T23" s="10"/>
     </row>
     <row r="24" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A24" s="11" t="s">
+      <c r="A24" s="10" t="s">
         <v>77</v>
       </c>
-      <c r="B24" s="11" t="str">
+      <c r="B24" s="10" t="str">
         <f>VLOOKUP(Πίνακας3[[#This Row],[Τύπος SQL]],types,2,FALSE)</f>
         <v>Δεκαδικός αριθμός</v>
       </c>
-      <c r="C24" s="11" t="s">
+      <c r="C24" s="10" t="s">
         <v>135</v>
       </c>
-      <c r="D24" s="11" t="s">
-        <v>132</v>
-      </c>
-      <c r="E24" s="11"/>
-      <c r="F24" s="11"/>
-      <c r="G24" s="11"/>
-      <c r="H24" s="11" t="str">
+      <c r="D24" s="10" t="s">
+        <v>132</v>
+      </c>
+      <c r="E24" s="10"/>
+      <c r="F24" s="10"/>
+      <c r="G24" s="10"/>
+      <c r="H24" s="10" t="str">
         <f>"`cases`.`"&amp;Πίνακας3[[#This Row],[Πεδίο]]&amp;"` AS `"&amp;Πίνακας3[[#This Row],[Πεδίο]]&amp;"`,"</f>
         <v>`cases`.`wbc` AS `wbc`,</v>
       </c>
-      <c r="I24" s="11"/>
-      <c r="O24" s="11"/>
-      <c r="P24" s="11"/>
-      <c r="Q24" s="11"/>
-      <c r="R24" s="11"/>
-      <c r="S24" s="11"/>
-      <c r="T24" s="11"/>
+      <c r="I24" s="10"/>
+      <c r="O24" s="10"/>
+      <c r="P24" s="10"/>
+      <c r="Q24" s="10"/>
+      <c r="R24" s="10"/>
+      <c r="S24" s="10"/>
+      <c r="T24" s="10"/>
     </row>
     <row r="25" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A25" s="11" t="s">
+      <c r="A25" s="10" t="s">
         <v>94</v>
       </c>
-      <c r="B25" s="11" t="str">
+      <c r="B25" s="10" t="str">
         <f>VLOOKUP(Πίνακας3[[#This Row],[Τύπος SQL]],types,2,FALSE)</f>
         <v>Δεκαδικός αριθμός</v>
       </c>
-      <c r="C25" s="11" t="s">
+      <c r="C25" s="10" t="s">
         <v>135</v>
       </c>
-      <c r="D25" s="11" t="s">
-        <v>132</v>
-      </c>
-      <c r="E25" s="11"/>
-      <c r="F25" s="11"/>
-      <c r="G25" s="11"/>
-      <c r="H25" s="11" t="str">
+      <c r="D25" s="10" t="s">
+        <v>132</v>
+      </c>
+      <c r="E25" s="10"/>
+      <c r="F25" s="10"/>
+      <c r="G25" s="10"/>
+      <c r="H25" s="10" t="str">
         <f>"`cases`.`"&amp;Πίνακας3[[#This Row],[Πεδίο]]&amp;"` AS `"&amp;Πίνακας3[[#This Row],[Πεδίο]]&amp;"`,"</f>
         <v>`cases`.`imt` AS `imt`,</v>
       </c>
-      <c r="I25" s="11"/>
-      <c r="O25" s="11"/>
-      <c r="P25" s="11"/>
-      <c r="Q25" s="11"/>
-      <c r="R25" s="11"/>
-      <c r="S25" s="11"/>
-      <c r="T25" s="11"/>
+      <c r="I25" s="10"/>
+      <c r="O25" s="10"/>
+      <c r="P25" s="10"/>
+      <c r="Q25" s="10"/>
+      <c r="R25" s="10"/>
+      <c r="S25" s="10"/>
+      <c r="T25" s="10"/>
     </row>
     <row r="26" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A26" s="11" t="s">
+      <c r="A26" s="10" t="s">
         <v>64</v>
       </c>
-      <c r="B26" s="11" t="str">
+      <c r="B26" s="10" t="str">
         <f>VLOOKUP(Πίνακας3[[#This Row],[Τύπος SQL]],types,2,FALSE)</f>
         <v>Δεκαδικός αριθμός</v>
       </c>
-      <c r="C26" s="11" t="s">
+      <c r="C26" s="10" t="s">
         <v>135</v>
       </c>
-      <c r="D26" s="11" t="s">
-        <v>132</v>
-      </c>
-      <c r="E26" s="11"/>
-      <c r="F26" s="11"/>
-      <c r="G26" s="11"/>
-      <c r="H26" s="11" t="str">
+      <c r="D26" s="10" t="s">
+        <v>132</v>
+      </c>
+      <c r="E26" s="10"/>
+      <c r="F26" s="10"/>
+      <c r="G26" s="10"/>
+      <c r="H26" s="10" t="str">
         <f>"`cases`.`"&amp;Πίνακας3[[#This Row],[Πεδίο]]&amp;"` AS `"&amp;Πίνακας3[[#This Row],[Πεδίο]]&amp;"`,"</f>
         <v>`cases`.`ef` AS `ef`,</v>
       </c>
-      <c r="I26" s="11"/>
-      <c r="O26" s="11"/>
-      <c r="P26" s="11"/>
-      <c r="Q26" s="11"/>
-      <c r="R26" s="11"/>
-      <c r="S26" s="11"/>
-      <c r="T26" s="11"/>
+      <c r="I26" s="10"/>
+      <c r="O26" s="10"/>
+      <c r="P26" s="10"/>
+      <c r="Q26" s="10"/>
+      <c r="R26" s="10"/>
+      <c r="S26" s="10"/>
+      <c r="T26" s="10"/>
     </row>
     <row r="27" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A27" s="11" t="s">
+      <c r="A27" s="10" t="s">
         <v>82</v>
       </c>
-      <c r="B27" s="11" t="str">
+      <c r="B27" s="10" t="str">
         <f>VLOOKUP(Πίνακας3[[#This Row],[Τύπος SQL]],types,2,FALSE)</f>
         <v>Δεκαδικός αριθμός</v>
       </c>
-      <c r="C27" s="11" t="s">
+      <c r="C27" s="10" t="s">
         <v>135</v>
       </c>
-      <c r="D27" s="11" t="s">
-        <v>132</v>
-      </c>
-      <c r="E27" s="11"/>
-      <c r="F27" s="11"/>
-      <c r="G27" s="11"/>
-      <c r="H27" s="11" t="str">
+      <c r="D27" s="10" t="s">
+        <v>132</v>
+      </c>
+      <c r="E27" s="10"/>
+      <c r="F27" s="10"/>
+      <c r="G27" s="10"/>
+      <c r="H27" s="10" t="str">
         <f>"`cases`.`"&amp;Πίνακας3[[#This Row],[Πεδίο]]&amp;"` AS `"&amp;Πίνακας3[[#This Row],[Πεδίο]]&amp;"`,"</f>
         <v>`cases`.`calciumscore` AS `calciumscore`,</v>
       </c>
-      <c r="I27" s="11"/>
-      <c r="O27" s="11"/>
-      <c r="P27" s="11"/>
-      <c r="Q27" s="11"/>
-      <c r="R27" s="11"/>
-      <c r="S27" s="11"/>
-      <c r="T27" s="11"/>
+      <c r="I27" s="10"/>
+      <c r="O27" s="10"/>
+      <c r="P27" s="10"/>
+      <c r="Q27" s="10"/>
+      <c r="R27" s="10"/>
+      <c r="S27" s="10"/>
+      <c r="T27" s="10"/>
     </row>
     <row r="28" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A28" s="11" t="s">
+      <c r="A28" s="10" t="s">
         <v>65</v>
       </c>
-      <c r="B28" s="11" t="str">
+      <c r="B28" s="10" t="str">
         <f>VLOOKUP(Πίνακας3[[#This Row],[Τύπος SQL]],types,2,FALSE)</f>
         <v>Δεκαδικός αριθμός</v>
       </c>
-      <c r="C28" s="11" t="s">
+      <c r="C28" s="10" t="s">
         <v>135</v>
       </c>
-      <c r="D28" s="11" t="s">
-        <v>132</v>
-      </c>
-      <c r="E28" s="11"/>
-      <c r="F28" s="11"/>
-      <c r="G28" s="11"/>
-      <c r="H28" s="11" t="str">
+      <c r="D28" s="10" t="s">
+        <v>132</v>
+      </c>
+      <c r="E28" s="10"/>
+      <c r="F28" s="10"/>
+      <c r="G28" s="10"/>
+      <c r="H28" s="10" t="str">
         <f>"`cases`.`"&amp;Πίνακας3[[#This Row],[Πεδίο]]&amp;"` AS `"&amp;Πίνακας3[[#This Row],[Πεδίο]]&amp;"`,"</f>
         <v>`cases`.`lpa` AS `lpa`,</v>
       </c>
-      <c r="I28" s="11"/>
-      <c r="O28" s="11"/>
-      <c r="P28" s="11"/>
-      <c r="Q28" s="11"/>
-      <c r="R28" s="11"/>
-      <c r="S28" s="11"/>
-      <c r="T28" s="11"/>
+      <c r="I28" s="10"/>
+      <c r="O28" s="10"/>
+      <c r="P28" s="10"/>
+      <c r="Q28" s="10"/>
+      <c r="R28" s="10"/>
+      <c r="S28" s="10"/>
+      <c r="T28" s="10"/>
     </row>
     <row r="29" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A29" s="11" t="s">
+      <c r="A29" s="10" t="s">
         <v>71</v>
       </c>
-      <c r="B29" s="11" t="str">
+      <c r="B29" s="10" t="str">
         <f>VLOOKUP(Πίνακας3[[#This Row],[Τύπος SQL]],types,2,FALSE)</f>
         <v>Δεκαδικός αριθμός</v>
       </c>
-      <c r="C29" s="11" t="s">
+      <c r="C29" s="10" t="s">
         <v>135</v>
       </c>
-      <c r="D29" s="11" t="s">
-        <v>132</v>
-      </c>
-      <c r="E29" s="11"/>
-      <c r="F29" s="11"/>
-      <c r="G29" s="11"/>
-      <c r="H29" s="11" t="str">
+      <c r="D29" s="10" t="s">
+        <v>132</v>
+      </c>
+      <c r="E29" s="10"/>
+      <c r="F29" s="10"/>
+      <c r="G29" s="10"/>
+      <c r="H29" s="10" t="str">
         <f>"`cases`.`"&amp;Πίνακας3[[#This Row],[Πεδίο]]&amp;"` AS `"&amp;Πίνακας3[[#This Row],[Πεδίο]]&amp;"`,"</f>
         <v>`cases`.`creatinine` AS `creatinine`,</v>
       </c>
-      <c r="I29" s="11"/>
-      <c r="O29" s="11"/>
-      <c r="P29" s="11"/>
-      <c r="Q29" s="11"/>
-      <c r="R29" s="11"/>
-      <c r="S29" s="11"/>
-      <c r="T29" s="11"/>
-    </row>
-    <row r="30" spans="1:20" ht="30" x14ac:dyDescent="0.25">
-      <c r="A30" s="11" t="s">
+      <c r="I29" s="10"/>
+      <c r="O29" s="10"/>
+      <c r="P29" s="10"/>
+      <c r="Q29" s="10"/>
+      <c r="R29" s="10"/>
+      <c r="S29" s="10"/>
+      <c r="T29" s="10"/>
+    </row>
+    <row r="30" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A30" s="10" t="s">
         <v>85</v>
       </c>
-      <c r="B30" s="11" t="str">
+      <c r="B30" s="10" t="str">
         <f>VLOOKUP(Πίνακας3[[#This Row],[Τύπος SQL]],types,2,FALSE)</f>
         <v>Ναι/Όχι</v>
       </c>
-      <c r="C30" s="11" t="s">
+      <c r="C30" s="10" t="s">
         <v>127</v>
       </c>
-      <c r="D30" s="11" t="s">
-        <v>132</v>
-      </c>
-      <c r="E30" s="11"/>
-      <c r="F30" s="11"/>
-      <c r="G30" s="11"/>
-      <c r="H30" s="11" t="str">
+      <c r="D30" s="10" t="s">
+        <v>132</v>
+      </c>
+      <c r="E30" s="10"/>
+      <c r="F30" s="10"/>
+      <c r="G30" s="10"/>
+      <c r="H30" s="10" t="str">
         <f>"`cases`.`"&amp;Πίνακας3[[#This Row],[Πεδίο]]&amp;"` AS `"&amp;Πίνακας3[[#This Row],[Πεδίο]]&amp;"`,"</f>
         <v>`cases`.`atrialfibrillation` AS `atrialfibrillation`,</v>
       </c>
-      <c r="I30" s="11"/>
-      <c r="O30" s="11"/>
-      <c r="P30" s="11"/>
-      <c r="Q30" s="11"/>
-      <c r="R30" s="11"/>
-      <c r="S30" s="11"/>
-      <c r="T30" s="11"/>
+      <c r="I30" s="10"/>
+      <c r="O30" s="10"/>
+      <c r="P30" s="10"/>
+      <c r="Q30" s="10"/>
+      <c r="R30" s="10"/>
+      <c r="S30" s="10"/>
+      <c r="T30" s="10"/>
     </row>
     <row r="31" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A31" s="11" t="s">
+      <c r="A31" s="10" t="s">
         <v>69</v>
       </c>
-      <c r="B31" s="11" t="str">
+      <c r="B31" s="10" t="str">
         <f>VLOOKUP(Πίνακας3[[#This Row],[Τύπος SQL]],types,2,FALSE)</f>
         <v>Ναι/Όχι</v>
       </c>
-      <c r="C31" s="11" t="s">
+      <c r="C31" s="10" t="s">
         <v>127</v>
       </c>
-      <c r="D31" s="11" t="s">
-        <v>132</v>
-      </c>
-      <c r="E31" s="11"/>
-      <c r="F31" s="11"/>
-      <c r="G31" s="11"/>
-      <c r="H31" s="11" t="str">
+      <c r="D31" s="10" t="s">
+        <v>132</v>
+      </c>
+      <c r="E31" s="10"/>
+      <c r="F31" s="10"/>
+      <c r="G31" s="10"/>
+      <c r="H31" s="10" t="str">
         <f>"`cases`.`"&amp;Πίνακας3[[#This Row],[Πεδίο]]&amp;"` AS `"&amp;Πίνακας3[[#This Row],[Πεδίο]]&amp;"`,"</f>
         <v>`cases`.`heartfailure` AS `heartfailure`,</v>
       </c>
-      <c r="I31" s="11"/>
-      <c r="O31" s="11"/>
-      <c r="P31" s="11"/>
-      <c r="Q31" s="11"/>
-      <c r="R31" s="11"/>
-      <c r="S31" s="11"/>
-      <c r="T31" s="11"/>
+      <c r="I31" s="10"/>
+      <c r="O31" s="10"/>
+      <c r="P31" s="10"/>
+      <c r="Q31" s="10"/>
+      <c r="R31" s="10"/>
+      <c r="S31" s="10"/>
+      <c r="T31" s="10"/>
     </row>
     <row r="32" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A32" s="11" t="s">
+      <c r="A32" s="10" t="s">
         <v>138</v>
       </c>
-      <c r="B32" s="11" t="str">
+      <c r="B32" s="10" t="str">
         <f>VLOOKUP(Πίνακας3[[#This Row],[Τύπος SQL]],types,2,FALSE)</f>
         <v>Ναι/Όχι</v>
       </c>
-      <c r="C32" s="11" t="s">
+      <c r="C32" s="10" t="s">
         <v>127</v>
       </c>
-      <c r="D32" s="11" t="s">
-        <v>132</v>
-      </c>
-      <c r="E32" s="11"/>
-      <c r="F32" s="11"/>
-      <c r="G32" s="11"/>
-      <c r="H32" s="11" t="str">
+      <c r="D32" s="10" t="s">
+        <v>132</v>
+      </c>
+      <c r="E32" s="10"/>
+      <c r="F32" s="10"/>
+      <c r="G32" s="10"/>
+      <c r="H32" s="10" t="str">
         <f>"`cases`.`"&amp;Πίνακας3[[#This Row],[Πεδίο]]&amp;"` AS `"&amp;Πίνακας3[[#This Row],[Πεδίο]]&amp;"`,"</f>
         <v>`cases`.`cvd` AS `cvd`,</v>
       </c>
-      <c r="I32" s="11"/>
-      <c r="O32" s="11"/>
-      <c r="P32" s="11"/>
-      <c r="Q32" s="11"/>
-      <c r="R32" s="11"/>
-      <c r="S32" s="11"/>
-      <c r="T32" s="11"/>
+      <c r="I32" s="10"/>
+      <c r="O32" s="10"/>
+      <c r="P32" s="10"/>
+      <c r="Q32" s="10"/>
+      <c r="R32" s="10"/>
+      <c r="S32" s="10"/>
+      <c r="T32" s="10"/>
     </row>
     <row r="33" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A33" s="11" t="s">
+      <c r="A33" s="10" t="s">
         <v>139</v>
       </c>
-      <c r="B33" s="11" t="str">
+      <c r="B33" s="10" t="str">
         <f>VLOOKUP(Πίνακας3[[#This Row],[Τύπος SQL]],types,2,FALSE)</f>
         <v>Ακέραιος μέχρι 65535</v>
       </c>
-      <c r="C33" s="11" t="s">
+      <c r="C33" s="10" t="s">
         <v>140</v>
       </c>
-      <c r="D33" s="11" t="s">
-        <v>132</v>
-      </c>
-      <c r="E33" s="11"/>
-      <c r="F33" s="11"/>
-      <c r="G33" s="11"/>
-      <c r="H33" s="11" t="str">
+      <c r="D33" s="10" t="s">
+        <v>132</v>
+      </c>
+      <c r="E33" s="10"/>
+      <c r="F33" s="10"/>
+      <c r="G33" s="10"/>
+      <c r="H33" s="10" t="str">
         <f>"`cases`.`"&amp;Πίνακας3[[#This Row],[Πεδίο]]&amp;"` AS `"&amp;Πίνακας3[[#This Row],[Πεδίο]]&amp;"`,"</f>
         <v>`cases`.`yrcvd` AS `yrcvd`,</v>
       </c>
-      <c r="I33" s="11"/>
-      <c r="O33" s="11"/>
-      <c r="P33" s="11"/>
-      <c r="Q33" s="11"/>
-      <c r="R33" s="11"/>
-      <c r="S33" s="11"/>
-      <c r="T33" s="11"/>
+      <c r="I33" s="10"/>
+      <c r="O33" s="10"/>
+      <c r="P33" s="10"/>
+      <c r="Q33" s="10"/>
+      <c r="R33" s="10"/>
+      <c r="S33" s="10"/>
+      <c r="T33" s="10"/>
     </row>
     <row r="34" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A34" s="11" t="s">
+      <c r="A34" s="10" t="s">
         <v>121</v>
       </c>
-      <c r="B34" s="11" t="str">
+      <c r="B34" s="10" t="str">
         <f>VLOOKUP(Πίνακας3[[#This Row],[Τύπος SQL]],types,2,FALSE)</f>
         <v>Ναι/Όχι</v>
       </c>
-      <c r="C34" s="11" t="s">
+      <c r="C34" s="10" t="s">
         <v>127</v>
       </c>
-      <c r="D34" s="11" t="s">
-        <v>132</v>
-      </c>
-      <c r="E34" s="11"/>
-      <c r="F34" s="11"/>
-      <c r="G34" s="11"/>
-      <c r="H34" s="11" t="str">
+      <c r="D34" s="10" t="s">
+        <v>132</v>
+      </c>
+      <c r="E34" s="10"/>
+      <c r="F34" s="10"/>
+      <c r="G34" s="10"/>
+      <c r="H34" s="10" t="str">
         <f>"`cases`.`"&amp;Πίνακας3[[#This Row],[Πεδίο]]&amp;"` AS `"&amp;Πίνακας3[[#This Row],[Πεδίο]]&amp;"`,"</f>
         <v>`cases`.`deathcvd` AS `deathcvd`,</v>
       </c>
-      <c r="I34" s="11"/>
-      <c r="O34" s="11"/>
-      <c r="P34" s="11"/>
-      <c r="Q34" s="11"/>
-      <c r="R34" s="11"/>
-      <c r="S34" s="11"/>
-      <c r="T34" s="11"/>
+      <c r="I34" s="10"/>
+      <c r="O34" s="10"/>
+      <c r="P34" s="10"/>
+      <c r="Q34" s="10"/>
+      <c r="R34" s="10"/>
+      <c r="S34" s="10"/>
+      <c r="T34" s="10"/>
     </row>
     <row r="35" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A35" s="11" t="s">
+      <c r="A35" s="10" t="s">
         <v>122</v>
       </c>
-      <c r="B35" s="11" t="str">
+      <c r="B35" s="10" t="str">
         <f>VLOOKUP(Πίνακας3[[#This Row],[Τύπος SQL]],types,2,FALSE)</f>
         <v>Ακέραιος μέχρι 65535</v>
       </c>
-      <c r="C35" s="11" t="s">
+      <c r="C35" s="10" t="s">
         <v>140</v>
       </c>
-      <c r="D35" s="11" t="s">
-        <v>132</v>
-      </c>
-      <c r="E35" s="11"/>
-      <c r="F35" s="11"/>
-      <c r="G35" s="11"/>
-      <c r="H35" s="11" t="str">
+      <c r="D35" s="10" t="s">
+        <v>132</v>
+      </c>
+      <c r="E35" s="10"/>
+      <c r="F35" s="10"/>
+      <c r="G35" s="10"/>
+      <c r="H35" s="10" t="str">
         <f>"`cases`.`"&amp;Πίνακας3[[#This Row],[Πεδίο]]&amp;"` AS `"&amp;Πίνακας3[[#This Row],[Πεδίο]]&amp;"`,"</f>
         <v>`cases`.`yrcvddeath` AS `yrcvddeath`,</v>
       </c>
-      <c r="I35" s="11"/>
-      <c r="O35" s="11"/>
-      <c r="P35" s="11"/>
-      <c r="Q35" s="11"/>
-      <c r="R35" s="11"/>
-      <c r="S35" s="11"/>
-      <c r="T35" s="11"/>
+      <c r="I35" s="10"/>
+      <c r="O35" s="10"/>
+      <c r="P35" s="10"/>
+      <c r="Q35" s="10"/>
+      <c r="R35" s="10"/>
+      <c r="S35" s="10"/>
+      <c r="T35" s="10"/>
     </row>
     <row r="36" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A36" s="11" t="s">
+      <c r="A36" s="10" t="s">
         <v>57</v>
       </c>
-      <c r="B36" s="11" t="str">
+      <c r="B36" s="10" t="str">
         <f>VLOOKUP(Πίνακας3[[#This Row],[Τύπος SQL]],types,2,FALSE)</f>
         <v>Ναι/Όχι</v>
       </c>
-      <c r="C36" s="11" t="s">
+      <c r="C36" s="10" t="s">
         <v>127</v>
       </c>
-      <c r="D36" s="11" t="s">
-        <v>132</v>
-      </c>
-      <c r="E36" s="11"/>
-      <c r="F36" s="11"/>
-      <c r="G36" s="11"/>
-      <c r="H36" s="11" t="str">
+      <c r="D36" s="10" t="s">
+        <v>132</v>
+      </c>
+      <c r="E36" s="10"/>
+      <c r="F36" s="10"/>
+      <c r="G36" s="10"/>
+      <c r="H36" s="10" t="str">
         <f>"`cases`.`"&amp;Πίνακας3[[#This Row],[Πεδίο]]&amp;"` AS `"&amp;Πίνακας3[[#This Row],[Πεδίο]]&amp;"`,"</f>
         <v>`cases`.`familyhistory` AS `familyhistory`,</v>
       </c>
-      <c r="I36" s="11"/>
-      <c r="O36" s="11"/>
-      <c r="P36" s="11"/>
-      <c r="Q36" s="11"/>
-      <c r="R36" s="11"/>
-      <c r="S36" s="11"/>
-      <c r="T36" s="11"/>
+      <c r="I36" s="10"/>
+      <c r="O36" s="10"/>
+      <c r="P36" s="10"/>
+      <c r="Q36" s="10"/>
+      <c r="R36" s="10"/>
+      <c r="S36" s="10"/>
+      <c r="T36" s="10"/>
     </row>
     <row r="37" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A37" s="11" t="s">
+      <c r="A37" s="10" t="s">
         <v>70</v>
       </c>
-      <c r="B37" s="11" t="str">
+      <c r="B37" s="10" t="str">
         <f>VLOOKUP(Πίνακας3[[#This Row],[Τύπος SQL]],types,2,FALSE)</f>
         <v>Ναι/Όχι</v>
       </c>
-      <c r="C37" s="11" t="s">
+      <c r="C37" s="10" t="s">
         <v>127</v>
       </c>
-      <c r="D37" s="11" t="s">
-        <v>132</v>
-      </c>
-      <c r="E37" s="11"/>
-      <c r="F37" s="11"/>
-      <c r="G37" s="11"/>
-      <c r="H37" s="11" t="str">
+      <c r="D37" s="10" t="s">
+        <v>132</v>
+      </c>
+      <c r="E37" s="10"/>
+      <c r="F37" s="10"/>
+      <c r="G37" s="10"/>
+      <c r="H37" s="10" t="str">
         <f>"`cases`.`"&amp;Πίνακας3[[#This Row],[Πεδίο]]&amp;"` AS `"&amp;Πίνακας3[[#This Row],[Πεδίο]]&amp;"`,"</f>
         <v>`cases`.`cancer` AS `cancer`,</v>
       </c>
-      <c r="I37" s="11"/>
-      <c r="O37" s="11"/>
-      <c r="P37" s="11"/>
-      <c r="Q37" s="11"/>
-      <c r="R37" s="11"/>
-      <c r="S37" s="11"/>
-      <c r="T37" s="11"/>
+      <c r="I37" s="10"/>
+      <c r="O37" s="10"/>
+      <c r="P37" s="10"/>
+      <c r="Q37" s="10"/>
+      <c r="R37" s="10"/>
+      <c r="S37" s="10"/>
+      <c r="T37" s="10"/>
     </row>
     <row r="38" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A38" s="11" t="s">
+      <c r="A38" s="10" t="s">
         <v>120</v>
       </c>
-      <c r="B38" s="11" t="str">
+      <c r="B38" s="10" t="str">
         <f>VLOOKUP(Πίνακας3[[#This Row],[Τύπος SQL]],types,2,FALSE)</f>
         <v>Ακέραιος μέχρι 65535</v>
       </c>
-      <c r="C38" s="11" t="s">
+      <c r="C38" s="10" t="s">
         <v>140</v>
       </c>
-      <c r="D38" s="11" t="s">
-        <v>132</v>
-      </c>
-      <c r="E38" s="11"/>
-      <c r="F38" s="11"/>
-      <c r="G38" s="11"/>
-      <c r="H38" s="11" t="str">
+      <c r="D38" s="10" t="s">
+        <v>132</v>
+      </c>
+      <c r="E38" s="10"/>
+      <c r="F38" s="10"/>
+      <c r="G38" s="10"/>
+      <c r="H38" s="10" t="str">
         <f>"`cases`.`"&amp;Πίνακας3[[#This Row],[Πεδίο]]&amp;"` AS `"&amp;Πίνακας3[[#This Row],[Πεδίο]]&amp;"`,"</f>
         <v>`cases`.`yrcancer` AS `yrcancer`,</v>
       </c>
-      <c r="I38" s="11"/>
-      <c r="O38" s="11"/>
-      <c r="P38" s="11"/>
-      <c r="Q38" s="11"/>
-      <c r="R38" s="11"/>
-      <c r="S38" s="11"/>
-      <c r="T38" s="11"/>
+      <c r="I38" s="10"/>
+      <c r="O38" s="10"/>
+      <c r="P38" s="10"/>
+      <c r="Q38" s="10"/>
+      <c r="R38" s="10"/>
+      <c r="S38" s="10"/>
+      <c r="T38" s="10"/>
     </row>
     <row r="39" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A39" s="11" t="s">
+      <c r="A39" s="10" t="s">
         <v>141</v>
       </c>
-      <c r="B39" s="11" t="str">
+      <c r="B39" s="10" t="str">
         <f>VLOOKUP(Πίνακας3[[#This Row],[Τύπος SQL]],types,2,FALSE)</f>
         <v>Μεγάλο κείμενο</v>
       </c>
-      <c r="C39" s="11" t="s">
+      <c r="C39" s="10" t="s">
         <v>142</v>
       </c>
-      <c r="D39" s="11" t="s">
-        <v>132</v>
-      </c>
-      <c r="E39" s="11"/>
-      <c r="F39" s="11"/>
-      <c r="G39" s="11"/>
-      <c r="H39" s="11" t="str">
+      <c r="D39" s="10" t="s">
+        <v>132</v>
+      </c>
+      <c r="E39" s="10"/>
+      <c r="F39" s="10"/>
+      <c r="G39" s="10"/>
+      <c r="H39" s="10" t="str">
         <f>"`cases`.`"&amp;Πίνακας3[[#This Row],[Πεδίο]]&amp;"` AS `"&amp;Πίνακας3[[#This Row],[Πεδίο]]&amp;"`,"</f>
         <v>`cases`.`comments` AS `comments`,</v>
       </c>
-      <c r="I39" s="11"/>
-      <c r="O39" s="11"/>
-      <c r="P39" s="11"/>
-      <c r="Q39" s="11"/>
-      <c r="R39" s="11"/>
-      <c r="S39" s="11"/>
-      <c r="T39" s="11"/>
+      <c r="I39" s="10"/>
+      <c r="O39" s="10"/>
+      <c r="P39" s="10"/>
+      <c r="Q39" s="10"/>
+      <c r="R39" s="10"/>
+      <c r="S39" s="10"/>
+      <c r="T39" s="10"/>
     </row>
     <row r="40" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A40" s="11" t="s">
+      <c r="A40" s="10" t="s">
         <v>74</v>
       </c>
-      <c r="B40" s="11" t="str">
+      <c r="B40" s="10" t="str">
         <f>VLOOKUP(Πίνακας3[[#This Row],[Τύπος SQL]],types,2,FALSE)</f>
         <v>Ημερομηνία και Ώρα</v>
       </c>
-      <c r="C40" s="11" t="s">
+      <c r="C40" s="10" t="s">
         <v>143</v>
       </c>
-      <c r="D40" s="11" t="s">
+      <c r="D40" s="10" t="s">
         <v>124</v>
       </c>
-      <c r="E40" s="11"/>
-      <c r="F40" s="11"/>
-      <c r="G40" s="11"/>
-      <c r="H40" s="11" t="str">
+      <c r="E40" s="10"/>
+      <c r="F40" s="10"/>
+      <c r="G40" s="10"/>
+      <c r="H40" s="10" t="str">
         <f>"`cases`.`"&amp;Πίνακας3[[#This Row],[Πεδίο]]&amp;"` AS `"&amp;Πίνακας3[[#This Row],[Πεδίο]]&amp;"`,"</f>
         <v>`cases`.`createdAt` AS `createdAt`,</v>
       </c>
-      <c r="I40" s="11"/>
-      <c r="O40" s="11"/>
-      <c r="P40" s="11"/>
-      <c r="Q40" s="11"/>
-      <c r="R40" s="11"/>
-      <c r="S40" s="11"/>
-      <c r="T40" s="11"/>
+      <c r="I40" s="10"/>
+      <c r="O40" s="10"/>
+      <c r="P40" s="10"/>
+      <c r="Q40" s="10"/>
+      <c r="R40" s="10"/>
+      <c r="S40" s="10"/>
+      <c r="T40" s="10"/>
     </row>
     <row r="41" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A41" s="11" t="s">
+      <c r="A41" s="10" t="s">
         <v>75</v>
       </c>
-      <c r="B41" s="11" t="str">
+      <c r="B41" s="10" t="str">
         <f>VLOOKUP(Πίνακας3[[#This Row],[Τύπος SQL]],types,2,FALSE)</f>
         <v>Ημερομηνία και Ώρα</v>
       </c>
-      <c r="C41" s="11" t="s">
+      <c r="C41" s="10" t="s">
         <v>143</v>
       </c>
-      <c r="D41" s="11" t="s">
+      <c r="D41" s="10" t="s">
         <v>124</v>
       </c>
-      <c r="E41" s="11"/>
-      <c r="F41" s="11"/>
-      <c r="G41" s="11"/>
-      <c r="H41" s="11" t="str">
+      <c r="E41" s="10"/>
+      <c r="F41" s="10"/>
+      <c r="G41" s="10"/>
+      <c r="H41" s="10" t="str">
         <f>"`cases`.`"&amp;Πίνακας3[[#This Row],[Πεδίο]]&amp;"` AS `"&amp;Πίνακας3[[#This Row],[Πεδίο]]&amp;"`,"</f>
         <v>`cases`.`updatedAt` AS `updatedAt`,</v>
       </c>
-      <c r="I41" s="11"/>
-      <c r="O41" s="11"/>
-      <c r="P41" s="11"/>
-      <c r="Q41" s="11"/>
-      <c r="R41" s="11"/>
-      <c r="S41" s="11"/>
-      <c r="T41" s="11"/>
+      <c r="I41" s="10"/>
+      <c r="O41" s="10"/>
+      <c r="P41" s="10"/>
+      <c r="Q41" s="10"/>
+      <c r="R41" s="10"/>
+      <c r="S41" s="10"/>
+      <c r="T41" s="10"/>
     </row>
     <row r="42" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A42" s="11" t="s">
+      <c r="A42" s="10" t="s">
         <v>73</v>
       </c>
-      <c r="B42" s="11" t="str">
+      <c r="B42" s="10" t="str">
         <f>VLOOKUP(Πίνακας3[[#This Row],[Τύπος SQL]],types,2,FALSE)</f>
         <v>Σύντομο κείμενο</v>
       </c>
-      <c r="C42" s="11" t="s">
+      <c r="C42" s="10" t="s">
         <v>129</v>
       </c>
-      <c r="D42" s="11" t="s">
-        <v>132</v>
-      </c>
-      <c r="E42" s="11" t="s">
+      <c r="D42" s="10" t="s">
+        <v>132</v>
+      </c>
+      <c r="E42" s="10" t="s">
         <v>130</v>
       </c>
-      <c r="F42" s="11"/>
-      <c r="G42" s="11"/>
-      <c r="H42" s="11" t="str">
+      <c r="F42" s="10"/>
+      <c r="G42" s="10"/>
+      <c r="H42" s="10" t="str">
         <f>"`cases`.`"&amp;Πίνακας3[[#This Row],[Πεδίο]]&amp;"` AS `"&amp;Πίνακας3[[#This Row],[Πεδίο]]&amp;"`,"</f>
         <v>`cases`.`author` AS `author`,</v>
       </c>
-      <c r="I42" s="11"/>
-      <c r="O42" s="11"/>
-      <c r="P42" s="11"/>
-      <c r="Q42" s="11"/>
-      <c r="R42" s="11"/>
-      <c r="S42" s="11"/>
-      <c r="T42" s="11"/>
+      <c r="I42" s="10"/>
+      <c r="O42" s="10"/>
+      <c r="P42" s="10"/>
+      <c r="Q42" s="10"/>
+      <c r="R42" s="10"/>
+      <c r="S42" s="10"/>
+      <c r="T42" s="10"/>
     </row>
     <row r="50" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B50" s="14"/>
+      <c r="B50" s="13"/>
     </row>
     <row r="51" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B51" s="15"/>
+      <c r="B51" s="14"/>
     </row>
     <row r="52" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B52" s="14"/>
+      <c r="B52" s="13"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
2.5 - case db changes
</commit_message>
<xml_diff>
--- a/Docs/ΕΥΚΑΡΔΙΑ Πεδία Βάσης Δεδομένων.xlsx
+++ b/Docs/ΕΥΚΑΡΔΙΑ Πεδία Βάσης Δεδομένων.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20392"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20402"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Development\Eukardia\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34582209-90B0-4A04-B843-107CE28D85B5}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4ECD03BF-904E-46E3-9D35-A38977559B60}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11625" tabRatio="481" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="27495" windowHeight="11280" activeTab="1" xr2:uid="{0B5BD202-A035-444D-B556-E8A6C1CCE3CE}"/>
   </bookViews>
   <sheets>
     <sheet name="Πεδία" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="354" uniqueCount="157">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="371" uniqueCount="165">
   <si>
     <t>Όνομα πεδίου</t>
   </si>
@@ -501,6 +501,30 @@
   </si>
   <si>
     <t>SQL view</t>
+  </si>
+  <si>
+    <t>Έτος ένταξης στην μελέτη</t>
+  </si>
+  <si>
+    <t>yrinc</t>
+  </si>
+  <si>
+    <t>weight</t>
+  </si>
+  <si>
+    <t>height</t>
+  </si>
+  <si>
+    <t>Βάρος</t>
+  </si>
+  <si>
+    <t>Ύψος</t>
+  </si>
+  <si>
+    <t>Σχόλια</t>
+  </si>
+  <si>
+    <t>Κείμενο</t>
   </si>
 </sst>
 </file>
@@ -640,7 +664,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -665,6 +689,9 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -977,8 +1004,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Πίνακας1" displayName="Πίνακας1" ref="A1:G37" totalsRowShown="0" headerRowDxfId="27" dataDxfId="26">
-  <autoFilter ref="A1:G37" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Πίνακας1" displayName="Πίνακας1" ref="A1:G41" totalsRowShown="0" headerRowDxfId="27" dataDxfId="26">
+  <autoFilter ref="A1:G41" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="7">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Περιγραφή πεδίου" dataDxfId="25"/>
     <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Υποχρεωτική συμπλήρωση" dataDxfId="24"/>
@@ -993,8 +1020,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Πίνακας2" displayName="Πίνακας2" ref="A42:G46" totalsRowShown="0" headerRowDxfId="18" dataDxfId="17" tableBorderDxfId="16">
-  <autoFilter ref="A42:G46" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Πίνακας2" displayName="Πίνακας2" ref="A45:G49" totalsRowShown="0" headerRowDxfId="18" dataDxfId="17" tableBorderDxfId="16">
+  <autoFilter ref="A45:G49" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
   <tableColumns count="7">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="Όνομα πεδίου" dataDxfId="15"/>
     <tableColumn id="4" xr3:uid="{00000000-0010-0000-0100-000004000000}" name="Υποχρεωτικό" dataDxfId="14"/>
@@ -1009,8 +1036,8 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{124B803E-62B7-4DF6-97EB-31E33393CFE8}" name="Πίνακας3" displayName="Πίνακας3" ref="A1:H42" totalsRowShown="0" dataDxfId="8">
-  <autoFilter ref="A1:H42" xr:uid="{89C5C1E3-CE08-4CF4-BF51-207D1F88BF61}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{124B803E-62B7-4DF6-97EB-31E33393CFE8}" name="Πίνακας3" displayName="Πίνακας3" ref="A1:H45" totalsRowShown="0" dataDxfId="8">
+  <autoFilter ref="A1:H45" xr:uid="{89C5C1E3-CE08-4CF4-BF51-207D1F88BF61}"/>
   <tableColumns count="8">
     <tableColumn id="1" xr3:uid="{310BA3A6-8BAB-4AFE-9044-3DBC1F268DB3}" name="Πεδίο" dataDxfId="7"/>
     <tableColumn id="2" xr3:uid="{3986543B-C60B-42C6-BDEF-7981CFB32FA8}" name="Τύπος (κατανοητός)" dataDxfId="6">
@@ -1296,10 +1323,10 @@
     <tabColor rgb="FF00B0F0"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:G46"/>
+  <dimension ref="A1:G49"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1354,526 +1381,512 @@
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="E3" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="F3" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="G3" s="3" t="s">
-        <v>40</v>
-      </c>
+      <c r="A3" t="s">
+        <v>157</v>
+      </c>
+      <c r="B3" s="4"/>
+      <c r="C3" s="10" t="s">
+        <v>158</v>
+      </c>
+      <c r="E3" s="4"/>
+      <c r="F3" s="4"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>5</v>
+        <v>34</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>6</v>
+        <v>35</v>
       </c>
       <c r="E4" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="F4" s="3" t="s">
-        <v>7</v>
+      <c r="F4" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="E5" s="3" t="s">
-        <v>28</v>
+        <v>6</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>30</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>46</v>
+        <v>7</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>115</v>
+        <v>8</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>92</v>
+        <v>55</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>6</v>
+        <v>27</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>28</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>91</v>
+        <v>46</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>9</v>
-      </c>
+        <v>161</v>
+      </c>
+      <c r="B7" s="4"/>
       <c r="C7" s="3" t="s">
-        <v>97</v>
+        <v>159</v>
       </c>
       <c r="D7" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="E7" s="3" t="s">
-        <v>78</v>
-      </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
-        <v>96</v>
+        <v>162</v>
       </c>
       <c r="B8" s="4"/>
       <c r="C8" s="3" t="s">
-        <v>98</v>
+        <v>160</v>
       </c>
       <c r="D8" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="E8" s="3" t="s">
-        <v>78</v>
-      </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
-        <v>10</v>
-      </c>
+        <v>106</v>
+      </c>
+      <c r="B9" s="4"/>
       <c r="C9" s="3" t="s">
-        <v>56</v>
+        <v>62</v>
       </c>
       <c r="D9" s="3" t="s">
         <v>27</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="B10" s="4"/>
+        <v>115</v>
+      </c>
       <c r="C10" s="3" t="s">
-        <v>68</v>
+        <v>92</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="E10" s="3" t="s">
-        <v>87</v>
+        <v>6</v>
+      </c>
+      <c r="F10" s="3" t="s">
+        <v>91</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="B11" s="4"/>
+        <v>9</v>
+      </c>
       <c r="C11" s="3" t="s">
-        <v>83</v>
-      </c>
-      <c r="D11" s="9" t="s">
-        <v>118</v>
+        <v>97</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>27</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="F11" s="3" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
-        <v>11</v>
-      </c>
+        <v>96</v>
+      </c>
+      <c r="B12" s="4"/>
       <c r="C12" s="3" t="s">
-        <v>58</v>
+        <v>98</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="E12" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="F12" s="3" t="s">
-        <v>104</v>
-      </c>
-      <c r="G12" s="1" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+        <v>27</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="E13" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="F13" s="1" t="s">
-        <v>119</v>
-      </c>
-      <c r="G13" s="1" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+        <v>27</v>
+      </c>
+      <c r="E13" s="3" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
-        <v>108</v>
-      </c>
+        <v>23</v>
+      </c>
+      <c r="B14" s="4"/>
       <c r="C14" s="3" t="s">
-        <v>109</v>
+        <v>68</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="F14" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="G14" s="1" t="s">
-        <v>107</v>
+        <v>27</v>
+      </c>
+      <c r="E14" s="3" t="s">
+        <v>87</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B15" s="4"/>
+      <c r="C15" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="D15" s="9" t="s">
+        <v>118</v>
+      </c>
+      <c r="E15" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="F15" s="3" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A16" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E16" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="F16" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="G16" s="1" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A17" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E17" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="G17" s="1" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A18" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="D18" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="G18" s="1" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="C15" s="3" t="s">
+      <c r="C19" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="D15" s="3" t="s">
+      <c r="D19" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="E15" s="4" t="s">
+      <c r="E19" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="F15" s="3" t="s">
+      <c r="F19" s="3" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16" s="3" t="s">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20" s="3" t="s">
         <v>89</v>
-      </c>
-      <c r="B16" s="4"/>
-      <c r="C16" s="3" t="s">
-        <v>90</v>
-      </c>
-      <c r="D16" s="9" t="s">
-        <v>118</v>
-      </c>
-      <c r="E16" s="4"/>
-      <c r="F16" s="3" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="B17" s="4"/>
-      <c r="C17" s="3" t="s">
-        <v>84</v>
-      </c>
-      <c r="D17" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="E17" s="3" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="B18" s="4"/>
-      <c r="C18" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="D18" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="E18" s="3" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="B19" s="4"/>
-      <c r="C19" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="D19" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="E19" s="3" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A20" s="3" t="s">
-        <v>22</v>
       </c>
       <c r="B20" s="4"/>
       <c r="C20" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="D20" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="E20" s="3" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+        <v>90</v>
+      </c>
+      <c r="D20" s="9" t="s">
+        <v>118</v>
+      </c>
+      <c r="E20" s="4"/>
+      <c r="F20" s="3" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
-        <v>106</v>
+        <v>20</v>
       </c>
       <c r="B21" s="4"/>
       <c r="C21" s="3" t="s">
-        <v>62</v>
+        <v>84</v>
       </c>
       <c r="D21" s="3" t="s">
         <v>27</v>
       </c>
       <c r="E21" s="3" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B22" s="4"/>
       <c r="C22" s="3" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="D22" s="3" t="s">
         <v>27</v>
       </c>
       <c r="E22" s="3" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="B23" s="4"/>
       <c r="C23" s="3" t="s">
-        <v>77</v>
+        <v>66</v>
       </c>
       <c r="D23" s="3" t="s">
         <v>27</v>
       </c>
       <c r="E23" s="3" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
-        <v>49</v>
+        <v>22</v>
       </c>
       <c r="B24" s="4"/>
       <c r="C24" s="3" t="s">
-        <v>94</v>
+        <v>67</v>
       </c>
       <c r="D24" s="3" t="s">
         <v>27</v>
       </c>
       <c r="E24" s="3" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B25" s="4"/>
       <c r="C25" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D25" s="3" t="s">
         <v>27</v>
       </c>
       <c r="E25" s="3" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B26" s="4"/>
       <c r="C26" s="3" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="D26" s="3" t="s">
         <v>27</v>
       </c>
       <c r="E26" s="3" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
-        <v>19</v>
+        <v>49</v>
       </c>
       <c r="B27" s="4"/>
       <c r="C27" s="3" t="s">
-        <v>65</v>
+        <v>94</v>
       </c>
       <c r="D27" s="3" t="s">
         <v>27</v>
       </c>
       <c r="E27" s="3" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
-        <v>26</v>
+        <v>17</v>
       </c>
       <c r="B28" s="4"/>
       <c r="C28" s="3" t="s">
-        <v>71</v>
+        <v>64</v>
       </c>
       <c r="D28" s="3" t="s">
         <v>27</v>
       </c>
       <c r="E28" s="3" t="s">
-        <v>79</v>
-      </c>
-      <c r="F28" s="4"/>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
-        <v>111</v>
+        <v>18</v>
       </c>
       <c r="B29" s="4"/>
       <c r="C29" s="3" t="s">
-        <v>85</v>
-      </c>
-      <c r="D29" s="9" t="s">
-        <v>118</v>
-      </c>
-      <c r="E29" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="D29" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="E29" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="F29" s="3" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" s="3" t="s">
-        <v>114</v>
+        <v>19</v>
       </c>
       <c r="B30" s="4"/>
       <c r="C30" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="D30" s="9" t="s">
-        <v>118</v>
-      </c>
-      <c r="E30" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="F30" s="3" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+        <v>65</v>
+      </c>
+      <c r="D30" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="E30" s="3" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" s="3" t="s">
-        <v>113</v>
+        <v>26</v>
       </c>
       <c r="B31" s="4"/>
       <c r="C31" s="3" t="s">
-        <v>95</v>
-      </c>
-      <c r="D31" s="9" t="s">
-        <v>118</v>
-      </c>
-      <c r="E31" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="F31" s="3" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+        <v>71</v>
+      </c>
+      <c r="D31" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="E31" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="F31" s="4"/>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" s="3" t="s">
-        <v>101</v>
+        <v>25</v>
       </c>
       <c r="B32" s="4"/>
       <c r="C32" s="3" t="s">
-        <v>102</v>
-      </c>
-      <c r="D32" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="E32" s="3" t="s">
-        <v>103</v>
+        <v>70</v>
+      </c>
+      <c r="D32" s="9" t="s">
+        <v>118</v>
+      </c>
+      <c r="E32" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="F32" s="3" t="s">
+        <v>91</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" s="3" t="s">
-        <v>112</v>
-      </c>
-      <c r="B33" s="4"/>
+        <v>105</v>
+      </c>
       <c r="C33" s="3" t="s">
-        <v>121</v>
-      </c>
-      <c r="D33" s="9" t="s">
-        <v>118</v>
-      </c>
-      <c r="F33" s="3" t="s">
-        <v>91</v>
+        <v>120</v>
+      </c>
+      <c r="D33" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="E33" s="3" t="s">
+        <v>103</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" s="3" t="s">
-        <v>117</v>
+        <v>111</v>
       </c>
       <c r="B34" s="4"/>
       <c r="C34" s="3" t="s">
-        <v>122</v>
-      </c>
-      <c r="D34" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="E34" s="3" t="s">
-        <v>103</v>
+        <v>85</v>
+      </c>
+      <c r="D34" s="9" t="s">
+        <v>118</v>
+      </c>
+      <c r="E34" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="F34" s="3" t="s">
+        <v>91</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" s="3" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="B35" s="4"/>
       <c r="C35" s="3" t="s">
-        <v>57</v>
+        <v>69</v>
       </c>
       <c r="D35" s="9" t="s">
         <v>118</v>
@@ -1881,17 +1894,17 @@
       <c r="E35" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="F35" s="4" t="s">
+      <c r="F35" s="3" t="s">
         <v>91</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" s="3" t="s">
-        <v>25</v>
+        <v>113</v>
       </c>
       <c r="B36" s="4"/>
       <c r="C36" s="3" t="s">
-        <v>70</v>
+        <v>95</v>
       </c>
       <c r="D36" s="9" t="s">
         <v>118</v>
@@ -1905,10 +1918,11 @@
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" s="3" t="s">
-        <v>105</v>
-      </c>
+        <v>101</v>
+      </c>
+      <c r="B37" s="4"/>
       <c r="C37" s="3" t="s">
-        <v>120</v>
+        <v>102</v>
       </c>
       <c r="D37" s="3" t="s">
         <v>27</v>
@@ -1917,120 +1931,180 @@
         <v>103</v>
       </c>
     </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A38" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="B38" s="4"/>
+      <c r="C38" s="3" t="s">
+        <v>121</v>
+      </c>
+      <c r="D38" s="9" t="s">
+        <v>118</v>
+      </c>
+      <c r="F38" s="3" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A39" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="B39" s="4"/>
+      <c r="C39" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="D39" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="E39" s="3" t="s">
+        <v>103</v>
+      </c>
+    </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A40" s="3" t="s">
+        <v>116</v>
+      </c>
       <c r="B40" s="4"/>
+      <c r="C40" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="D40" s="9" t="s">
+        <v>118</v>
+      </c>
+      <c r="E40" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="F40" s="4" t="s">
+        <v>91</v>
+      </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" s="3" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="42" spans="1:7" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="B42" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="C42" s="5" t="s">
-        <v>76</v>
-      </c>
-      <c r="D42" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="E42" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="F42" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="G42" s="6" t="s">
-        <v>39</v>
+        <v>163</v>
+      </c>
+      <c r="B41" s="4"/>
+      <c r="C41" s="10" t="s">
+        <v>141</v>
+      </c>
+      <c r="D41" s="3" t="s">
+        <v>164</v>
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A43" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="B43" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="C43" s="3" t="s">
-        <v>72</v>
-      </c>
-      <c r="D43" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="E43" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="F43" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="G43" s="3" t="s">
-        <v>41</v>
-      </c>
+      <c r="B43" s="4"/>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A44" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="B44" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="C44" s="3" t="s">
-        <v>73</v>
-      </c>
-      <c r="D44" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="E44" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="F44" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="G44" s="3" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A45" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="B45" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="C45" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="D45" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="E45" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="F45" s="4" t="s">
-        <v>44</v>
+        <v>48</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A45" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B45" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="C45" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="D45" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="E45" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="F45" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="G45" s="6" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A46" s="3" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B46" s="4" t="s">
         <v>29</v>
       </c>
       <c r="C46" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="D46" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="E46" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="F46" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="G46" s="3" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A47" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="B47" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="C47" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="D47" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="E47" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="F47" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="G47" s="3" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A48" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="B48" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="C48" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="D48" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="E48" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="F48" s="4" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A49" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="B49" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="C49" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="D46" s="3" t="s">
+      <c r="D49" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="E46" s="4" t="s">
+      <c r="E49" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="F46" s="4" t="s">
+      <c r="F49" s="4" t="s">
         <v>44</v>
       </c>
     </row>
@@ -2050,9 +2124,11 @@
   <sheetPr>
     <tabColor rgb="FF7030A0"/>
   </sheetPr>
-  <dimension ref="A1:T52"/>
+  <dimension ref="A1:T55"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="25.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -2182,26 +2258,22 @@
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A4" s="10" t="s">
-        <v>128</v>
+        <v>158</v>
       </c>
       <c r="B4" s="10" t="str">
         <f>VLOOKUP(Πίνακας3[[#This Row],[Τύπος SQL]],types,2,FALSE)</f>
-        <v>Σύντομο κείμενο</v>
+        <v>Ακέραιος μέχρι 65535</v>
       </c>
       <c r="C4" s="10" t="s">
-        <v>129</v>
-      </c>
-      <c r="D4" s="10" t="s">
-        <v>124</v>
-      </c>
-      <c r="E4" s="10" t="s">
-        <v>130</v>
-      </c>
+        <v>140</v>
+      </c>
+      <c r="D4" s="10"/>
+      <c r="E4" s="10"/>
       <c r="F4" s="10"/>
       <c r="G4" s="10"/>
-      <c r="H4" s="10" t="str">
-        <f>"`cases`.`"&amp;Πίνακας3[[#This Row],[Πεδίο]]&amp;"` AS `"&amp;Πίνακας3[[#This Row],[Πεδίο]]&amp;"`,"</f>
-        <v>`cases`.`patientId` AS `patientId`,</v>
+      <c r="H4" s="15" t="str">
+        <f>"`cases`.`"&amp;Πίνακας3[[#This Row],[Πεδίο]]&amp;"` AS `"&amp;Πίνακας3[[#This Row],[Πεδίο]]&amp;"`,"</f>
+        <v>`cases`.`yrinc` AS `yrinc`,</v>
       </c>
       <c r="I4" s="10"/>
       <c r="K4" s="12" t="s">
@@ -2219,24 +2291,26 @@
     </row>
     <row r="5" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A5" s="10" t="s">
-        <v>54</v>
+        <v>128</v>
       </c>
       <c r="B5" s="10" t="str">
         <f>VLOOKUP(Πίνακας3[[#This Row],[Τύπος SQL]],types,2,FALSE)</f>
-        <v xml:space="preserve">Ακέραιος ή λίστα μέχρι 127 </v>
+        <v>Σύντομο κείμενο</v>
       </c>
       <c r="C5" s="10" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="D5" s="10" t="s">
-        <v>132</v>
-      </c>
-      <c r="E5" s="10"/>
+        <v>124</v>
+      </c>
+      <c r="E5" s="10" t="s">
+        <v>130</v>
+      </c>
       <c r="F5" s="10"/>
       <c r="G5" s="10"/>
       <c r="H5" s="10" t="str">
         <f>"`cases`.`"&amp;Πίνακας3[[#This Row],[Πεδίο]]&amp;"` AS `"&amp;Πίνακας3[[#This Row],[Πεδίο]]&amp;"`,"</f>
-        <v>`cases`.`gender` AS `gender`,</v>
+        <v>`cases`.`patientId` AS `patientId`,</v>
       </c>
       <c r="I5" s="10"/>
       <c r="K5" s="12" t="s">
@@ -2254,7 +2328,7 @@
     </row>
     <row r="6" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A6" s="10" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B6" s="10" t="str">
         <f>VLOOKUP(Πίνακας3[[#This Row],[Τύπος SQL]],types,2,FALSE)</f>
@@ -2271,7 +2345,7 @@
       <c r="G6" s="10"/>
       <c r="H6" s="10" t="str">
         <f>"`cases`.`"&amp;Πίνακας3[[#This Row],[Πεδίο]]&amp;"` AS `"&amp;Πίνακας3[[#This Row],[Πεδίο]]&amp;"`,"</f>
-        <v>`cases`.`age` AS `age`,</v>
+        <v>`cases`.`gender` AS `gender`,</v>
       </c>
       <c r="I6" s="10"/>
       <c r="K6" s="12" t="s">
@@ -2289,14 +2363,14 @@
     </row>
     <row r="7" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A7" s="10" t="s">
-        <v>133</v>
+        <v>55</v>
       </c>
       <c r="B7" s="10" t="str">
         <f>VLOOKUP(Πίνακας3[[#This Row],[Τύπος SQL]],types,2,FALSE)</f>
-        <v>Ναι/Όχι</v>
+        <v>Ακέραιος μέχρι 65535</v>
       </c>
       <c r="C7" s="10" t="s">
-        <v>127</v>
+        <v>140</v>
       </c>
       <c r="D7" s="10" t="s">
         <v>132</v>
@@ -2306,7 +2380,7 @@
       <c r="G7" s="10"/>
       <c r="H7" s="10" t="str">
         <f>"`cases`.`"&amp;Πίνακας3[[#This Row],[Πεδίο]]&amp;"` AS `"&amp;Πίνακας3[[#This Row],[Πεδίο]]&amp;"`,"</f>
-        <v>`cases`.`drugbp` AS `drugbp`,</v>
+        <v>`cases`.`age` AS `age`,</v>
       </c>
       <c r="I7" s="10"/>
       <c r="K7" s="12" t="s">
@@ -2324,24 +2398,22 @@
     </row>
     <row r="8" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A8" s="10" t="s">
-        <v>134</v>
-      </c>
-      <c r="B8" s="10" t="str">
-        <f>VLOOKUP(Πίνακας3[[#This Row],[Τύπος SQL]],types,2,FALSE)</f>
-        <v>Δεκαδικός αριθμός</v>
+        <v>159</v>
+      </c>
+      <c r="B8" s="15" t="str">
+        <f>VLOOKUP(Πίνακας3[[#This Row],[Τύπος SQL]],types,2,FALSE)</f>
+        <v>Ακέραιος μέχρι 65535</v>
       </c>
       <c r="C8" s="10" t="s">
-        <v>135</v>
-      </c>
-      <c r="D8" s="10" t="s">
-        <v>132</v>
-      </c>
+        <v>140</v>
+      </c>
+      <c r="D8" s="10"/>
       <c r="E8" s="10"/>
       <c r="F8" s="10"/>
       <c r="G8" s="10"/>
-      <c r="H8" s="10" t="str">
-        <f>"`cases`.`"&amp;Πίνακας3[[#This Row],[Πεδίο]]&amp;"` AS `"&amp;Πίνακας3[[#This Row],[Πεδίο]]&amp;"`,"</f>
-        <v>`cases`.`sbp` AS `sbp`,</v>
+      <c r="H8" s="15" t="str">
+        <f>"`cases`.`"&amp;Πίνακας3[[#This Row],[Πεδίο]]&amp;"` AS `"&amp;Πίνακας3[[#This Row],[Πεδίο]]&amp;"`,"</f>
+        <v>`cases`.`weight` AS `weight`,</v>
       </c>
       <c r="I8" s="10"/>
       <c r="K8" s="12" t="s">
@@ -2359,24 +2431,22 @@
     </row>
     <row r="9" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A9" s="10" t="s">
-        <v>136</v>
-      </c>
-      <c r="B9" s="10" t="str">
+        <v>160</v>
+      </c>
+      <c r="B9" s="15" t="str">
         <f>VLOOKUP(Πίνακας3[[#This Row],[Τύπος SQL]],types,2,FALSE)</f>
         <v>Δεκαδικός αριθμός</v>
       </c>
       <c r="C9" s="10" t="s">
         <v>135</v>
       </c>
-      <c r="D9" s="10" t="s">
-        <v>132</v>
-      </c>
+      <c r="D9" s="10"/>
       <c r="E9" s="10"/>
       <c r="F9" s="10"/>
       <c r="G9" s="10"/>
-      <c r="H9" s="10" t="str">
-        <f>"`cases`.`"&amp;Πίνακας3[[#This Row],[Πεδίο]]&amp;"` AS `"&amp;Πίνακας3[[#This Row],[Πεδίο]]&amp;"`,"</f>
-        <v>`cases`.`dbp` AS `dbp`,</v>
+      <c r="H9" s="15" t="str">
+        <f>"`cases`.`"&amp;Πίνακας3[[#This Row],[Πεδίο]]&amp;"` AS `"&amp;Πίνακας3[[#This Row],[Πεδίο]]&amp;"`,"</f>
+        <v>`cases`.`height` AS `height`,</v>
       </c>
       <c r="I9" s="10"/>
       <c r="K9" s="12" t="s">
@@ -2394,7 +2464,7 @@
     </row>
     <row r="10" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A10" s="10" t="s">
-        <v>56</v>
+        <v>62</v>
       </c>
       <c r="B10" s="10" t="str">
         <f>VLOOKUP(Πίνακας3[[#This Row],[Τύπος SQL]],types,2,FALSE)</f>
@@ -2411,7 +2481,7 @@
       <c r="G10" s="10"/>
       <c r="H10" s="10" t="str">
         <f>"`cases`.`"&amp;Πίνακας3[[#This Row],[Πεδίο]]&amp;"` AS `"&amp;Πίνακας3[[#This Row],[Πεδίο]]&amp;"`,"</f>
-        <v>`cases`.`glucose` AS `glucose`,</v>
+        <v>`cases`.`bmi` AS `bmi`,</v>
       </c>
       <c r="I10" s="10"/>
       <c r="O10" s="10"/>
@@ -2423,14 +2493,14 @@
     </row>
     <row r="11" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A11" s="10" t="s">
-        <v>68</v>
+        <v>133</v>
       </c>
       <c r="B11" s="10" t="str">
         <f>VLOOKUP(Πίνακας3[[#This Row],[Τύπος SQL]],types,2,FALSE)</f>
-        <v>Δεκαδικός αριθμός</v>
+        <v>Ναι/Όχι</v>
       </c>
       <c r="C11" s="10" t="s">
-        <v>135</v>
+        <v>127</v>
       </c>
       <c r="D11" s="10" t="s">
         <v>132</v>
@@ -2440,7 +2510,7 @@
       <c r="G11" s="10"/>
       <c r="H11" s="10" t="str">
         <f>"`cases`.`"&amp;Πίνακας3[[#This Row],[Πεδίο]]&amp;"` AS `"&amp;Πίνακας3[[#This Row],[Πεδίο]]&amp;"`,"</f>
-        <v>`cases`.`hba1c` AS `hba1c`,</v>
+        <v>`cases`.`drugbp` AS `drugbp`,</v>
       </c>
       <c r="I11" s="10"/>
       <c r="O11" s="10"/>
@@ -2452,14 +2522,14 @@
     </row>
     <row r="12" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A12" s="10" t="s">
-        <v>83</v>
+        <v>134</v>
       </c>
       <c r="B12" s="10" t="str">
         <f>VLOOKUP(Πίνακας3[[#This Row],[Τύπος SQL]],types,2,FALSE)</f>
-        <v>Ναι/Όχι</v>
+        <v>Δεκαδικός αριθμός</v>
       </c>
       <c r="C12" s="10" t="s">
-        <v>127</v>
+        <v>135</v>
       </c>
       <c r="D12" s="10" t="s">
         <v>132</v>
@@ -2469,7 +2539,7 @@
       <c r="G12" s="10"/>
       <c r="H12" s="10" t="str">
         <f>"`cases`.`"&amp;Πίνακας3[[#This Row],[Πεδίο]]&amp;"` AS `"&amp;Πίνακας3[[#This Row],[Πεδίο]]&amp;"`,"</f>
-        <v>`cases`.`diabetes` AS `diabetes`,</v>
+        <v>`cases`.`sbp` AS `sbp`,</v>
       </c>
       <c r="I12" s="10"/>
       <c r="O12" s="10"/>
@@ -2481,14 +2551,14 @@
     </row>
     <row r="13" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A13" s="10" t="s">
-        <v>58</v>
+        <v>136</v>
       </c>
       <c r="B13" s="10" t="str">
         <f>VLOOKUP(Πίνακας3[[#This Row],[Τύπος SQL]],types,2,FALSE)</f>
-        <v xml:space="preserve">Ακέραιος ή λίστα μέχρι 127 </v>
+        <v>Δεκαδικός αριθμός</v>
       </c>
       <c r="C13" s="10" t="s">
-        <v>131</v>
+        <v>135</v>
       </c>
       <c r="D13" s="10" t="s">
         <v>132</v>
@@ -2498,7 +2568,7 @@
       <c r="G13" s="10"/>
       <c r="H13" s="10" t="str">
         <f>"`cases`.`"&amp;Πίνακας3[[#This Row],[Πεδίο]]&amp;"` AS `"&amp;Πίνακας3[[#This Row],[Πεδίο]]&amp;"`,"</f>
-        <v>`cases`.`activity` AS `activity`,</v>
+        <v>`cases`.`dbp` AS `dbp`,</v>
       </c>
       <c r="I13" s="10"/>
       <c r="O13" s="10"/>
@@ -2510,14 +2580,14 @@
     </row>
     <row r="14" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A14" s="10" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="B14" s="10" t="str">
         <f>VLOOKUP(Πίνακας3[[#This Row],[Τύπος SQL]],types,2,FALSE)</f>
-        <v xml:space="preserve">Ακέραιος ή λίστα μέχρι 127 </v>
+        <v>Δεκαδικός αριθμός</v>
       </c>
       <c r="C14" s="10" t="s">
-        <v>131</v>
+        <v>135</v>
       </c>
       <c r="D14" s="10" t="s">
         <v>132</v>
@@ -2527,7 +2597,7 @@
       <c r="G14" s="10"/>
       <c r="H14" s="10" t="str">
         <f>"`cases`.`"&amp;Πίνακας3[[#This Row],[Πεδίο]]&amp;"` AS `"&amp;Πίνακας3[[#This Row],[Πεδίο]]&amp;"`,"</f>
-        <v>`cases`.`diet` AS `diet`,</v>
+        <v>`cases`.`glucose` AS `glucose`,</v>
       </c>
       <c r="I14" s="10"/>
       <c r="O14" s="10"/>
@@ -2539,14 +2609,14 @@
     </row>
     <row r="15" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A15" s="10" t="s">
-        <v>109</v>
+        <v>68</v>
       </c>
       <c r="B15" s="10" t="str">
         <f>VLOOKUP(Πίνακας3[[#This Row],[Τύπος SQL]],types,2,FALSE)</f>
-        <v xml:space="preserve">Ακέραιος ή λίστα μέχρι 127 </v>
+        <v>Δεκαδικός αριθμός</v>
       </c>
       <c r="C15" s="10" t="s">
-        <v>131</v>
+        <v>135</v>
       </c>
       <c r="D15" s="10" t="s">
         <v>132</v>
@@ -2556,7 +2626,7 @@
       <c r="G15" s="10"/>
       <c r="H15" s="10" t="str">
         <f>"`cases`.`"&amp;Πίνακας3[[#This Row],[Πεδίο]]&amp;"` AS `"&amp;Πίνακας3[[#This Row],[Πεδίο]]&amp;"`,"</f>
-        <v>`cases`.`alcohol` AS `alcohol`,</v>
+        <v>`cases`.`hba1c` AS `hba1c`,</v>
       </c>
       <c r="I15" s="10"/>
       <c r="O15" s="10"/>
@@ -2568,14 +2638,14 @@
     </row>
     <row r="16" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A16" s="10" t="s">
-        <v>60</v>
+        <v>83</v>
       </c>
       <c r="B16" s="10" t="str">
         <f>VLOOKUP(Πίνακας3[[#This Row],[Τύπος SQL]],types,2,FALSE)</f>
-        <v xml:space="preserve">Ακέραιος ή λίστα μέχρι 127 </v>
+        <v>Ναι/Όχι</v>
       </c>
       <c r="C16" s="10" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="D16" s="10" t="s">
         <v>132</v>
@@ -2585,7 +2655,7 @@
       <c r="G16" s="10"/>
       <c r="H16" s="10" t="str">
         <f>"`cases`.`"&amp;Πίνακας3[[#This Row],[Πεδίο]]&amp;"` AS `"&amp;Πίνακας3[[#This Row],[Πεδίο]]&amp;"`,"</f>
-        <v>`cases`.`smoking` AS `smoking`,</v>
+        <v>`cases`.`diabetes` AS `diabetes`,</v>
       </c>
       <c r="I16" s="10"/>
       <c r="O16" s="10"/>
@@ -2597,14 +2667,14 @@
     </row>
     <row r="17" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A17" s="10" t="s">
-        <v>137</v>
+        <v>58</v>
       </c>
       <c r="B17" s="10" t="str">
         <f>VLOOKUP(Πίνακας3[[#This Row],[Τύπος SQL]],types,2,FALSE)</f>
-        <v>Ναι/Όχι</v>
+        <v xml:space="preserve">Ακέραιος ή λίστα μέχρι 127 </v>
       </c>
       <c r="C17" s="10" t="s">
-        <v>127</v>
+        <v>131</v>
       </c>
       <c r="D17" s="10" t="s">
         <v>132</v>
@@ -2614,7 +2684,7 @@
       <c r="G17" s="10"/>
       <c r="H17" s="10" t="str">
         <f>"`cases`.`"&amp;Πίνακας3[[#This Row],[Πεδίο]]&amp;"` AS `"&amp;Πίνακας3[[#This Row],[Πεδίο]]&amp;"`,"</f>
-        <v>`cases`.`druglipids` AS `druglipids`,</v>
+        <v>`cases`.`activity` AS `activity`,</v>
       </c>
       <c r="I17" s="10"/>
       <c r="O17" s="10"/>
@@ -2626,14 +2696,14 @@
     </row>
     <row r="18" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A18" s="10" t="s">
-        <v>84</v>
+        <v>59</v>
       </c>
       <c r="B18" s="10" t="str">
         <f>VLOOKUP(Πίνακας3[[#This Row],[Τύπος SQL]],types,2,FALSE)</f>
-        <v>Δεκαδικός αριθμός</v>
+        <v xml:space="preserve">Ακέραιος ή λίστα μέχρι 127 </v>
       </c>
       <c r="C18" s="10" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="D18" s="10" t="s">
         <v>132</v>
@@ -2643,7 +2713,7 @@
       <c r="G18" s="10"/>
       <c r="H18" s="10" t="str">
         <f>"`cases`.`"&amp;Πίνακας3[[#This Row],[Πεδίο]]&amp;"` AS `"&amp;Πίνακας3[[#This Row],[Πεδίο]]&amp;"`,"</f>
-        <v>`cases`.`triglycerides` AS `triglycerides`,</v>
+        <v>`cases`.`diet` AS `diet`,</v>
       </c>
       <c r="I18" s="10"/>
       <c r="O18" s="10"/>
@@ -2655,14 +2725,14 @@
     </row>
     <row r="19" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A19" s="10" t="s">
-        <v>61</v>
+        <v>109</v>
       </c>
       <c r="B19" s="10" t="str">
         <f>VLOOKUP(Πίνακας3[[#This Row],[Τύπος SQL]],types,2,FALSE)</f>
-        <v>Δεκαδικός αριθμός</v>
+        <v xml:space="preserve">Ακέραιος ή λίστα μέχρι 127 </v>
       </c>
       <c r="C19" s="10" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="D19" s="10" t="s">
         <v>132</v>
@@ -2672,7 +2742,7 @@
       <c r="G19" s="10"/>
       <c r="H19" s="10" t="str">
         <f>"`cases`.`"&amp;Πίνακας3[[#This Row],[Πεδίο]]&amp;"` AS `"&amp;Πίνακας3[[#This Row],[Πεδίο]]&amp;"`,"</f>
-        <v>`cases`.`cholesterol` AS `cholesterol`,</v>
+        <v>`cases`.`alcohol` AS `alcohol`,</v>
       </c>
       <c r="I19" s="10"/>
       <c r="O19" s="10"/>
@@ -2684,14 +2754,14 @@
     </row>
     <row r="20" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A20" s="10" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="B20" s="10" t="str">
         <f>VLOOKUP(Πίνακας3[[#This Row],[Τύπος SQL]],types,2,FALSE)</f>
-        <v>Δεκαδικός αριθμός</v>
+        <v xml:space="preserve">Ακέραιος ή λίστα μέχρι 127 </v>
       </c>
       <c r="C20" s="10" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="D20" s="10" t="s">
         <v>132</v>
@@ -2701,7 +2771,7 @@
       <c r="G20" s="10"/>
       <c r="H20" s="10" t="str">
         <f>"`cases`.`"&amp;Πίνακας3[[#This Row],[Πεδίο]]&amp;"` AS `"&amp;Πίνακας3[[#This Row],[Πεδίο]]&amp;"`,"</f>
-        <v>`cases`.`ldl` AS `ldl`,</v>
+        <v>`cases`.`smoking` AS `smoking`,</v>
       </c>
       <c r="I20" s="10"/>
       <c r="O20" s="10"/>
@@ -2713,14 +2783,14 @@
     </row>
     <row r="21" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A21" s="10" t="s">
-        <v>67</v>
+        <v>137</v>
       </c>
       <c r="B21" s="10" t="str">
         <f>VLOOKUP(Πίνακας3[[#This Row],[Τύπος SQL]],types,2,FALSE)</f>
-        <v>Δεκαδικός αριθμός</v>
+        <v>Ναι/Όχι</v>
       </c>
       <c r="C21" s="10" t="s">
-        <v>135</v>
+        <v>127</v>
       </c>
       <c r="D21" s="10" t="s">
         <v>132</v>
@@ -2730,7 +2800,7 @@
       <c r="G21" s="10"/>
       <c r="H21" s="10" t="str">
         <f>"`cases`.`"&amp;Πίνακας3[[#This Row],[Πεδίο]]&amp;"` AS `"&amp;Πίνακας3[[#This Row],[Πεδίο]]&amp;"`,"</f>
-        <v>`cases`.`hdl` AS `hdl`,</v>
+        <v>`cases`.`druglipids` AS `druglipids`,</v>
       </c>
       <c r="I21" s="10"/>
       <c r="O21" s="10"/>
@@ -2742,7 +2812,7 @@
     </row>
     <row r="22" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A22" s="10" t="s">
-        <v>62</v>
+        <v>84</v>
       </c>
       <c r="B22" s="10" t="str">
         <f>VLOOKUP(Πίνακας3[[#This Row],[Τύπος SQL]],types,2,FALSE)</f>
@@ -2759,7 +2829,7 @@
       <c r="G22" s="10"/>
       <c r="H22" s="10" t="str">
         <f>"`cases`.`"&amp;Πίνακας3[[#This Row],[Πεδίο]]&amp;"` AS `"&amp;Πίνακας3[[#This Row],[Πεδίο]]&amp;"`,"</f>
-        <v>`cases`.`bmi` AS `bmi`,</v>
+        <v>`cases`.`triglycerides` AS `triglycerides`,</v>
       </c>
       <c r="I22" s="10"/>
       <c r="O22" s="10"/>
@@ -2771,7 +2841,7 @@
     </row>
     <row r="23" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A23" s="10" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B23" s="10" t="str">
         <f>VLOOKUP(Πίνακας3[[#This Row],[Τύπος SQL]],types,2,FALSE)</f>
@@ -2788,7 +2858,7 @@
       <c r="G23" s="10"/>
       <c r="H23" s="10" t="str">
         <f>"`cases`.`"&amp;Πίνακας3[[#This Row],[Πεδίο]]&amp;"` AS `"&amp;Πίνακας3[[#This Row],[Πεδίο]]&amp;"`,"</f>
-        <v>`cases`.`crp` AS `crp`,</v>
+        <v>`cases`.`cholesterol` AS `cholesterol`,</v>
       </c>
       <c r="I23" s="10"/>
       <c r="O23" s="10"/>
@@ -2800,7 +2870,7 @@
     </row>
     <row r="24" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A24" s="10" t="s">
-        <v>77</v>
+        <v>66</v>
       </c>
       <c r="B24" s="10" t="str">
         <f>VLOOKUP(Πίνακας3[[#This Row],[Τύπος SQL]],types,2,FALSE)</f>
@@ -2817,7 +2887,7 @@
       <c r="G24" s="10"/>
       <c r="H24" s="10" t="str">
         <f>"`cases`.`"&amp;Πίνακας3[[#This Row],[Πεδίο]]&amp;"` AS `"&amp;Πίνακας3[[#This Row],[Πεδίο]]&amp;"`,"</f>
-        <v>`cases`.`wbc` AS `wbc`,</v>
+        <v>`cases`.`ldl` AS `ldl`,</v>
       </c>
       <c r="I24" s="10"/>
       <c r="O24" s="10"/>
@@ -2829,7 +2899,7 @@
     </row>
     <row r="25" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A25" s="10" t="s">
-        <v>94</v>
+        <v>67</v>
       </c>
       <c r="B25" s="10" t="str">
         <f>VLOOKUP(Πίνακας3[[#This Row],[Τύπος SQL]],types,2,FALSE)</f>
@@ -2846,7 +2916,7 @@
       <c r="G25" s="10"/>
       <c r="H25" s="10" t="str">
         <f>"`cases`.`"&amp;Πίνακας3[[#This Row],[Πεδίο]]&amp;"` AS `"&amp;Πίνακας3[[#This Row],[Πεδίο]]&amp;"`,"</f>
-        <v>`cases`.`imt` AS `imt`,</v>
+        <v>`cases`.`hdl` AS `hdl`,</v>
       </c>
       <c r="I25" s="10"/>
       <c r="O25" s="10"/>
@@ -2858,7 +2928,7 @@
     </row>
     <row r="26" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A26" s="10" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B26" s="10" t="str">
         <f>VLOOKUP(Πίνακας3[[#This Row],[Τύπος SQL]],types,2,FALSE)</f>
@@ -2875,7 +2945,7 @@
       <c r="G26" s="10"/>
       <c r="H26" s="10" t="str">
         <f>"`cases`.`"&amp;Πίνακας3[[#This Row],[Πεδίο]]&amp;"` AS `"&amp;Πίνακας3[[#This Row],[Πεδίο]]&amp;"`,"</f>
-        <v>`cases`.`ef` AS `ef`,</v>
+        <v>`cases`.`crp` AS `crp`,</v>
       </c>
       <c r="I26" s="10"/>
       <c r="O26" s="10"/>
@@ -2887,7 +2957,7 @@
     </row>
     <row r="27" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A27" s="10" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="B27" s="10" t="str">
         <f>VLOOKUP(Πίνακας3[[#This Row],[Τύπος SQL]],types,2,FALSE)</f>
@@ -2904,7 +2974,7 @@
       <c r="G27" s="10"/>
       <c r="H27" s="10" t="str">
         <f>"`cases`.`"&amp;Πίνακας3[[#This Row],[Πεδίο]]&amp;"` AS `"&amp;Πίνακας3[[#This Row],[Πεδίο]]&amp;"`,"</f>
-        <v>`cases`.`calciumscore` AS `calciumscore`,</v>
+        <v>`cases`.`wbc` AS `wbc`,</v>
       </c>
       <c r="I27" s="10"/>
       <c r="O27" s="10"/>
@@ -2916,7 +2986,7 @@
     </row>
     <row r="28" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A28" s="10" t="s">
-        <v>65</v>
+        <v>94</v>
       </c>
       <c r="B28" s="10" t="str">
         <f>VLOOKUP(Πίνακας3[[#This Row],[Τύπος SQL]],types,2,FALSE)</f>
@@ -2933,7 +3003,7 @@
       <c r="G28" s="10"/>
       <c r="H28" s="10" t="str">
         <f>"`cases`.`"&amp;Πίνακας3[[#This Row],[Πεδίο]]&amp;"` AS `"&amp;Πίνακας3[[#This Row],[Πεδίο]]&amp;"`,"</f>
-        <v>`cases`.`lpa` AS `lpa`,</v>
+        <v>`cases`.`imt` AS `imt`,</v>
       </c>
       <c r="I28" s="10"/>
       <c r="O28" s="10"/>
@@ -2945,7 +3015,7 @@
     </row>
     <row r="29" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A29" s="10" t="s">
-        <v>71</v>
+        <v>64</v>
       </c>
       <c r="B29" s="10" t="str">
         <f>VLOOKUP(Πίνακας3[[#This Row],[Τύπος SQL]],types,2,FALSE)</f>
@@ -2962,7 +3032,7 @@
       <c r="G29" s="10"/>
       <c r="H29" s="10" t="str">
         <f>"`cases`.`"&amp;Πίνακας3[[#This Row],[Πεδίο]]&amp;"` AS `"&amp;Πίνακας3[[#This Row],[Πεδίο]]&amp;"`,"</f>
-        <v>`cases`.`creatinine` AS `creatinine`,</v>
+        <v>`cases`.`ef` AS `ef`,</v>
       </c>
       <c r="I29" s="10"/>
       <c r="O29" s="10"/>
@@ -2974,14 +3044,14 @@
     </row>
     <row r="30" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A30" s="10" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="B30" s="10" t="str">
         <f>VLOOKUP(Πίνακας3[[#This Row],[Τύπος SQL]],types,2,FALSE)</f>
-        <v>Ναι/Όχι</v>
+        <v>Δεκαδικός αριθμός</v>
       </c>
       <c r="C30" s="10" t="s">
-        <v>127</v>
+        <v>135</v>
       </c>
       <c r="D30" s="10" t="s">
         <v>132</v>
@@ -2991,7 +3061,7 @@
       <c r="G30" s="10"/>
       <c r="H30" s="10" t="str">
         <f>"`cases`.`"&amp;Πίνακας3[[#This Row],[Πεδίο]]&amp;"` AS `"&amp;Πίνακας3[[#This Row],[Πεδίο]]&amp;"`,"</f>
-        <v>`cases`.`atrialfibrillation` AS `atrialfibrillation`,</v>
+        <v>`cases`.`calciumscore` AS `calciumscore`,</v>
       </c>
       <c r="I30" s="10"/>
       <c r="O30" s="10"/>
@@ -3003,14 +3073,14 @@
     </row>
     <row r="31" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A31" s="10" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="B31" s="10" t="str">
         <f>VLOOKUP(Πίνακας3[[#This Row],[Τύπος SQL]],types,2,FALSE)</f>
-        <v>Ναι/Όχι</v>
+        <v>Δεκαδικός αριθμός</v>
       </c>
       <c r="C31" s="10" t="s">
-        <v>127</v>
+        <v>135</v>
       </c>
       <c r="D31" s="10" t="s">
         <v>132</v>
@@ -3020,7 +3090,7 @@
       <c r="G31" s="10"/>
       <c r="H31" s="10" t="str">
         <f>"`cases`.`"&amp;Πίνακας3[[#This Row],[Πεδίο]]&amp;"` AS `"&amp;Πίνακας3[[#This Row],[Πεδίο]]&amp;"`,"</f>
-        <v>`cases`.`heartfailure` AS `heartfailure`,</v>
+        <v>`cases`.`lpa` AS `lpa`,</v>
       </c>
       <c r="I31" s="10"/>
       <c r="O31" s="10"/>
@@ -3032,14 +3102,14 @@
     </row>
     <row r="32" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A32" s="10" t="s">
-        <v>138</v>
+        <v>71</v>
       </c>
       <c r="B32" s="10" t="str">
         <f>VLOOKUP(Πίνακας3[[#This Row],[Τύπος SQL]],types,2,FALSE)</f>
-        <v>Ναι/Όχι</v>
+        <v>Δεκαδικός αριθμός</v>
       </c>
       <c r="C32" s="10" t="s">
-        <v>127</v>
+        <v>135</v>
       </c>
       <c r="D32" s="10" t="s">
         <v>132</v>
@@ -3049,7 +3119,7 @@
       <c r="G32" s="10"/>
       <c r="H32" s="10" t="str">
         <f>"`cases`.`"&amp;Πίνακας3[[#This Row],[Πεδίο]]&amp;"` AS `"&amp;Πίνακας3[[#This Row],[Πεδίο]]&amp;"`,"</f>
-        <v>`cases`.`cvd` AS `cvd`,</v>
+        <v>`cases`.`creatinine` AS `creatinine`,</v>
       </c>
       <c r="I32" s="10"/>
       <c r="O32" s="10"/>
@@ -3061,14 +3131,14 @@
     </row>
     <row r="33" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A33" s="10" t="s">
-        <v>139</v>
+        <v>70</v>
       </c>
       <c r="B33" s="10" t="str">
         <f>VLOOKUP(Πίνακας3[[#This Row],[Τύπος SQL]],types,2,FALSE)</f>
-        <v>Ακέραιος μέχρι 65535</v>
+        <v>Ναι/Όχι</v>
       </c>
       <c r="C33" s="10" t="s">
-        <v>140</v>
+        <v>127</v>
       </c>
       <c r="D33" s="10" t="s">
         <v>132</v>
@@ -3078,7 +3148,7 @@
       <c r="G33" s="10"/>
       <c r="H33" s="10" t="str">
         <f>"`cases`.`"&amp;Πίνακας3[[#This Row],[Πεδίο]]&amp;"` AS `"&amp;Πίνακας3[[#This Row],[Πεδίο]]&amp;"`,"</f>
-        <v>`cases`.`yrcvd` AS `yrcvd`,</v>
+        <v>`cases`.`cancer` AS `cancer`,</v>
       </c>
       <c r="I33" s="10"/>
       <c r="O33" s="10"/>
@@ -3090,14 +3160,14 @@
     </row>
     <row r="34" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A34" s="10" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B34" s="10" t="str">
         <f>VLOOKUP(Πίνακας3[[#This Row],[Τύπος SQL]],types,2,FALSE)</f>
-        <v>Ναι/Όχι</v>
+        <v>Ακέραιος μέχρι 65535</v>
       </c>
       <c r="C34" s="10" t="s">
-        <v>127</v>
+        <v>140</v>
       </c>
       <c r="D34" s="10" t="s">
         <v>132</v>
@@ -3107,7 +3177,7 @@
       <c r="G34" s="10"/>
       <c r="H34" s="10" t="str">
         <f>"`cases`.`"&amp;Πίνακας3[[#This Row],[Πεδίο]]&amp;"` AS `"&amp;Πίνακας3[[#This Row],[Πεδίο]]&amp;"`,"</f>
-        <v>`cases`.`deathcvd` AS `deathcvd`,</v>
+        <v>`cases`.`yrcancer` AS `yrcancer`,</v>
       </c>
       <c r="I34" s="10"/>
       <c r="O34" s="10"/>
@@ -3119,14 +3189,14 @@
     </row>
     <row r="35" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A35" s="10" t="s">
-        <v>122</v>
+        <v>85</v>
       </c>
       <c r="B35" s="10" t="str">
         <f>VLOOKUP(Πίνακας3[[#This Row],[Τύπος SQL]],types,2,FALSE)</f>
-        <v>Ακέραιος μέχρι 65535</v>
+        <v>Ναι/Όχι</v>
       </c>
       <c r="C35" s="10" t="s">
-        <v>140</v>
+        <v>127</v>
       </c>
       <c r="D35" s="10" t="s">
         <v>132</v>
@@ -3136,7 +3206,7 @@
       <c r="G35" s="10"/>
       <c r="H35" s="10" t="str">
         <f>"`cases`.`"&amp;Πίνακας3[[#This Row],[Πεδίο]]&amp;"` AS `"&amp;Πίνακας3[[#This Row],[Πεδίο]]&amp;"`,"</f>
-        <v>`cases`.`yrcvddeath` AS `yrcvddeath`,</v>
+        <v>`cases`.`atrialfibrillation` AS `atrialfibrillation`,</v>
       </c>
       <c r="I35" s="10"/>
       <c r="O35" s="10"/>
@@ -3148,7 +3218,7 @@
     </row>
     <row r="36" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A36" s="10" t="s">
-        <v>57</v>
+        <v>69</v>
       </c>
       <c r="B36" s="10" t="str">
         <f>VLOOKUP(Πίνακας3[[#This Row],[Τύπος SQL]],types,2,FALSE)</f>
@@ -3165,7 +3235,7 @@
       <c r="G36" s="10"/>
       <c r="H36" s="10" t="str">
         <f>"`cases`.`"&amp;Πίνακας3[[#This Row],[Πεδίο]]&amp;"` AS `"&amp;Πίνακας3[[#This Row],[Πεδίο]]&amp;"`,"</f>
-        <v>`cases`.`familyhistory` AS `familyhistory`,</v>
+        <v>`cases`.`heartfailure` AS `heartfailure`,</v>
       </c>
       <c r="I36" s="10"/>
       <c r="O36" s="10"/>
@@ -3177,7 +3247,7 @@
     </row>
     <row r="37" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A37" s="10" t="s">
-        <v>70</v>
+        <v>138</v>
       </c>
       <c r="B37" s="10" t="str">
         <f>VLOOKUP(Πίνακας3[[#This Row],[Τύπος SQL]],types,2,FALSE)</f>
@@ -3194,7 +3264,7 @@
       <c r="G37" s="10"/>
       <c r="H37" s="10" t="str">
         <f>"`cases`.`"&amp;Πίνακας3[[#This Row],[Πεδίο]]&amp;"` AS `"&amp;Πίνακας3[[#This Row],[Πεδίο]]&amp;"`,"</f>
-        <v>`cases`.`cancer` AS `cancer`,</v>
+        <v>`cases`.`cvd` AS `cvd`,</v>
       </c>
       <c r="I37" s="10"/>
       <c r="O37" s="10"/>
@@ -3206,7 +3276,7 @@
     </row>
     <row r="38" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A38" s="10" t="s">
-        <v>120</v>
+        <v>139</v>
       </c>
       <c r="B38" s="10" t="str">
         <f>VLOOKUP(Πίνακας3[[#This Row],[Τύπος SQL]],types,2,FALSE)</f>
@@ -3223,7 +3293,7 @@
       <c r="G38" s="10"/>
       <c r="H38" s="10" t="str">
         <f>"`cases`.`"&amp;Πίνακας3[[#This Row],[Πεδίο]]&amp;"` AS `"&amp;Πίνακας3[[#This Row],[Πεδίο]]&amp;"`,"</f>
-        <v>`cases`.`yrcancer` AS `yrcancer`,</v>
+        <v>`cases`.`yrcvd` AS `yrcvd`,</v>
       </c>
       <c r="I38" s="10"/>
       <c r="O38" s="10"/>
@@ -3235,14 +3305,14 @@
     </row>
     <row r="39" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A39" s="10" t="s">
-        <v>141</v>
+        <v>121</v>
       </c>
       <c r="B39" s="10" t="str">
         <f>VLOOKUP(Πίνακας3[[#This Row],[Τύπος SQL]],types,2,FALSE)</f>
-        <v>Μεγάλο κείμενο</v>
+        <v>Ναι/Όχι</v>
       </c>
       <c r="C39" s="10" t="s">
-        <v>142</v>
+        <v>127</v>
       </c>
       <c r="D39" s="10" t="s">
         <v>132</v>
@@ -3252,7 +3322,7 @@
       <c r="G39" s="10"/>
       <c r="H39" s="10" t="str">
         <f>"`cases`.`"&amp;Πίνακας3[[#This Row],[Πεδίο]]&amp;"` AS `"&amp;Πίνακας3[[#This Row],[Πεδίο]]&amp;"`,"</f>
-        <v>`cases`.`comments` AS `comments`,</v>
+        <v>`cases`.`deathcvd` AS `deathcvd`,</v>
       </c>
       <c r="I39" s="10"/>
       <c r="O39" s="10"/>
@@ -3264,24 +3334,24 @@
     </row>
     <row r="40" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A40" s="10" t="s">
-        <v>74</v>
+        <v>122</v>
       </c>
       <c r="B40" s="10" t="str">
         <f>VLOOKUP(Πίνακας3[[#This Row],[Τύπος SQL]],types,2,FALSE)</f>
-        <v>Ημερομηνία και Ώρα</v>
+        <v>Ακέραιος μέχρι 65535</v>
       </c>
       <c r="C40" s="10" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="D40" s="10" t="s">
-        <v>124</v>
+        <v>132</v>
       </c>
       <c r="E40" s="10"/>
       <c r="F40" s="10"/>
       <c r="G40" s="10"/>
       <c r="H40" s="10" t="str">
         <f>"`cases`.`"&amp;Πίνακας3[[#This Row],[Πεδίο]]&amp;"` AS `"&amp;Πίνακας3[[#This Row],[Πεδίο]]&amp;"`,"</f>
-        <v>`cases`.`createdAt` AS `createdAt`,</v>
+        <v>`cases`.`yrcvddeath` AS `yrcvddeath`,</v>
       </c>
       <c r="I40" s="10"/>
       <c r="O40" s="10"/>
@@ -3293,24 +3363,24 @@
     </row>
     <row r="41" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A41" s="10" t="s">
-        <v>75</v>
+        <v>57</v>
       </c>
       <c r="B41" s="10" t="str">
         <f>VLOOKUP(Πίνακας3[[#This Row],[Τύπος SQL]],types,2,FALSE)</f>
-        <v>Ημερομηνία και Ώρα</v>
+        <v>Ναι/Όχι</v>
       </c>
       <c r="C41" s="10" t="s">
-        <v>143</v>
+        <v>127</v>
       </c>
       <c r="D41" s="10" t="s">
-        <v>124</v>
+        <v>132</v>
       </c>
       <c r="E41" s="10"/>
       <c r="F41" s="10"/>
       <c r="G41" s="10"/>
       <c r="H41" s="10" t="str">
         <f>"`cases`.`"&amp;Πίνακας3[[#This Row],[Πεδίο]]&amp;"` AS `"&amp;Πίνακας3[[#This Row],[Πεδίο]]&amp;"`,"</f>
-        <v>`cases`.`updatedAt` AS `updatedAt`,</v>
+        <v>`cases`.`familyhistory` AS `familyhistory`,</v>
       </c>
       <c r="I41" s="10"/>
       <c r="O41" s="10"/>
@@ -3322,26 +3392,24 @@
     </row>
     <row r="42" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A42" s="10" t="s">
-        <v>73</v>
+        <v>141</v>
       </c>
       <c r="B42" s="10" t="str">
         <f>VLOOKUP(Πίνακας3[[#This Row],[Τύπος SQL]],types,2,FALSE)</f>
-        <v>Σύντομο κείμενο</v>
+        <v>Μεγάλο κείμενο</v>
       </c>
       <c r="C42" s="10" t="s">
-        <v>129</v>
+        <v>142</v>
       </c>
       <c r="D42" s="10" t="s">
         <v>132</v>
       </c>
-      <c r="E42" s="10" t="s">
-        <v>130</v>
-      </c>
+      <c r="E42" s="10"/>
       <c r="F42" s="10"/>
       <c r="G42" s="10"/>
       <c r="H42" s="10" t="str">
         <f>"`cases`.`"&amp;Πίνακας3[[#This Row],[Πεδίο]]&amp;"` AS `"&amp;Πίνακας3[[#This Row],[Πεδίο]]&amp;"`,"</f>
-        <v>`cases`.`author` AS `author`,</v>
+        <v>`cases`.`comments` AS `comments`,</v>
       </c>
       <c r="I42" s="10"/>
       <c r="O42" s="10"/>
@@ -3351,14 +3419,103 @@
       <c r="S42" s="10"/>
       <c r="T42" s="10"/>
     </row>
-    <row r="50" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B50" s="13"/>
-    </row>
-    <row r="51" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B51" s="14"/>
-    </row>
-    <row r="52" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B52" s="13"/>
+    <row r="43" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A43" s="10" t="s">
+        <v>74</v>
+      </c>
+      <c r="B43" s="10" t="str">
+        <f>VLOOKUP(Πίνακας3[[#This Row],[Τύπος SQL]],types,2,FALSE)</f>
+        <v>Ημερομηνία και Ώρα</v>
+      </c>
+      <c r="C43" s="10" t="s">
+        <v>143</v>
+      </c>
+      <c r="D43" s="10" t="s">
+        <v>124</v>
+      </c>
+      <c r="E43" s="10"/>
+      <c r="F43" s="10"/>
+      <c r="G43" s="10"/>
+      <c r="H43" s="10" t="str">
+        <f>"`cases`.`"&amp;Πίνακας3[[#This Row],[Πεδίο]]&amp;"` AS `"&amp;Πίνακας3[[#This Row],[Πεδίο]]&amp;"`,"</f>
+        <v>`cases`.`createdAt` AS `createdAt`,</v>
+      </c>
+      <c r="I43" s="10"/>
+      <c r="O43" s="10"/>
+      <c r="P43" s="10"/>
+      <c r="Q43" s="10"/>
+      <c r="R43" s="10"/>
+      <c r="S43" s="10"/>
+      <c r="T43" s="10"/>
+    </row>
+    <row r="44" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A44" s="10" t="s">
+        <v>75</v>
+      </c>
+      <c r="B44" s="10" t="str">
+        <f>VLOOKUP(Πίνακας3[[#This Row],[Τύπος SQL]],types,2,FALSE)</f>
+        <v>Ημερομηνία και Ώρα</v>
+      </c>
+      <c r="C44" s="10" t="s">
+        <v>143</v>
+      </c>
+      <c r="D44" s="10" t="s">
+        <v>124</v>
+      </c>
+      <c r="E44" s="10"/>
+      <c r="F44" s="10"/>
+      <c r="G44" s="10"/>
+      <c r="H44" s="10" t="str">
+        <f>"`cases`.`"&amp;Πίνακας3[[#This Row],[Πεδίο]]&amp;"` AS `"&amp;Πίνακας3[[#This Row],[Πεδίο]]&amp;"`,"</f>
+        <v>`cases`.`updatedAt` AS `updatedAt`,</v>
+      </c>
+      <c r="I44" s="10"/>
+      <c r="O44" s="10"/>
+      <c r="P44" s="10"/>
+      <c r="Q44" s="10"/>
+      <c r="R44" s="10"/>
+      <c r="S44" s="10"/>
+      <c r="T44" s="10"/>
+    </row>
+    <row r="45" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A45" s="10" t="s">
+        <v>73</v>
+      </c>
+      <c r="B45" s="10" t="str">
+        <f>VLOOKUP(Πίνακας3[[#This Row],[Τύπος SQL]],types,2,FALSE)</f>
+        <v>Σύντομο κείμενο</v>
+      </c>
+      <c r="C45" s="10" t="s">
+        <v>129</v>
+      </c>
+      <c r="D45" s="10" t="s">
+        <v>132</v>
+      </c>
+      <c r="E45" s="10" t="s">
+        <v>130</v>
+      </c>
+      <c r="F45" s="10"/>
+      <c r="G45" s="10"/>
+      <c r="H45" s="10" t="str">
+        <f>"`cases`.`"&amp;Πίνακας3[[#This Row],[Πεδίο]]&amp;"` AS `"&amp;Πίνακας3[[#This Row],[Πεδίο]]&amp;"`,"</f>
+        <v>`cases`.`author` AS `author`,</v>
+      </c>
+      <c r="I45" s="10"/>
+      <c r="O45" s="10"/>
+      <c r="P45" s="10"/>
+      <c r="Q45" s="10"/>
+      <c r="R45" s="10"/>
+      <c r="S45" s="10"/>
+      <c r="T45" s="10"/>
+    </row>
+    <row r="53" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B53" s="13"/>
+    </row>
+    <row r="54" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B54" s="14"/>
+    </row>
+    <row r="55" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B55" s="13"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>